<commit_message>
Big balance pass, added notes
  * Barters, in general, have some higher minimum standards and don't pay out quite as well. That way you're not just waiting for the right trade and sometimes you'll just need to fight.
  * Added notes to each card to record my motivations for why the card needs to exist
  * Added lookup to show the card back easily
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -76,12 +76,6 @@
     <t>Minor Ductwork</t>
   </si>
   <si>
-    <t>2:1 Fabric:Duct Tape</t>
-  </si>
-  <si>
-    <t>Rusty Toolbox</t>
-  </si>
-  <si>
     <t>Tetanus Worms</t>
   </si>
   <si>
@@ -97,12 +91,6 @@
     <t>Sprocket Bats</t>
   </si>
   <si>
-    <t>Can of Lube</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
     <t>Recipe</t>
   </si>
   <si>
@@ -142,9 +130,6 @@
     <t>4:3:2:1 for Metal:Fabric:Oil:Duct Tape</t>
   </si>
   <si>
-    <t>3:1 Metal:Duct Tape</t>
-  </si>
-  <si>
     <t>Tape Dispensor</t>
   </si>
   <si>
@@ -164,12 +149,6 @@
   </si>
   <si>
     <t>Sewing Machine</t>
-  </si>
-  <si>
-    <t>4:1:1:1 Metal:Fabric:Oil:Duct Tape</t>
-  </si>
-  <si>
-    <t>Max</t>
   </si>
   <si>
     <t>Tote Bag
@@ -223,14 +202,6 @@
     <t>+1 ATK for 4 Metal</t>
   </si>
   <si>
-    <t>3 HP. 3 ATK.
- ⃠ Use Tote Bag</t>
-  </si>
-  <si>
-    <t>12 HP. 4 ATK
-⃠ Have Whacking Plank</t>
-  </si>
-  <si>
     <t xml:space="preserve">+2 Duct Tape for Disassembling 1 Tool </t>
   </si>
   <si>
@@ -257,11 +228,6 @@
 for 3 Metal, 1 Oil</t>
   </si>
   <si>
-    <t>1:1 Metal:Oil
-or
-1:1 Fabric:Oil</t>
-  </si>
-  <si>
     <t>8 HP. 2 ATK.</t>
   </si>
   <si>
@@ -269,9 +235,6 @@
  ⃠ Have Tote Bag</t>
   </si>
   <si>
-    <t>Recover 3/6/9 HP for 1/2/3 Oil</t>
-  </si>
-  <si>
     <t>Strong Magnet
 for 2 Metal</t>
   </si>
@@ -303,13 +266,100 @@
   </si>
   <si>
     <t xml:space="preserve">17 HP. 4 ATK. </t>
+  </si>
+  <si>
+    <t>5:3 Metal:Fabric</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>3:2 Metal:Oil
+or
+2:1 Fabric:Oil</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Attack creature, but now with metal.</t>
+  </si>
+  <si>
+    <t>General store. Everything is balanced against him.</t>
+  </si>
+  <si>
+    <t>Fabric dealer. Tote bags.</t>
+  </si>
+  <si>
+    <t>Metal dealer. Good to beat if you have a tote bag</t>
+  </si>
+  <si>
+    <t>Oil dealer, but you need a good volume of Metal.</t>
+  </si>
+  <si>
+    <t>Healer. Doesn't give much but healing is awesome</t>
+  </si>
+  <si>
+    <t>Tool check, instead of general store. Requires duct tape or tool to pass!!</t>
+  </si>
+  <si>
+    <t>Fabric dealer. Tote bags. (Better version of Curtain Ghost)</t>
+  </si>
+  <si>
+    <t>Duct tape dealer.</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Duct tape dealer, but with oil.</t>
+  </si>
+  <si>
+    <t>2:3 Metal:Fabric</t>
+  </si>
+  <si>
+    <t>Oil to both Metal and Fabric</t>
+  </si>
+  <si>
+    <t>Metal dealer, but you need lots of fabric. Or lots of Metal.</t>
+  </si>
+  <si>
+    <t>15 HP. 3 ATK.
+ ⃠ Use Tote Bag</t>
+  </si>
+  <si>
+    <t>11 HP. 4 ATK
+⃠ Have Whacking Plank</t>
+  </si>
+  <si>
+    <t>Friendly Can of Lube</t>
+  </si>
+  <si>
+    <t>Rusty the Toolbox</t>
+  </si>
+  <si>
+    <t>3:2 Fabric:Duct Tape</t>
+  </si>
+  <si>
+    <t>+1 Duct Tape for 3 Fabric
+or
++2 Duct Tape for 4 Fabric</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Recover 3/6/10 HP for 1/2/3 Oil</t>
+  </si>
+  <si>
+    <t>Duct tape dealer, repeatable but not quite as good. Tons of goods.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,16 +375,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -342,50 +411,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -692,32 +816,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="11"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="11" width="66" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -729,482 +855,586 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="9">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="9">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="F2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="9">
         <v>1</v>
       </c>
       <c r="J2" s="11">
         <f>C2/4 + D2/3+E2/2</f>
         <v>1.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="K2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="8" t="str">
+        <f>INDEX(A$9:A$15,MATCH(I2,I$9:I$15,0))</f>
+        <v>Oil Nymph</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="9">
         <v>0</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="9">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="F3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="9">
         <v>2</v>
       </c>
       <c r="J3" s="11">
         <f t="shared" ref="J3:J15" si="0">C3/4 + D3/3+E3/2</f>
         <v>1.8333333333333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="K3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f>INDEX(A$9:A$15,MATCH(I3,I$9:I$15,0))</f>
+        <v>Petulant Tig Welder</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="9">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="9">
         <v>3</v>
       </c>
       <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="K4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f t="shared" ref="L4:L7" si="1">INDEX(A$9:A$15,MATCH(I4,I$9:I$15,0))</f>
+        <v>Sewing Machine</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="9">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="9">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="9">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="F5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="9">
         <v>4</v>
       </c>
       <c r="J5" s="11">
         <f t="shared" si="0"/>
         <v>1.5833333333333333</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="K5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Major Ductwork</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="9">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="9">
         <v>4</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="F6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="9">
         <v>5</v>
       </c>
       <c r="J6" s="11">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="K6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>The Crusher</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="9">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="9">
         <v>0</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="F7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="9">
         <v>6</v>
       </c>
       <c r="J7" s="11">
         <f t="shared" si="0"/>
         <v>1.9166666666666665</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="K7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Tap Spider</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="9">
         <v>7</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="9">
         <v>0</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="F8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="9">
         <v>7</v>
       </c>
       <c r="J8" s="11">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="K8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f>INDEX(A$9:A$15,MATCH(I8,I$9:I$15,0))</f>
+        <v>Sprocket Bats</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3">
+      <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="15">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="15">
         <v>5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="15">
         <v>5</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="F9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="15">
+        <v>7</v>
+      </c>
+      <c r="J9" s="18">
         <f t="shared" si="0"/>
         <v>5.416666666666667</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="K9" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="14" t="str">
+        <f>INDEX(A$2:A$8,MATCH(I9,I$2:I$8,0))</f>
+        <v>Curtain Ghost</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="15">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="15">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="15">
         <v>5</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="3">
-        <v>2</v>
-      </c>
-      <c r="J10" s="11">
+      <c r="F10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="15">
+        <v>1</v>
+      </c>
+      <c r="J10" s="18">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="K10" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="14" t="str">
+        <f t="shared" ref="L10:L15" si="2">INDEX(A$2:A$8,MATCH(I10,I$2:I$8,0))</f>
+        <v>Bolt Rats</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="15">
         <v>7</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="15">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="15">
         <v>1</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="3">
-        <v>3</v>
-      </c>
-      <c r="J11" s="11">
+      <c r="F11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="15">
+        <v>2</v>
+      </c>
+      <c r="J11" s="18">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="K11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Friendly Can of Lube</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="15">
         <v>8</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="15">
         <v>5</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="15">
         <v>3</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="F12" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="15">
         <v>4</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="18">
         <f t="shared" si="0"/>
         <v>5.166666666666667</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="K12" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Minor Ductwork</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15">
         <v>6</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="15">
         <v>6</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="15">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="3">
-        <v>5</v>
-      </c>
-      <c r="J13" s="11">
+      <c r="F13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="15">
+        <v>3</v>
+      </c>
+      <c r="J13" s="18">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="K13" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Socket Wrench Puppy</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="15">
         <v>8</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="15">
         <v>4</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="15">
         <v>4</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="F14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="3">
-        <v>6</v>
-      </c>
-      <c r="J14" s="11">
+      <c r="H14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="15">
+        <v>5</v>
+      </c>
+      <c r="J14" s="18">
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="K14" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Rusty the Toolbox</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="15">
         <v>5</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="15">
         <v>1</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="15">
         <v>1</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="3">
-        <v>7</v>
-      </c>
-      <c r="J15" s="11">
+      <c r="F15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="15">
+        <v>6</v>
+      </c>
+      <c r="J15" s="18">
         <f t="shared" si="0"/>
         <v>2.083333333333333</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="L15" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>Tetanus Worms</v>
       </c>
     </row>
   </sheetData>
@@ -1215,106 +1445,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1330,7 +1535,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,26 +1543,26 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1383,7 +1588,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <f>SUM(Cards!C9:C15)</f>
@@ -1404,7 +1609,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>

</xml_diff>

<commit_message>
layout: rearrange a bit, add version
Make it more horizontal and readable.

Use text's align to differentiate for now.
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -274,11 +274,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>3:2 Metal:Oil
-or
-2:1 Fabric:Oil</t>
-  </si>
-  <si>
     <t>Back</t>
   </si>
   <si>
@@ -341,18 +336,21 @@
     <t>3:2 Fabric:Duct Tape</t>
   </si>
   <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Recover 3/6/10 HP for 1/2/3 Oil</t>
+  </si>
+  <si>
+    <t>Duct tape dealer, repeatable but not quite as good. Tons of goods.</t>
+  </si>
+  <si>
+    <t>3:2 Metal:Oil
+or 2:1 Fabric:Oil</t>
+  </si>
+  <si>
     <t>+1 Duct Tape for 3 Fabric
-or
-+2 Duct Tape for 4 Fabric</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Recover 3/6/10 HP for 1/2/3 Oil</t>
-  </si>
-  <si>
-    <t>Duct tape dealer, repeatable but not quite as good. Tons of goods.</t>
+or +2 Duct Tape for 4 Fabric</t>
   </si>
 </sst>
 </file>
@@ -440,71 +438,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -819,620 +817,620 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="23"/>
-    <col min="11" max="11" width="66" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="22"/>
+    <col min="11" max="11" width="66" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="L1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>3</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>1</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="10">
         <f>C2/4 + D2/3+E2/2</f>
         <v>1.25</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="8" t="str">
+      <c r="K2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I2,I$9:I$15,0))</f>
         <v>Oil Nymph</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>1</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>2</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <f t="shared" ref="J3:J15" si="0">C3/4 + D3/3+E3/2</f>
         <v>1.8333333333333333</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="8" t="str">
+      <c r="K3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I3,I$9:I$15,0))</f>
         <v>Petulant Tig Welder</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>3</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" s="8" t="str">
+      <c r="K4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="7" t="str">
         <f t="shared" ref="L4:L7" si="1">INDEX(A$9:A$15,MATCH(I4,I$9:I$15,0))</f>
         <v>Sewing Machine</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>4</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <f t="shared" si="0"/>
         <v>1.5833333333333333</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" s="8" t="str">
+      <c r="K5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Major Ductwork</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>4</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>5</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6" s="8" t="str">
+      <c r="K6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>The Crusher</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>5</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>6</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <f t="shared" si="0"/>
         <v>1.9166666666666665</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="L7" s="8" t="str">
+      <c r="K7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Tap Spider</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>7</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>0</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <v>7</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L8" s="8" t="str">
+      <c r="K8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I8,I$9:I$15,0))</f>
         <v>Sprocket Bats</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>5</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>5</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>5</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="H9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="14">
         <v>7</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="17">
         <f t="shared" si="0"/>
         <v>5.416666666666667</v>
       </c>
-      <c r="K9" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="14" t="str">
+      <c r="K9" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="13" t="str">
         <f>INDEX(A$2:A$8,MATCH(I9,I$2:I$8,0))</f>
         <v>Curtain Ghost</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>0</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>0</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>5</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="14">
         <v>1</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="17">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="K10" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" s="14" t="str">
+      <c r="K10" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="13" t="str">
         <f t="shared" ref="L10:L15" si="2">INDEX(A$2:A$8,MATCH(I10,I$2:I$8,0))</f>
         <v>Bolt Rats</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>7</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>1</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>1</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="14">
         <v>2</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="17">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
-      <c r="K11" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="L11" s="14" t="str">
+      <c r="K11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Friendly Can of Lube</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>8</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>5</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>3</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="14">
         <v>4</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="17">
         <f t="shared" si="0"/>
         <v>5.166666666666667</v>
       </c>
-      <c r="K12" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="14" t="str">
+      <c r="K12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Minor Ductwork</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>6</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>6</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>2</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="14">
         <v>3</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="17">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="K13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="L13" s="14" t="str">
+      <c r="K13" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Socket Wrench Puppy</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>8</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>4</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>4</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="14">
         <v>5</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="17">
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="K14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" s="14" t="str">
+      <c r="K14" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Rusty the Toolbox</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>5</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>1</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>1</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="I15" s="15">
+      <c r="H15" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="14">
         <v>6</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <f t="shared" si="0"/>
         <v>2.083333333333333</v>
       </c>
-      <c r="K15" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="L15" s="14" t="str">
+      <c r="K15" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="L15" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Tetanus Worms</v>
       </c>
@@ -1544,12 +1542,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">

</xml_diff>

<commit_message>
Balancing and naming changes
  * Bolt rats are more worthwhile to kill
  * Bolt rats are more of a metal generator than Fabric-to-Oil
  * Sewing Machine --> Jacket Wraith
  * More oil to be in line with the economy (Minor Ductwork, Tetanus Worms)
  * "Use" --> "Ditch" for insta-slaughter powers
  * The Crusher has another way to beat it with the Strong Magnet
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -79,18 +79,12 @@
     <t>Tetanus Worms</t>
   </si>
   <si>
-    <t>Curtain Ghost</t>
-  </si>
-  <si>
     <t>Big</t>
   </si>
   <si>
     <t>Major Ductwork</t>
   </si>
   <si>
-    <t>Sprocket Bats</t>
-  </si>
-  <si>
     <t>Recipe</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>Build</t>
   </si>
   <si>
-    <t>3:1:1 Metal:Fabric:Oil</t>
-  </si>
-  <si>
     <t>Socket Wrench Puppy</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
   </si>
   <si>
     <t>Petulant Tig Welder</t>
-  </si>
-  <si>
-    <t>Sewing Machine</t>
   </si>
   <si>
     <t>Tote Bag
@@ -158,10 +146,6 @@
     <t>1:1 Oil:Duct Tape</t>
   </si>
   <si>
-    <t>13 HP. 3 ATK. 
- ⃠ Use Fireball</t>
-  </si>
-  <si>
     <t>Use for +1 Carry</t>
   </si>
   <si>
@@ -172,10 +156,6 @@
  ⃠ Have Strong Magnet</t>
   </si>
   <si>
-    <t>14 HP. 2 ATK.
- ⃠ Use Bandages</t>
-  </si>
-  <si>
     <t>+1 ATK for 1 Oil</t>
   </si>
   <si>
@@ -239,13 +219,7 @@
 for 2 Metal</t>
   </si>
   <si>
-    <t>Recover 2 HP for 1 Oil, any time</t>
-  </si>
-  <si>
     <t>Use in battle for -5 Creature HP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain 2 Metal at beginning of each Round </t>
   </si>
   <si>
     <t>May convert 3/2/1 Metal/Fabric/Oil to 1 Duct Tape any time</t>
@@ -286,9 +260,6 @@
     <t>Fabric dealer. Tote bags.</t>
   </si>
   <si>
-    <t>Metal dealer. Good to beat if you have a tote bag</t>
-  </si>
-  <si>
     <t>Oil dealer, but you need a good volume of Metal.</t>
   </si>
   <si>
@@ -317,10 +288,6 @@
   </si>
   <si>
     <t>Metal dealer, but you need lots of fabric. Or lots of Metal.</t>
-  </si>
-  <si>
-    <t>15 HP. 3 ATK.
- ⃠ Use Tote Bag</t>
   </si>
   <si>
     <t>11 HP. 4 ATK
@@ -355,12 +322,65 @@
   <si>
     <t>Strong Magnet
 for 3 Metal</t>
+  </si>
+  <si>
+    <t>Metal dealer. Good to beat if you have a tote bag.</t>
+  </si>
+  <si>
+    <t>14 HP. 2 ATK.
+ ⃠ Ditch Bandages</t>
+  </si>
+  <si>
+    <t>15 HP. 3 ATK.
+ ⃠ Ditch Tote Bag</t>
+  </si>
+  <si>
+    <t>13 HP. 3 ATK. 
+ ⃠ Ditch Fireball</t>
+  </si>
+  <si>
+    <t>20 HP. 4 ATK.
+Creature has 15 HP if you have Strong Magnet</t>
+  </si>
+  <si>
+    <t>Recover 3 HP for 1 Oil, any time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain 2 Metal at first encounter each round </t>
+  </si>
+  <si>
+    <t>% Total</t>
+  </si>
+  <si>
+    <t>4/3/2 %</t>
+  </si>
+  <si>
+    <t>Jacket Wraith</t>
+  </si>
+  <si>
+    <t>Ugly Sweater Ghost</t>
+  </si>
+  <si>
+    <t>3:2 Metal:Fabric
+or 3:1 Metal:Oil</t>
+  </si>
+  <si>
+    <t>Sprocket Snake</t>
+  </si>
+  <si>
+    <t>% Small</t>
+  </si>
+  <si>
+    <t>% Big</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,7 +454,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,6 +526,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -821,7 +844,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,22 +884,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -887,7 +910,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -895,24 +918,24 @@
       <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
+      <c r="F2" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I2" s="8">
         <v>1</v>
       </c>
       <c r="J2" s="10">
         <f>C2/4 + D2/3+E2/2</f>
-        <v>1.25</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>77</v>
+        <v>1.75</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="L2" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I2,I$9:I$15,0))</f>
@@ -921,7 +944,7 @@
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -936,13 +959,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I3" s="8">
         <v>2</v>
@@ -952,7 +975,7 @@
         <v>1.8333333333333333</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L3" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I3,I$9:I$15,0))</f>
@@ -961,7 +984,7 @@
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
@@ -976,10 +999,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>10</v>
@@ -992,11 +1015,11 @@
         <v>1</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L4" s="7" t="str">
         <f t="shared" ref="L4:L7" si="1">INDEX(A$9:A$15,MATCH(I4,I$9:I$15,0))</f>
-        <v>Sewing Machine</v>
+        <v>Jacket Wraith</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1013,26 +1036,26 @@
         <v>1</v>
       </c>
       <c r="E5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>90</v>
       </c>
       <c r="I5" s="8">
         <v>4</v>
       </c>
       <c r="J5" s="10">
         <f t="shared" si="0"/>
-        <v>1.5833333333333333</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="L5" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1041,7 +1064,7 @@
     </row>
     <row r="6" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -1056,13 +1079,13 @@
         <v>2</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I6" s="8">
         <v>5</v>
@@ -1072,7 +1095,7 @@
         <v>3.333333333333333</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="L6" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1090,29 +1113,29 @@
         <v>5</v>
       </c>
       <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I7" s="8">
         <v>6</v>
       </c>
       <c r="J7" s="10">
         <f t="shared" si="0"/>
-        <v>1.9166666666666665</v>
+        <v>2.25</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="L7" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1121,7 +1144,7 @@
     </row>
     <row r="8" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -1136,13 +1159,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I8" s="8">
         <v>7</v>
@@ -1152,19 +1175,19 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="L8" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I8,I$9:I$15,0))</f>
-        <v>Sprocket Bats</v>
+        <v>Sprocket Snake</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>16</v>
+      <c r="A9" s="18" t="s">
+        <v>101</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="14">
         <v>5</v>
@@ -1176,13 +1199,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I9" s="14">
         <v>7</v>
@@ -1192,11 +1215,11 @@
         <v>5.416666666666667</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="L9" s="13" t="str">
         <f>INDEX(A$2:A$8,MATCH(I9,I$2:I$8,0))</f>
-        <v>Curtain Ghost</v>
+        <v>Ugly Sweater Ghost</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1204,7 +1227,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="14">
         <v>0</v>
@@ -1216,13 +1239,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="I10" s="14">
         <v>1</v>
@@ -1232,7 +1255,7 @@
         <v>2.5</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="L10" s="13" t="str">
         <f t="shared" ref="L10:L15" si="2">INDEX(A$2:A$8,MATCH(I10,I$2:I$8,0))</f>
@@ -1241,10 +1264,10 @@
     </row>
     <row r="11" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="14">
         <v>7</v>
@@ -1256,13 +1279,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I11" s="14">
         <v>2</v>
@@ -1272,7 +1295,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="L11" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1281,10 +1304,10 @@
     </row>
     <row r="12" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="14">
         <v>8</v>
@@ -1296,13 +1319,13 @@
         <v>3</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I12" s="14">
         <v>4</v>
@@ -1312,7 +1335,7 @@
         <v>5.166666666666667</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="L12" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1320,11 +1343,11 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>36</v>
+      <c r="A13" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="14">
         <v>6</v>
@@ -1336,13 +1359,13 @@
         <v>2</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I13" s="14">
         <v>3</v>
@@ -1352,19 +1375,19 @@
         <v>4.5</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L13" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Socket Wrench Puppy</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="14">
         <v>8</v>
@@ -1376,13 +1399,13 @@
         <v>4</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="I14" s="14">
         <v>5</v>
@@ -1392,7 +1415,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="L14" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1401,10 +1424,10 @@
     </row>
     <row r="15" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="14">
         <v>5</v>
@@ -1416,13 +1439,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I15" s="14">
         <v>6</v>
@@ -1432,7 +1455,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="L15" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1450,7 +1473,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,66 +1485,66 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1534,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1570,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1564,7 +1587,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1573,15 +1596,15 @@
       </c>
       <c r="B3" s="1">
         <f>SUM(Cards!C2:C8)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <f>SUM(Cards!D2:D8)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(Cards!E2:E8)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(Cards!F2:F8)</f>
@@ -1590,7 +1613,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <f>SUM(Cards!C9:C15)</f>
@@ -1611,23 +1634,91 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1">
         <f>SUM(Cards!D2:D15)</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <f>SUM(Cards!E2:E15)</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
         <f>SUM(Cards!F2:F15)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="25">
+        <f>B3/SUM($B3:$D3)</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="C6" s="25">
+        <f t="shared" ref="C6:D7" si="0">C3/SUM($B3:$D3)</f>
+        <v>0.29545454545454547</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="25">
+        <f>B4/SUM($B4:$D4)</f>
+        <v>0.47560975609756095</v>
+      </c>
+      <c r="C7" s="25">
+        <f t="shared" si="0"/>
+        <v>0.26829268292682928</v>
+      </c>
+      <c r="D7" s="25">
+        <f t="shared" si="0"/>
+        <v>0.25609756097560976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="25">
+        <f>B5/SUM($B5:$D5)</f>
+        <v>0.46825396825396826</v>
+      </c>
+      <c r="C8" s="25">
+        <f>C5/SUM($B5:$D5)</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D8" s="25">
+        <f>D5/SUM($B5:$D5)</f>
+        <v>0.25396825396825395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="25">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C9" s="25">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="25">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
     </row>
   </sheetData>
@@ -1635,6 +1726,6 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
balance changes for 6.0, and a thematic choice
* Whacking plank is cheaper to get
* Carry can be gained by defeating Toolbox.
* Fabric is a little more prevalent economically
* Tetanus Worms are tough little bastards
* Can of Lube --> Tig Welder is a little nicer now
* Bandage healing can be done with Duct Tape.
* Oil Rag (formerly Pan) is a generator from barters
* Tape Dispensor is a generator too.

With these changes, it should be a tad less about immediately gaining Carry (Toolbox, and Bandages healing). Duct Tape should be more useful as well.

Also: I'm not going to name any creatures. They don't talk. They're just animals. So now it's just "Rusted-out Toolbox".
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -152,10 +152,6 @@
     <t>15 HP. 2 ATK.</t>
   </si>
   <si>
-    <t>8 HP. 3 ATK.
- ⃠ Have Strong Magnet</t>
-  </si>
-  <si>
     <t>+1 ATK for 1 Oil</t>
   </si>
   <si>
@@ -172,9 +168,6 @@
     <t>Est. Value</t>
   </si>
   <si>
-    <t>10 HP. 3 ATK.</t>
-  </si>
-  <si>
     <t>16 HP. 3 ATK.
  ⃠ Have Strong Magnet</t>
   </si>
@@ -188,10 +181,6 @@
     <t>+2 Metal and +2 Fabric for 2 Oil</t>
   </si>
   <si>
-    <t>Whacking Plank
-for 3 Metal, 1 Duct tape</t>
-  </si>
-  <si>
     <t>Bandages
 for 1 Fabric, 1 Duct Tape</t>
   </si>
@@ -222,15 +211,6 @@
     <t>Use in battle for -5 Creature HP</t>
   </si>
   <si>
-    <t>May convert 3/2/1 Metal/Fabric/Oil to 1 Duct Tape any time</t>
-  </si>
-  <si>
-    <t>Gain +1 Oil after each battle</t>
-  </si>
-  <si>
-    <t>Oil Pan</t>
-  </si>
-  <si>
     <t>Oil Pan
 for 3 Metal, 1 Duct Tape</t>
   </si>
@@ -254,9 +234,6 @@
     <t>Attack creature, but now with metal.</t>
   </si>
   <si>
-    <t>General store. Everything is balanced against him.</t>
-  </si>
-  <si>
     <t>Fabric dealer. Tote bags.</t>
   </si>
   <si>
@@ -273,9 +250,6 @@
   </si>
   <si>
     <t>Duct tape dealer.</t>
-  </si>
-  <si>
-    <t>Trainer</t>
   </si>
   <si>
     <t>Duct tape dealer, but with oil.</t>
@@ -297,9 +271,6 @@
     <t>Friendly Can of Lube</t>
   </si>
   <si>
-    <t>Rusty the Toolbox</t>
-  </si>
-  <si>
     <t>3:2 Fabric:Duct Tape</t>
   </si>
   <si>
@@ -343,9 +314,6 @@
 Creature has 15 HP if you have Strong Magnet</t>
   </si>
   <si>
-    <t>Recover 3 HP for 1 Oil, any time</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gain 2 Metal at first encounter each round </t>
   </si>
   <si>
@@ -372,6 +340,39 @@
   </si>
   <si>
     <t>% Big</t>
+  </si>
+  <si>
+    <t>Recover 3 HP for 1 Oil, or 5 HP for 1 Duct Tape, any time</t>
+  </si>
+  <si>
+    <t>Gain +1 Oil on any Barter that involves Oil.</t>
+  </si>
+  <si>
+    <t>Oil Rag</t>
+  </si>
+  <si>
+    <t>Gain 1 Duct Tape at first encounter each round</t>
+  </si>
+  <si>
+    <t>10 HP. 3 ATK.
++1 Carry upon Defeat</t>
+  </si>
+  <si>
+    <t>General store. Everything is balanced against him. An extra way to get Carry too. Turns into Crusher though.</t>
+  </si>
+  <si>
+    <t>Whacking Plank
+for 2 Metal, 1 Fabric</t>
+  </si>
+  <si>
+    <t>Trainer. They bite!</t>
+  </si>
+  <si>
+    <t>8 HP. 4 ATK.
+ ⃠ Have Strong Magnet</t>
+  </si>
+  <si>
+    <t>Rusted-out Toolbox</t>
   </si>
 </sst>
 </file>
@@ -525,10 +526,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -844,7 +845,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,16 +891,16 @@
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -919,13 +920,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I2" s="8">
         <v>1</v>
@@ -935,7 +936,7 @@
         <v>1.75</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="L2" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I2,I$9:I$15,0))</f>
@@ -944,38 +945,38 @@
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
         <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
       </c>
       <c r="E3" s="8">
         <v>3</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="I3" s="8">
         <v>2</v>
       </c>
       <c r="J3" s="10">
         <f t="shared" ref="J3:J15" si="0">C3/4 + D3/3+E3/2</f>
-        <v>1.8333333333333333</v>
+        <v>2</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="L3" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I3,I$9:I$15,0))</f>
@@ -999,10 +1000,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>10</v>
@@ -1015,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L4" s="7" t="str">
         <f t="shared" ref="L4:L7" si="1">INDEX(A$9:A$15,MATCH(I4,I$9:I$15,0))</f>
@@ -1033,29 +1034,29 @@
         <v>3</v>
       </c>
       <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="E5" s="8">
-        <v>2</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I5" s="8">
         <v>4</v>
       </c>
       <c r="J5" s="10">
         <f t="shared" si="0"/>
-        <v>2.083333333333333</v>
+        <v>2.25</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L5" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1064,7 +1065,7 @@
     </row>
     <row r="6" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -1082,10 +1083,10 @@
         <v>26</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="I6" s="8">
         <v>5</v>
@@ -1094,8 +1095,8 @@
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>67</v>
+      <c r="K6" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="L6" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1119,13 +1120,13 @@
         <v>2</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="9" t="s">
         <v>37</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="I7" s="8">
         <v>6</v>
@@ -1135,7 +1136,7 @@
         <v>2.25</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="L7" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1144,7 +1145,7 @@
     </row>
     <row r="8" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -1159,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>33</v>
@@ -1175,7 +1176,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L8" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(I8,I$9:I$15,0))</f>
@@ -1184,7 +1185,7 @@
     </row>
     <row r="9" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>13</v>
@@ -1199,13 +1200,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I9" s="14">
         <v>7</v>
@@ -1215,7 +1216,7 @@
         <v>5.416666666666667</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="L9" s="13" t="str">
         <f>INDEX(A$2:A$8,MATCH(I9,I$2:I$8,0))</f>
@@ -1242,10 +1243,10 @@
         <v>34</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I10" s="14">
         <v>1</v>
@@ -1255,7 +1256,7 @@
         <v>2.5</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="L10" s="13" t="str">
         <f t="shared" ref="L10:L15" si="2">INDEX(A$2:A$8,MATCH(I10,I$2:I$8,0))</f>
@@ -1279,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11" s="14">
         <v>2</v>
@@ -1295,7 +1296,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L11" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1319,13 +1320,13 @@
         <v>3</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="14">
         <v>4</v>
@@ -1335,7 +1336,7 @@
         <v>5.166666666666667</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="L12" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1344,7 +1345,7 @@
     </row>
     <row r="13" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>13</v>
@@ -1359,13 +1360,13 @@
         <v>2</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I13" s="14">
         <v>3</v>
@@ -1375,7 +1376,7 @@
         <v>4.5</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="L13" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1399,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I14" s="14">
         <v>5</v>
@@ -1415,11 +1416,11 @@
         <v>5.333333333333333</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="L14" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>Rusty the Toolbox</v>
+        <v>Rusted-out Toolbox</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1439,13 +1440,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="I15" s="14">
         <v>6</v>
@@ -1455,7 +1456,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="L15" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1473,7 +1474,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,15 +1505,15 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1521,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1529,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1569,12 +1570,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1596,15 +1597,15 @@
       </c>
       <c r="B3" s="1">
         <f>SUM(Cards!C2:C8)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1">
         <f>SUM(Cards!D2:D8)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(Cards!E2:E8)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(Cards!F2:F8)</f>
@@ -1638,15 +1639,15 @@
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <f>SUM(Cards!D2:D15)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1">
         <f>SUM(Cards!E2:E15)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1">
         <f>SUM(Cards!F2:F15)</f>
@@ -1655,68 +1656,68 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="25">
+        <v>92</v>
+      </c>
+      <c r="B6" s="24">
         <f>B3/SUM($B3:$D3)</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="C6" s="25">
+        <v>0.47826086956521741</v>
+      </c>
+      <c r="C6" s="24">
         <f t="shared" ref="C6:D7" si="0">C3/SUM($B3:$D3)</f>
-        <v>0.29545454545454547</v>
-      </c>
-      <c r="D6" s="25">
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="D6" s="24">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.21739130434782608</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="25">
+        <v>93</v>
+      </c>
+      <c r="B7" s="24">
         <f>B4/SUM($B4:$D4)</f>
         <v>0.47560975609756095</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <f t="shared" si="0"/>
         <v>0.26829268292682928</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <f t="shared" si="0"/>
         <v>0.25609756097560976</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="25">
+        <v>86</v>
+      </c>
+      <c r="B8" s="24">
         <f>B5/SUM($B5:$D5)</f>
-        <v>0.46825396825396826</v>
-      </c>
-      <c r="C8" s="25">
+        <v>0.4765625</v>
+      </c>
+      <c r="C8" s="24">
         <f>C5/SUM($B5:$D5)</f>
-        <v>0.27777777777777779</v>
-      </c>
-      <c r="D8" s="25">
+        <v>0.28125</v>
+      </c>
+      <c r="D8" s="24">
         <f>D5/SUM($B5:$D5)</f>
-        <v>0.25396825396825395</v>
+        <v>0.2421875</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="25">
+        <v>87</v>
+      </c>
+      <c r="B9" s="24">
         <f>4/9</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <f>3/9</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <f>2/9</f>
         <v>0.22222222222222221</v>
       </c>

</xml_diff>

<commit_message>
playtesting: made excel sheet to track
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
     <sheet name="Tools" sheetId="2" r:id="rId2"/>
     <sheet name="Economy" sheetId="3" r:id="rId3"/>
+    <sheet name="Playtest" sheetId="4" r:id="rId4"/>
+    <sheet name="Playtest Options" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="game" localSheetId="0">Cards!$A$1:$H$17</definedName>
+    <definedName name="game" localSheetId="0">Cards!$A$1:$J$17</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -373,6 +378,54 @@
   </si>
   <si>
     <t>Rusted-out Toolbox</t>
+  </si>
+  <si>
+    <t>Playtest#</t>
+  </si>
+  <si>
+    <t>Creature</t>
+  </si>
+  <si>
+    <t>RND</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Starting out</t>
+  </si>
+  <si>
+    <t>Carry</t>
+  </si>
+  <si>
+    <t>Choices</t>
+  </si>
+  <si>
+    <t>Net Worth</t>
+  </si>
+  <si>
+    <t>Win%</t>
+  </si>
+  <si>
+    <t>Battle Creature HP</t>
+  </si>
+  <si>
+    <t>Battle Creature ATK</t>
+  </si>
+  <si>
+    <t>Win %</t>
   </si>
 </sst>
 </file>
@@ -455,7 +508,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -532,6 +585,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -549,6 +617,315 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="combat_sim_results"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+          <cell r="B2">
+            <v>0</v>
+          </cell>
+          <cell r="C2">
+            <v>1</v>
+          </cell>
+          <cell r="D2">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>1</v>
+          </cell>
+          <cell r="C3">
+            <v>1</v>
+          </cell>
+          <cell r="D3">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>1</v>
+          </cell>
+          <cell r="C4">
+            <v>1</v>
+          </cell>
+          <cell r="D4">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>1</v>
+          </cell>
+          <cell r="C5">
+            <v>1</v>
+          </cell>
+          <cell r="D5">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>1</v>
+          </cell>
+          <cell r="C6">
+            <v>2</v>
+          </cell>
+          <cell r="D6">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>1</v>
+          </cell>
+          <cell r="C7">
+            <v>2</v>
+          </cell>
+          <cell r="D7">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>1</v>
+          </cell>
+          <cell r="C8">
+            <v>2</v>
+          </cell>
+          <cell r="D8">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1</v>
+          </cell>
+          <cell r="C9">
+            <v>2</v>
+          </cell>
+          <cell r="D9">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>1</v>
+          </cell>
+          <cell r="C10">
+            <v>3</v>
+          </cell>
+          <cell r="D10">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>1</v>
+          </cell>
+          <cell r="C11">
+            <v>3</v>
+          </cell>
+          <cell r="D11">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1</v>
+          </cell>
+          <cell r="C12">
+            <v>3</v>
+          </cell>
+          <cell r="D12">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>1</v>
+          </cell>
+          <cell r="C13">
+            <v>3</v>
+          </cell>
+          <cell r="D13">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>1</v>
+          </cell>
+          <cell r="C14">
+            <v>4</v>
+          </cell>
+          <cell r="D14">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>1</v>
+          </cell>
+          <cell r="C15">
+            <v>4</v>
+          </cell>
+          <cell r="D15">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>1</v>
+          </cell>
+          <cell r="C16">
+            <v>4</v>
+          </cell>
+          <cell r="D16">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>1</v>
+          </cell>
+          <cell r="C17">
+            <v>4</v>
+          </cell>
+          <cell r="D17">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>1</v>
+          </cell>
+          <cell r="C18">
+            <v>5</v>
+          </cell>
+          <cell r="D18">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>1</v>
+          </cell>
+          <cell r="C19">
+            <v>5</v>
+          </cell>
+          <cell r="D19">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>1</v>
+          </cell>
+          <cell r="C20">
+            <v>5</v>
+          </cell>
+          <cell r="D20">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>1</v>
+          </cell>
+          <cell r="C21">
+            <v>5</v>
+          </cell>
+          <cell r="D21">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>1</v>
+          </cell>
+          <cell r="C22">
+            <v>6</v>
+          </cell>
+          <cell r="D22">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>1</v>
+          </cell>
+          <cell r="C23">
+            <v>6</v>
+          </cell>
+          <cell r="D23">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>1</v>
+          </cell>
+          <cell r="C24">
+            <v>6</v>
+          </cell>
+          <cell r="D24">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>1</v>
+          </cell>
+          <cell r="C25">
+            <v>6</v>
+          </cell>
+          <cell r="D25">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="10000">
+          <cell r="A10000">
+            <v>20</v>
+          </cell>
+          <cell r="B10000">
+            <v>4</v>
+          </cell>
+          <cell r="C10000">
+            <v>25</v>
+          </cell>
+          <cell r="D10000">
+            <v>4</v>
+          </cell>
+          <cell r="E10000">
+            <v>0.85899999999999999</v>
+          </cell>
+        </row>
+        <row r="10001">
+          <cell r="C10001">
+            <v>25</v>
+          </cell>
+          <cell r="D10001">
+            <v>5</v>
+          </cell>
+          <cell r="E10001">
+            <v>0.64600000000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -842,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,17 +1232,19 @@
     <col min="3" max="3" width="6.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="22"/>
-    <col min="11" max="11" width="66" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="20"/>
+    <col min="6" max="6" width="3.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="22"/>
+    <col min="13" max="13" width="66" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -881,29 +1260,35 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -919,31 +1304,37 @@
       <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="8">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="I2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="8">
-        <v>1</v>
-      </c>
-      <c r="J2" s="10">
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10">
         <f>C2/4 + D2/3+E2/2</f>
         <v>1.75</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="7" t="str">
-        <f>INDEX(A$9:A$15,MATCH(I2,I$9:I$15,0))</f>
+      <c r="N2" s="7" t="str">
+        <f>INDEX(A$9:A$15,MATCH(K2,K$9:K$15,0))</f>
         <v>Oil Nymph</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
@@ -959,31 +1350,37 @@
       <c r="E3" s="8">
         <v>3</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="8">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+      <c r="H3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="8">
+      <c r="K3" s="8">
         <v>2</v>
       </c>
-      <c r="J3" s="10">
-        <f t="shared" ref="J3:J15" si="0">C3/4 + D3/3+E3/2</f>
+      <c r="L3" s="10">
+        <f t="shared" ref="L3:L15" si="0">C3/4 + D3/3+E3/2</f>
         <v>2</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="7" t="str">
-        <f>INDEX(A$9:A$15,MATCH(I3,I$9:I$15,0))</f>
+      <c r="N3" s="7" t="str">
+        <f>INDEX(A$9:A$15,MATCH(K3,K$9:K$15,0))</f>
         <v>Petulant Tig Welder</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -999,31 +1396,37 @@
       <c r="E4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="8">
+      <c r="K4" s="8">
         <v>3</v>
       </c>
-      <c r="J4" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="7" t="str">
-        <f t="shared" ref="L4:L7" si="1">INDEX(A$9:A$15,MATCH(I4,I$9:I$15,0))</f>
+      <c r="N4" s="7" t="str">
+        <f t="shared" ref="N4:N7" si="1">INDEX(A$9:A$15,MATCH(K4,K$9:K$15,0))</f>
         <v>Jacket Wraith</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1039,31 +1442,37 @@
       <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="J5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="8">
+      <c r="K5" s="8">
         <v>4</v>
       </c>
-      <c r="J5" s="10">
+      <c r="L5" s="10">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="7" t="str">
+      <c r="N5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Major Ductwork</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>103</v>
       </c>
@@ -1079,31 +1488,37 @@
       <c r="E6" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="J6" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="8">
+      <c r="K6" s="8">
         <v>5</v>
       </c>
-      <c r="J6" s="10">
+      <c r="L6" s="10">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L6" s="7" t="str">
+      <c r="N6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>The Crusher</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1119,31 +1534,37 @@
       <c r="E7" s="8">
         <v>2</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="8">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8">
+        <v>4</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="I7" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="J7" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="8">
+      <c r="K7" s="8">
         <v>6</v>
       </c>
-      <c r="J7" s="10">
+      <c r="L7" s="10">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="L7" s="7" t="str">
+      <c r="N7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Tap Spider</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -1159,31 +1580,37 @@
       <c r="E8" s="8">
         <v>0</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="8">
+        <v>15</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="8">
+      <c r="K8" s="8">
         <v>7</v>
       </c>
-      <c r="J8" s="10">
+      <c r="L8" s="10">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="M8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="7" t="str">
-        <f>INDEX(A$9:A$15,MATCH(I8,I$9:I$15,0))</f>
+      <c r="N8" s="7" t="str">
+        <f>INDEX(A$9:A$15,MATCH(K8,K$9:K$15,0))</f>
         <v>Sprocket Snake</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>91</v>
       </c>
@@ -1199,31 +1626,37 @@
       <c r="E9" s="14">
         <v>5</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="14">
+        <v>15</v>
+      </c>
+      <c r="G9" s="14">
+        <v>3</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="14">
+      <c r="K9" s="14">
         <v>7</v>
       </c>
-      <c r="J9" s="17">
+      <c r="L9" s="17">
         <f t="shared" si="0"/>
         <v>5.416666666666667</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="M9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="13" t="str">
-        <f>INDEX(A$2:A$8,MATCH(I9,I$2:I$8,0))</f>
+      <c r="N9" s="13" t="str">
+        <f>INDEX(A$2:A$8,MATCH(K9,K$2:K$8,0))</f>
         <v>Ugly Sweater Ghost</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
@@ -1239,31 +1672,37 @@
       <c r="E10" s="14">
         <v>5</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="14">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14">
+        <v>3</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="17">
+      <c r="K10" s="14">
+        <v>1</v>
+      </c>
+      <c r="L10" s="17">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="M10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L10" s="13" t="str">
-        <f t="shared" ref="L10:L15" si="2">INDEX(A$2:A$8,MATCH(I10,I$2:I$8,0))</f>
+      <c r="N10" s="13" t="str">
+        <f t="shared" ref="N10:N15" si="2">INDEX(A$2:A$8,MATCH(K10,K$2:K$8,0))</f>
         <v>Bolt Rats</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>32</v>
       </c>
@@ -1279,31 +1718,37 @@
       <c r="E11" s="14">
         <v>1</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="14">
+        <v>16</v>
+      </c>
+      <c r="G11" s="14">
+        <v>3</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="14">
+      <c r="K11" s="14">
         <v>2</v>
       </c>
-      <c r="J11" s="17">
+      <c r="L11" s="17">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="M11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="13" t="str">
+      <c r="N11" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Friendly Can of Lube</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
@@ -1319,31 +1764,37 @@
       <c r="E12" s="14">
         <v>3</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="14">
+        <v>20</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4</v>
+      </c>
+      <c r="H12" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="14">
+      <c r="K12" s="14">
         <v>4</v>
       </c>
-      <c r="J12" s="17">
+      <c r="L12" s="17">
         <f t="shared" si="0"/>
         <v>5.166666666666667</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="M12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="13" t="str">
+      <c r="N12" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Minor Ductwork</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>88</v>
       </c>
@@ -1359,31 +1810,37 @@
       <c r="E13" s="14">
         <v>2</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14">
+        <v>17</v>
+      </c>
+      <c r="G13" s="14">
+        <v>4</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="J13" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="14">
+      <c r="K13" s="14">
         <v>3</v>
       </c>
-      <c r="J13" s="17">
+      <c r="L13" s="17">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="M13" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="L13" s="13" t="str">
+      <c r="N13" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Socket Wrench Puppy</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>25</v>
       </c>
@@ -1399,31 +1856,37 @@
       <c r="E14" s="14">
         <v>4</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="14">
+        <v>20</v>
+      </c>
+      <c r="G14" s="14">
+        <v>4</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="I14" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="J14" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="14">
+      <c r="K14" s="14">
         <v>5</v>
       </c>
-      <c r="J14" s="17">
+      <c r="L14" s="17">
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="M14" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="13" t="str">
+      <c r="N14" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Rusted-out Toolbox</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
@@ -1439,26 +1902,32 @@
       <c r="E15" s="14">
         <v>1</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="14">
+        <v>11</v>
+      </c>
+      <c r="G15" s="14">
+        <v>4</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="I15" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="J15" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="14">
+      <c r="K15" s="14">
         <v>6</v>
       </c>
-      <c r="J15" s="17">
+      <c r="L15" s="17">
         <f t="shared" si="0"/>
         <v>2.083333333333333</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="M15" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="13" t="str">
+      <c r="N15" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Tetanus Worms</v>
       </c>
@@ -1474,7 +1943,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,12 +2039,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1608,7 +2077,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1">
-        <f>SUM(Cards!F2:F8)</f>
+        <f>SUM(Cards!H2:H8)</f>
         <v>0</v>
       </c>
     </row>
@@ -1629,7 +2098,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="1">
-        <f>SUM(Cards!F9:F15)</f>
+        <f>SUM(Cards!H9:H15)</f>
         <v>0</v>
       </c>
     </row>
@@ -1650,7 +2119,7 @@
         <v>31</v>
       </c>
       <c r="E5" s="1">
-        <f>SUM(Cards!F2:F15)</f>
+        <f>SUM(Cards!H2:H15)</f>
         <v>0</v>
       </c>
     </row>
@@ -1729,4 +2198,987 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="27" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="18.5703125" style="27" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="6.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" style="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" style="27" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="F2" s="30" t="str">
+        <f>IF(E2="Battle",100,"")</f>
+        <v/>
+      </c>
+      <c r="J2" s="27">
+        <v>4</v>
+      </c>
+      <c r="K2" s="27">
+        <v>3</v>
+      </c>
+      <c r="L2" s="27">
+        <v>1</v>
+      </c>
+      <c r="M2" s="27">
+        <v>0</v>
+      </c>
+      <c r="N2" s="27">
+        <v>0</v>
+      </c>
+      <c r="O2" s="27">
+        <v>10</v>
+      </c>
+      <c r="P2" s="27">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="27">
+        <v>0</v>
+      </c>
+      <c r="R2" s="27">
+        <v>0</v>
+      </c>
+      <c r="S2" s="27">
+        <v>0</v>
+      </c>
+      <c r="T2" s="27">
+        <v>0</v>
+      </c>
+      <c r="U2" s="27">
+        <v>0</v>
+      </c>
+      <c r="V2" s="27">
+        <v>0</v>
+      </c>
+      <c r="W2" s="27">
+        <v>0</v>
+      </c>
+      <c r="X2" s="27">
+        <f>J2/4+K2/3+L2/2+M2</f>
+        <v>2.5</v>
+      </c>
+      <c r="Y2" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27">
+        <v>7</v>
+      </c>
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="30">
+        <f>IF(E3="Battle",I3,"")</f>
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="G3" s="27">
+        <f>VLOOKUP(D3,Cards!A$2:G$15,6)</f>
+        <v>8</v>
+      </c>
+      <c r="H3" s="27">
+        <f>VLOOKUP(D3,Cards!A$2:G$15,7)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="27">
+        <f t="array" ref="I3">INDEX([1]combat_sim_results!A2:'[1]combat_sim_results'!E10000, MATCH(1, ([1]combat_sim_results!C2:'[1]combat_sim_results'!C10000=G3)*([1]combat_sim_results!D2:'[1]combat_sim_results'!D10000=H3)*([1]combat_sim_results!A2:'[1]combat_sim_results'!A10000=O2)*([1]combat_sim_results!B2:'[1]combat_sim_results'!B10000=N2), 0),5)</f>
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="X3" s="27">
+        <f t="shared" ref="X3:X26" si="0">J3/4+K3/3+L3/2+M3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>1</v>
+      </c>
+      <c r="B4" s="27">
+        <v>7</v>
+      </c>
+      <c r="C4" s="27">
+        <v>2</v>
+      </c>
+      <c r="F4" s="30" t="str">
+        <f t="shared" ref="F4:F26" si="1">IF(E4="Battle",I4,"")</f>
+        <v/>
+      </c>
+      <c r="G4" s="27" t="e">
+        <f>VLOOKUP(D4,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H4" s="27" t="e">
+        <f>VLOOKUP(D4,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="27" t="e">
+        <f t="array" ref="I4">INDEX([1]combat_sim_results!A3:'[1]combat_sim_results'!E10001, MATCH(1, ([1]combat_sim_results!C3:'[1]combat_sim_results'!C10001=G4)* ([1]combat_sim_results!D3:'[1]combat_sim_results'!D10001=H4), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X4" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>1</v>
+      </c>
+      <c r="B5" s="27">
+        <v>7</v>
+      </c>
+      <c r="C5" s="27">
+        <v>3</v>
+      </c>
+      <c r="F5" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G5" s="27" t="e">
+        <f>VLOOKUP(D5,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="27" t="e">
+        <f>VLOOKUP(D5,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="27" t="e">
+        <f t="array" ref="I5">INDEX([1]combat_sim_results!A4:'[1]combat_sim_results'!E10002, MATCH(1, ([1]combat_sim_results!C4:'[1]combat_sim_results'!C10002=G5)* ([1]combat_sim_results!D4:'[1]combat_sim_results'!D10002=H5), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X5" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>1</v>
+      </c>
+      <c r="B6" s="27">
+        <v>6</v>
+      </c>
+      <c r="C6" s="27">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G6" s="27" t="e">
+        <f>VLOOKUP(D6,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="27" t="e">
+        <f>VLOOKUP(D6,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="27" t="e">
+        <f t="array" ref="I6">INDEX([1]combat_sim_results!A5:'[1]combat_sim_results'!E10003, MATCH(1, ([1]combat_sim_results!C5:'[1]combat_sim_results'!C10003=G6)* ([1]combat_sim_results!D5:'[1]combat_sim_results'!D10003=H6), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X6" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>1</v>
+      </c>
+      <c r="B7" s="27">
+        <v>6</v>
+      </c>
+      <c r="C7" s="27">
+        <v>2</v>
+      </c>
+      <c r="F7" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G7" s="27" t="e">
+        <f>VLOOKUP(D7,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="27" t="e">
+        <f>VLOOKUP(D7,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="27" t="e">
+        <f t="array" ref="I7">INDEX([1]combat_sim_results!A6:'[1]combat_sim_results'!E10004, MATCH(1, ([1]combat_sim_results!C6:'[1]combat_sim_results'!C10004=G7)* ([1]combat_sim_results!D6:'[1]combat_sim_results'!D10004=H7), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>1</v>
+      </c>
+      <c r="B8" s="27">
+        <v>6</v>
+      </c>
+      <c r="C8" s="27">
+        <v>3</v>
+      </c>
+      <c r="F8" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G8" s="27" t="e">
+        <f>VLOOKUP(D8,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H8" s="27" t="e">
+        <f>VLOOKUP(D8,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I8" s="27" t="e">
+        <f t="array" ref="I8">INDEX([1]combat_sim_results!A7:'[1]combat_sim_results'!E10005, MATCH(1, ([1]combat_sim_results!C7:'[1]combat_sim_results'!C10005=G8)* ([1]combat_sim_results!D7:'[1]combat_sim_results'!D10005=H8), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X8" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>1</v>
+      </c>
+      <c r="B9" s="27">
+        <v>5</v>
+      </c>
+      <c r="C9" s="27">
+        <v>1</v>
+      </c>
+      <c r="F9" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G9" s="27" t="e">
+        <f>VLOOKUP(D9,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H9" s="27" t="e">
+        <f>VLOOKUP(D9,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I9" s="27" t="e">
+        <f t="array" ref="I9">INDEX([1]combat_sim_results!A8:'[1]combat_sim_results'!E10006, MATCH(1, ([1]combat_sim_results!C8:'[1]combat_sim_results'!C10006=G9)* ([1]combat_sim_results!D8:'[1]combat_sim_results'!D10006=H9), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X9" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <v>1</v>
+      </c>
+      <c r="B10" s="27">
+        <v>5</v>
+      </c>
+      <c r="C10" s="27">
+        <v>2</v>
+      </c>
+      <c r="F10" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G10" s="27" t="e">
+        <f>VLOOKUP(D10,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H10" s="27" t="e">
+        <f>VLOOKUP(D10,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I10" s="27" t="e">
+        <f t="array" ref="I10">INDEX([1]combat_sim_results!A9:'[1]combat_sim_results'!E10007, MATCH(1, ([1]combat_sim_results!C9:'[1]combat_sim_results'!C10007=G10)* ([1]combat_sim_results!D9:'[1]combat_sim_results'!D10007=H10), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X10" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <v>1</v>
+      </c>
+      <c r="B11" s="27">
+        <v>5</v>
+      </c>
+      <c r="C11" s="27">
+        <v>3</v>
+      </c>
+      <c r="F11" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G11" s="27" t="e">
+        <f>VLOOKUP(D11,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H11" s="27" t="e">
+        <f>VLOOKUP(D11,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I11" s="27" t="e">
+        <f t="array" ref="I11">INDEX([1]combat_sim_results!A10:'[1]combat_sim_results'!E10008, MATCH(1, ([1]combat_sim_results!C10:'[1]combat_sim_results'!C10008=G11)* ([1]combat_sim_results!D10:'[1]combat_sim_results'!D10008=H11), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X11" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>1</v>
+      </c>
+      <c r="B12" s="27">
+        <v>4</v>
+      </c>
+      <c r="C12" s="27">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G12" s="27" t="e">
+        <f>VLOOKUP(D12,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H12" s="27" t="e">
+        <f>VLOOKUP(D12,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I12" s="27" t="e">
+        <f t="array" ref="I12">INDEX([1]combat_sim_results!A11:'[1]combat_sim_results'!E10009, MATCH(1, ([1]combat_sim_results!C11:'[1]combat_sim_results'!C10009=G12)* ([1]combat_sim_results!D11:'[1]combat_sim_results'!D10009=H12), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X12" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>1</v>
+      </c>
+      <c r="B13" s="27">
+        <v>4</v>
+      </c>
+      <c r="C13" s="27">
+        <v>2</v>
+      </c>
+      <c r="F13" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G13" s="27" t="e">
+        <f>VLOOKUP(D13,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H13" s="27" t="e">
+        <f>VLOOKUP(D13,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I13" s="27" t="e">
+        <f t="array" ref="I13">INDEX([1]combat_sim_results!A12:'[1]combat_sim_results'!E10010, MATCH(1, ([1]combat_sim_results!C12:'[1]combat_sim_results'!C10010=G13)* ([1]combat_sim_results!D12:'[1]combat_sim_results'!D10010=H13), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X13" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <v>1</v>
+      </c>
+      <c r="B14" s="27">
+        <v>4</v>
+      </c>
+      <c r="C14" s="27">
+        <v>3</v>
+      </c>
+      <c r="F14" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G14" s="27" t="e">
+        <f>VLOOKUP(D14,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="27" t="e">
+        <f>VLOOKUP(D14,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I14" s="27" t="e">
+        <f t="array" ref="I14">INDEX([1]combat_sim_results!A13:'[1]combat_sim_results'!E10011, MATCH(1, ([1]combat_sim_results!C13:'[1]combat_sim_results'!C10011=G14)* ([1]combat_sim_results!D13:'[1]combat_sim_results'!D10011=H14), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X14" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <v>1</v>
+      </c>
+      <c r="B15" s="27">
+        <v>3</v>
+      </c>
+      <c r="C15" s="27">
+        <v>1</v>
+      </c>
+      <c r="F15" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G15" s="27" t="e">
+        <f>VLOOKUP(D15,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="27" t="e">
+        <f>VLOOKUP(D15,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I15" s="27" t="e">
+        <f t="array" ref="I15">INDEX([1]combat_sim_results!A14:'[1]combat_sim_results'!E10012, MATCH(1, ([1]combat_sim_results!C14:'[1]combat_sim_results'!C10012=G15)* ([1]combat_sim_results!D14:'[1]combat_sim_results'!D10012=H15), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X15" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>1</v>
+      </c>
+      <c r="B16" s="27">
+        <v>3</v>
+      </c>
+      <c r="C16" s="27">
+        <v>2</v>
+      </c>
+      <c r="F16" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G16" s="27" t="e">
+        <f>VLOOKUP(D16,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H16" s="27" t="e">
+        <f>VLOOKUP(D16,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I16" s="27" t="e">
+        <f t="array" ref="I16">INDEX([1]combat_sim_results!A15:'[1]combat_sim_results'!E10013, MATCH(1, ([1]combat_sim_results!C15:'[1]combat_sim_results'!C10013=G16)* ([1]combat_sim_results!D15:'[1]combat_sim_results'!D10013=H16), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X16" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <v>1</v>
+      </c>
+      <c r="B17" s="27">
+        <v>3</v>
+      </c>
+      <c r="C17" s="27">
+        <v>3</v>
+      </c>
+      <c r="F17" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G17" s="27" t="e">
+        <f>VLOOKUP(D17,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H17" s="27" t="e">
+        <f>VLOOKUP(D17,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I17" s="27" t="e">
+        <f t="array" ref="I17">INDEX([1]combat_sim_results!A16:'[1]combat_sim_results'!E10014, MATCH(1, ([1]combat_sim_results!C16:'[1]combat_sim_results'!C10014=G17)* ([1]combat_sim_results!D16:'[1]combat_sim_results'!D10014=H17), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X17" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>1</v>
+      </c>
+      <c r="B18" s="27">
+        <v>2</v>
+      </c>
+      <c r="C18" s="27">
+        <v>1</v>
+      </c>
+      <c r="F18" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G18" s="27" t="e">
+        <f>VLOOKUP(D18,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H18" s="27" t="e">
+        <f>VLOOKUP(D18,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I18" s="27" t="e">
+        <f t="array" ref="I18">INDEX([1]combat_sim_results!A17:'[1]combat_sim_results'!E10015, MATCH(1, ([1]combat_sim_results!C17:'[1]combat_sim_results'!C10015=G18)* ([1]combat_sim_results!D17:'[1]combat_sim_results'!D10015=H18), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X18" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>1</v>
+      </c>
+      <c r="B19" s="27">
+        <v>2</v>
+      </c>
+      <c r="C19" s="27">
+        <v>2</v>
+      </c>
+      <c r="F19" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G19" s="27" t="e">
+        <f>VLOOKUP(D19,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H19" s="27" t="e">
+        <f>VLOOKUP(D19,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I19" s="27" t="e">
+        <f t="array" ref="I19">INDEX([1]combat_sim_results!A18:'[1]combat_sim_results'!E10016, MATCH(1, ([1]combat_sim_results!C18:'[1]combat_sim_results'!C10016=G19)* ([1]combat_sim_results!D18:'[1]combat_sim_results'!D10016=H19), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X19" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>1</v>
+      </c>
+      <c r="B20" s="27">
+        <v>2</v>
+      </c>
+      <c r="C20" s="27">
+        <v>3</v>
+      </c>
+      <c r="F20" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G20" s="27" t="e">
+        <f>VLOOKUP(D20,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H20" s="27" t="e">
+        <f>VLOOKUP(D20,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I20" s="27" t="e">
+        <f t="array" ref="I20">INDEX([1]combat_sim_results!A19:'[1]combat_sim_results'!E10017, MATCH(1, ([1]combat_sim_results!C19:'[1]combat_sim_results'!C10017=G20)* ([1]combat_sim_results!D19:'[1]combat_sim_results'!D10017=H20), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X20" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
+        <v>1</v>
+      </c>
+      <c r="B21" s="27">
+        <v>1</v>
+      </c>
+      <c r="C21" s="27">
+        <v>1</v>
+      </c>
+      <c r="F21" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G21" s="27" t="e">
+        <f>VLOOKUP(D21,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H21" s="27" t="e">
+        <f>VLOOKUP(D21,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I21" s="27" t="e">
+        <f t="array" ref="I21">INDEX([1]combat_sim_results!A20:'[1]combat_sim_results'!E10018, MATCH(1, ([1]combat_sim_results!C20:'[1]combat_sim_results'!C10018=G21)* ([1]combat_sim_results!D20:'[1]combat_sim_results'!D10018=H21), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X21" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
+        <v>1</v>
+      </c>
+      <c r="B22" s="27">
+        <v>1</v>
+      </c>
+      <c r="C22" s="27">
+        <v>2</v>
+      </c>
+      <c r="F22" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G22" s="27" t="e">
+        <f>VLOOKUP(D22,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H22" s="27" t="e">
+        <f>VLOOKUP(D22,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I22" s="27" t="e">
+        <f t="array" ref="I22">INDEX([1]combat_sim_results!A21:'[1]combat_sim_results'!E10019, MATCH(1, ([1]combat_sim_results!C21:'[1]combat_sim_results'!C10019=G22)* ([1]combat_sim_results!D21:'[1]combat_sim_results'!D10019=H22), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X22" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="27">
+        <v>1</v>
+      </c>
+      <c r="B23" s="27">
+        <v>1</v>
+      </c>
+      <c r="C23" s="27">
+        <v>3</v>
+      </c>
+      <c r="F23" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G23" s="27" t="e">
+        <f>VLOOKUP(D23,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H23" s="27" t="e">
+        <f>VLOOKUP(D23,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I23" s="27" t="e">
+        <f t="array" ref="I23">INDEX([1]combat_sim_results!A22:'[1]combat_sim_results'!E10020, MATCH(1, ([1]combat_sim_results!C22:'[1]combat_sim_results'!C10020=G23)* ([1]combat_sim_results!D22:'[1]combat_sim_results'!D10020=H23), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X23" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <v>1</v>
+      </c>
+      <c r="B24" s="27">
+        <v>0</v>
+      </c>
+      <c r="C24" s="27">
+        <v>1</v>
+      </c>
+      <c r="F24" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G24" s="27" t="e">
+        <f>VLOOKUP(D24,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H24" s="27" t="e">
+        <f>VLOOKUP(D24,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I24" s="27" t="e">
+        <f t="array" ref="I24">INDEX([1]combat_sim_results!A23:'[1]combat_sim_results'!E10021, MATCH(1, ([1]combat_sim_results!C23:'[1]combat_sim_results'!C10021=G24)* ([1]combat_sim_results!D23:'[1]combat_sim_results'!D10021=H24), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X24" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
+        <v>1</v>
+      </c>
+      <c r="B25" s="27">
+        <v>0</v>
+      </c>
+      <c r="C25" s="27">
+        <v>2</v>
+      </c>
+      <c r="F25" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G25" s="27" t="e">
+        <f>VLOOKUP(D25,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H25" s="27" t="e">
+        <f>VLOOKUP(D25,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I25" s="27" t="e">
+        <f t="array" ref="I25">INDEX([1]combat_sim_results!A24:'[1]combat_sim_results'!E10022, MATCH(1, ([1]combat_sim_results!C24:'[1]combat_sim_results'!C10022=G25)* ([1]combat_sim_results!D24:'[1]combat_sim_results'!D10022=H25), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X25" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="27">
+        <v>1</v>
+      </c>
+      <c r="B26" s="27">
+        <v>0</v>
+      </c>
+      <c r="C26" s="27">
+        <v>3</v>
+      </c>
+      <c r="F26" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G26" s="27" t="e">
+        <f>VLOOKUP(D26,Cards!A$2:G$15,6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H26" s="27" t="e">
+        <f>VLOOKUP(D26,Cards!A$2:G$15,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I26" s="27" t="e">
+        <f t="array" ref="I26">INDEX([1]combat_sim_results!A25:'[1]combat_sim_results'!E10023, MATCH(1, ([1]combat_sim_results!C25:'[1]combat_sim_results'!C10023=G26)* ([1]combat_sim_results!D25:'[1]combat_sim_results'!D10023=H26), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X26" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F3" formula="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Cards!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Playtest Options'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E26</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
playtest: recorded on spreadsheet
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
     <sheet name="Tools" sheetId="2" r:id="rId2"/>
     <sheet name="Economy" sheetId="3" r:id="rId3"/>
-    <sheet name="Playtest" sheetId="4" r:id="rId4"/>
+    <sheet name="Playtests v6.0" sheetId="4" r:id="rId4"/>
     <sheet name="Playtest Options" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -426,6 +426,15 @@
   </si>
   <si>
     <t>Win %</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>We need to make Tap spider more useful. Improve ATK?</t>
+  </si>
+  <si>
+    <t>Built zeppelin! Beat him pretty easily even with 1 ATK. Soooo many HP.</t>
   </si>
 </sst>
 </file>
@@ -508,7 +517,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,9 +594,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,6 +605,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -645,6 +657,9 @@
           <cell r="A3">
             <v>1</v>
           </cell>
+          <cell r="B3">
+            <v>0</v>
+          </cell>
           <cell r="C3">
             <v>1</v>
           </cell>
@@ -656,6 +671,9 @@
           <cell r="A4">
             <v>1</v>
           </cell>
+          <cell r="B4">
+            <v>0</v>
+          </cell>
           <cell r="C4">
             <v>1</v>
           </cell>
@@ -667,6 +685,9 @@
           <cell r="A5">
             <v>1</v>
           </cell>
+          <cell r="B5">
+            <v>0</v>
+          </cell>
           <cell r="C5">
             <v>1</v>
           </cell>
@@ -678,6 +699,9 @@
           <cell r="A6">
             <v>1</v>
           </cell>
+          <cell r="B6">
+            <v>0</v>
+          </cell>
           <cell r="C6">
             <v>2</v>
           </cell>
@@ -689,6 +713,9 @@
           <cell r="A7">
             <v>1</v>
           </cell>
+          <cell r="B7">
+            <v>0</v>
+          </cell>
           <cell r="C7">
             <v>2</v>
           </cell>
@@ -700,6 +727,9 @@
           <cell r="A8">
             <v>1</v>
           </cell>
+          <cell r="B8">
+            <v>0</v>
+          </cell>
           <cell r="C8">
             <v>2</v>
           </cell>
@@ -711,6 +741,9 @@
           <cell r="A9">
             <v>1</v>
           </cell>
+          <cell r="B9">
+            <v>0</v>
+          </cell>
           <cell r="C9">
             <v>2</v>
           </cell>
@@ -722,6 +755,9 @@
           <cell r="A10">
             <v>1</v>
           </cell>
+          <cell r="B10">
+            <v>0</v>
+          </cell>
           <cell r="C10">
             <v>3</v>
           </cell>
@@ -733,6 +769,9 @@
           <cell r="A11">
             <v>1</v>
           </cell>
+          <cell r="B11">
+            <v>0</v>
+          </cell>
           <cell r="C11">
             <v>3</v>
           </cell>
@@ -744,6 +783,9 @@
           <cell r="A12">
             <v>1</v>
           </cell>
+          <cell r="B12">
+            <v>0</v>
+          </cell>
           <cell r="C12">
             <v>3</v>
           </cell>
@@ -755,6 +797,9 @@
           <cell r="A13">
             <v>1</v>
           </cell>
+          <cell r="B13">
+            <v>0</v>
+          </cell>
           <cell r="C13">
             <v>3</v>
           </cell>
@@ -766,6 +811,9 @@
           <cell r="A14">
             <v>1</v>
           </cell>
+          <cell r="B14">
+            <v>0</v>
+          </cell>
           <cell r="C14">
             <v>4</v>
           </cell>
@@ -777,6 +825,9 @@
           <cell r="A15">
             <v>1</v>
           </cell>
+          <cell r="B15">
+            <v>0</v>
+          </cell>
           <cell r="C15">
             <v>4</v>
           </cell>
@@ -788,6 +839,9 @@
           <cell r="A16">
             <v>1</v>
           </cell>
+          <cell r="B16">
+            <v>0</v>
+          </cell>
           <cell r="C16">
             <v>4</v>
           </cell>
@@ -799,6 +853,9 @@
           <cell r="A17">
             <v>1</v>
           </cell>
+          <cell r="B17">
+            <v>0</v>
+          </cell>
           <cell r="C17">
             <v>4</v>
           </cell>
@@ -810,6 +867,9 @@
           <cell r="A18">
             <v>1</v>
           </cell>
+          <cell r="B18">
+            <v>0</v>
+          </cell>
           <cell r="C18">
             <v>5</v>
           </cell>
@@ -821,28 +881,23 @@
           <cell r="A19">
             <v>1</v>
           </cell>
+          <cell r="B19">
+            <v>0</v>
+          </cell>
           <cell r="C19">
             <v>5</v>
           </cell>
           <cell r="D19">
             <v>3</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>1</v>
-          </cell>
-          <cell r="C20">
-            <v>5</v>
-          </cell>
-          <cell r="D20">
-            <v>4</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
             <v>1</v>
           </cell>
+          <cell r="B21">
+            <v>0</v>
+          </cell>
           <cell r="C21">
             <v>5</v>
           </cell>
@@ -854,6 +909,9 @@
           <cell r="A22">
             <v>1</v>
           </cell>
+          <cell r="B22">
+            <v>0</v>
+          </cell>
           <cell r="C22">
             <v>6</v>
           </cell>
@@ -865,6 +923,9 @@
           <cell r="A23">
             <v>1</v>
           </cell>
+          <cell r="B23">
+            <v>0</v>
+          </cell>
           <cell r="C23">
             <v>6</v>
           </cell>
@@ -876,6 +937,9 @@
           <cell r="A24">
             <v>1</v>
           </cell>
+          <cell r="B24">
+            <v>0</v>
+          </cell>
           <cell r="C24">
             <v>6</v>
           </cell>
@@ -887,6 +951,9 @@
           <cell r="A25">
             <v>1</v>
           </cell>
+          <cell r="B25">
+            <v>0</v>
+          </cell>
           <cell r="C25">
             <v>6</v>
           </cell>
@@ -912,6 +979,12 @@
           </cell>
         </row>
         <row r="10001">
+          <cell r="A10001">
+            <v>20</v>
+          </cell>
+          <cell r="B10001">
+            <v>4</v>
+          </cell>
           <cell r="C10001">
             <v>25</v>
           </cell>
@@ -2039,12 +2112,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -2202,921 +2275,1746 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="27" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="18.5703125" style="27" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="6.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15" style="27" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15" style="27" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="0" style="26" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="26" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="26" customWidth="1"/>
+    <col min="9" max="10" width="18.5703125" style="26" customWidth="1"/>
+    <col min="11" max="12" width="6.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="K1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="L1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="Q1" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="R1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="X1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="Y1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="Z1" s="27" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
-        <v>1</v>
-      </c>
-      <c r="F2" s="30" t="str">
-        <f>IF(E2="Battle",100,"")</f>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="26">
+        <v>1</v>
+      </c>
+      <c r="G2" s="29" t="str">
+        <f>IF(F2="Battle",100,"")</f>
         <v/>
       </c>
-      <c r="J2" s="27">
+      <c r="K2" s="26">
         <v>4</v>
       </c>
-      <c r="K2" s="27">
+      <c r="L2" s="26">
         <v>3</v>
       </c>
-      <c r="L2" s="27">
-        <v>1</v>
-      </c>
-      <c r="M2" s="27">
-        <v>0</v>
-      </c>
-      <c r="N2" s="27">
-        <v>0</v>
-      </c>
-      <c r="O2" s="27">
+      <c r="M2" s="26">
+        <v>1</v>
+      </c>
+      <c r="N2" s="26">
+        <v>0</v>
+      </c>
+      <c r="O2" s="26">
+        <v>0</v>
+      </c>
+      <c r="P2" s="26">
         <v>10</v>
       </c>
-      <c r="P2" s="27">
+      <c r="Q2" s="26">
         <v>3</v>
       </c>
-      <c r="Q2" s="27">
-        <v>0</v>
-      </c>
-      <c r="R2" s="27">
-        <v>0</v>
-      </c>
-      <c r="S2" s="27">
-        <v>0</v>
-      </c>
-      <c r="T2" s="27">
-        <v>0</v>
-      </c>
-      <c r="U2" s="27">
-        <v>0</v>
-      </c>
-      <c r="V2" s="27">
-        <v>0</v>
-      </c>
-      <c r="W2" s="27">
-        <v>0</v>
-      </c>
-      <c r="X2" s="27">
-        <f>J2/4+K2/3+L2/2+M2</f>
+      <c r="R2" s="26">
+        <v>0</v>
+      </c>
+      <c r="S2" s="26">
+        <v>0</v>
+      </c>
+      <c r="T2" s="26">
+        <v>0</v>
+      </c>
+      <c r="U2" s="26">
+        <v>0</v>
+      </c>
+      <c r="V2" s="26">
+        <v>0</v>
+      </c>
+      <c r="W2" s="26">
+        <v>0</v>
+      </c>
+      <c r="X2" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="26">
+        <f>K2/4+L2/3+M2/2+N2</f>
         <v>2.5</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Z2" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
-        <v>1</v>
-      </c>
-      <c r="B3" s="27">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26">
         <v>7</v>
       </c>
-      <c r="C3" s="27">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="30">
-        <f>IF(E3="Battle",I3,"")</f>
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="G3" s="27">
-        <f>VLOOKUP(D3,Cards!A$2:G$15,6)</f>
-        <v>8</v>
-      </c>
-      <c r="H3" s="27">
-        <f>VLOOKUP(D3,Cards!A$2:G$15,7)</f>
+      <c r="D3" s="26">
+        <v>1</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="29" t="str">
+        <f>IF(F3="Battle",J3,"")</f>
+        <v/>
+      </c>
+      <c r="J3" s="26" t="e">
+        <f t="array" ref="J3">INDEX([1]combat_sim_results!A2:'[1]combat_sim_results'!E10000, MATCH(1, ([1]combat_sim_results!C2:'[1]combat_sim_results'!C10000=H3)*([1]combat_sim_results!D2:'[1]combat_sim_results'!D10000=I3)*([1]combat_sim_results!A2:'[1]combat_sim_results'!A10000=P2)*([1]combat_sim_results!B2:'[1]combat_sim_results'!B10000=O2), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K3" s="26">
+        <v>4</v>
+      </c>
+      <c r="L3" s="26">
+        <v>3</v>
+      </c>
+      <c r="M3" s="26">
+        <v>0</v>
+      </c>
+      <c r="N3" s="26">
+        <v>0</v>
+      </c>
+      <c r="O3" s="26">
+        <v>1</v>
+      </c>
+      <c r="P3" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>3</v>
+      </c>
+      <c r="R3" s="26">
+        <v>0</v>
+      </c>
+      <c r="S3" s="26">
+        <v>0</v>
+      </c>
+      <c r="T3" s="26">
+        <v>0</v>
+      </c>
+      <c r="U3" s="26">
+        <v>0</v>
+      </c>
+      <c r="V3" s="26">
+        <v>0</v>
+      </c>
+      <c r="W3" s="26">
+        <v>0</v>
+      </c>
+      <c r="X3" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="26">
+        <f t="shared" ref="Y3:Y26" si="0">K3/4+L3/3+M3/2+N3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="27">
-        <f t="array" ref="I3">INDEX([1]combat_sim_results!A2:'[1]combat_sim_results'!E10000, MATCH(1, ([1]combat_sim_results!C2:'[1]combat_sim_results'!C10000=G3)*([1]combat_sim_results!D2:'[1]combat_sim_results'!D10000=H3)*([1]combat_sim_results!A2:'[1]combat_sim_results'!A10000=O2)*([1]combat_sim_results!B2:'[1]combat_sim_results'!B10000=N2), 0),5)</f>
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="X3" s="27">
-        <f t="shared" ref="X3:X26" si="0">J3/4+K3/3+L3/2+M3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
-        <v>1</v>
-      </c>
-      <c r="B4" s="27">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26">
         <v>7</v>
       </c>
-      <c r="C4" s="27">
+      <c r="D4" s="26">
         <v>2</v>
       </c>
-      <c r="F4" s="30" t="str">
-        <f t="shared" ref="F4:F26" si="1">IF(E4="Battle",I4,"")</f>
+      <c r="E4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="29" t="str">
+        <f t="shared" ref="G4:G26" si="1">IF(F4="Battle",J4,"")</f>
         <v/>
       </c>
-      <c r="G4" s="27" t="e">
-        <f>VLOOKUP(D4,Cards!A$2:G$15,6)</f>
+      <c r="J4" s="26" t="e">
+        <f t="array" ref="J4">INDEX([1]combat_sim_results!A3:'[1]combat_sim_results'!E10001, MATCH(1, ([1]combat_sim_results!C3:'[1]combat_sim_results'!C10001=H4)*([1]combat_sim_results!D3:'[1]combat_sim_results'!D10001=I4)*([1]combat_sim_results!A3:'[1]combat_sim_results'!A10001=P3)*([1]combat_sim_results!B3:'[1]combat_sim_results'!B10001=O3), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H4" s="27" t="e">
-        <f>VLOOKUP(D4,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I4" s="27" t="e">
-        <f t="array" ref="I4">INDEX([1]combat_sim_results!A3:'[1]combat_sim_results'!E10001, MATCH(1, ([1]combat_sim_results!C3:'[1]combat_sim_results'!C10001=G4)* ([1]combat_sim_results!D3:'[1]combat_sim_results'!D10001=H4), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X4" s="27">
+      <c r="K4" s="26">
+        <v>1</v>
+      </c>
+      <c r="L4" s="26">
+        <v>3</v>
+      </c>
+      <c r="M4" s="26">
+        <v>0</v>
+      </c>
+      <c r="N4" s="26">
+        <v>0</v>
+      </c>
+      <c r="O4" s="26">
+        <v>1</v>
+      </c>
+      <c r="P4" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>3</v>
+      </c>
+      <c r="R4" s="26">
+        <v>0</v>
+      </c>
+      <c r="S4" s="26">
+        <v>0</v>
+      </c>
+      <c r="T4" s="26">
+        <v>0</v>
+      </c>
+      <c r="U4" s="26">
+        <v>1</v>
+      </c>
+      <c r="V4" s="26">
+        <v>0</v>
+      </c>
+      <c r="W4" s="26">
+        <v>0</v>
+      </c>
+      <c r="X4" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
-        <v>1</v>
-      </c>
-      <c r="B5" s="27">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B5" s="26">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26">
         <v>7</v>
       </c>
-      <c r="C5" s="27">
+      <c r="D5" s="26">
         <v>3</v>
       </c>
-      <c r="F5" s="30" t="str">
+      <c r="E5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G5" s="27" t="e">
-        <f>VLOOKUP(D5,Cards!A$2:G$15,6)</f>
+      <c r="J5" s="26" t="e">
+        <f t="array" ref="J5">INDEX([1]combat_sim_results!A4:'[1]combat_sim_results'!E10002, MATCH(1, ([1]combat_sim_results!C4:'[1]combat_sim_results'!C10002=H5)*([1]combat_sim_results!D4:'[1]combat_sim_results'!D10002=I5)*([1]combat_sim_results!A4:'[1]combat_sim_results'!A10002=P4)*([1]combat_sim_results!B4:'[1]combat_sim_results'!B10002=O4), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="27" t="e">
-        <f>VLOOKUP(D5,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I5" s="27" t="e">
-        <f t="array" ref="I5">INDEX([1]combat_sim_results!A4:'[1]combat_sim_results'!E10002, MATCH(1, ([1]combat_sim_results!C4:'[1]combat_sim_results'!C10002=G5)* ([1]combat_sim_results!D4:'[1]combat_sim_results'!D10002=H5), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X5" s="27">
+      <c r="K5" s="26">
+        <v>1</v>
+      </c>
+      <c r="L5" s="26">
+        <v>0</v>
+      </c>
+      <c r="M5" s="26">
+        <v>0</v>
+      </c>
+      <c r="N5" s="26">
+        <v>0</v>
+      </c>
+      <c r="O5" s="26">
+        <v>1</v>
+      </c>
+      <c r="P5" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>3</v>
+      </c>
+      <c r="R5" s="26">
+        <v>0</v>
+      </c>
+      <c r="S5" s="26">
+        <v>0</v>
+      </c>
+      <c r="T5" s="26">
+        <v>0</v>
+      </c>
+      <c r="U5" s="26">
+        <v>1</v>
+      </c>
+      <c r="V5" s="26">
+        <v>0</v>
+      </c>
+      <c r="W5" s="26">
+        <v>1</v>
+      </c>
+      <c r="X5" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
-        <v>1</v>
-      </c>
-      <c r="B6" s="27">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B6" s="26">
+        <v>1</v>
+      </c>
+      <c r="C6" s="26">
         <v>6</v>
       </c>
-      <c r="C6" s="27">
-        <v>1</v>
-      </c>
-      <c r="F6" s="30" t="str">
+      <c r="D6" s="26">
+        <v>1</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="29">
+        <f t="shared" si="1"/>
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H6" s="26">
+        <v>14</v>
+      </c>
+      <c r="I6" s="26">
+        <v>2</v>
+      </c>
+      <c r="J6" s="26">
+        <f t="array" ref="J6">INDEX([1]combat_sim_results!A5:'[1]combat_sim_results'!E10003, MATCH(1, ([1]combat_sim_results!C5:'[1]combat_sim_results'!C10003=H6)*([1]combat_sim_results!D5:'[1]combat_sim_results'!D10003=I6)*([1]combat_sim_results!A5:'[1]combat_sim_results'!A10003=P5)*([1]combat_sim_results!B5:'[1]combat_sim_results'!B10003=O5), 0),5)</f>
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="K6" s="26">
+        <v>6</v>
+      </c>
+      <c r="L6" s="26">
+        <v>3</v>
+      </c>
+      <c r="M6" s="26">
+        <v>1</v>
+      </c>
+      <c r="N6" s="26">
+        <v>0</v>
+      </c>
+      <c r="O6" s="26">
+        <v>1</v>
+      </c>
+      <c r="P6" s="26">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>4</v>
+      </c>
+      <c r="R6" s="26">
+        <v>0</v>
+      </c>
+      <c r="S6" s="26">
+        <v>0</v>
+      </c>
+      <c r="T6" s="26">
+        <v>0</v>
+      </c>
+      <c r="U6" s="26">
+        <v>1</v>
+      </c>
+      <c r="V6" s="26">
+        <v>0</v>
+      </c>
+      <c r="W6" s="26">
+        <v>0</v>
+      </c>
+      <c r="X6" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B7" s="26">
+        <v>1</v>
+      </c>
+      <c r="C7" s="26">
+        <v>6</v>
+      </c>
+      <c r="D7" s="26">
+        <v>2</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G6" s="27" t="e">
-        <f>VLOOKUP(D6,Cards!A$2:G$15,6)</f>
+      <c r="J7" s="26" t="e">
+        <f t="array" ref="J7">INDEX([1]combat_sim_results!A6:'[1]combat_sim_results'!E10004, MATCH(1, ([1]combat_sim_results!C6:'[1]combat_sim_results'!C10004=H7)*([1]combat_sim_results!D6:'[1]combat_sim_results'!D10004=I7)*([1]combat_sim_results!A6:'[1]combat_sim_results'!A10004=P6)*([1]combat_sim_results!B6:'[1]combat_sim_results'!B10004=O6), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H6" s="27" t="e">
-        <f>VLOOKUP(D6,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I6" s="27" t="e">
-        <f t="array" ref="I6">INDEX([1]combat_sim_results!A5:'[1]combat_sim_results'!E10003, MATCH(1, ([1]combat_sim_results!C5:'[1]combat_sim_results'!C10003=G6)* ([1]combat_sim_results!D5:'[1]combat_sim_results'!D10003=H6), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X6" s="27">
+      <c r="K7" s="26">
+        <v>6</v>
+      </c>
+      <c r="L7" s="26">
+        <v>3</v>
+      </c>
+      <c r="M7" s="26">
+        <v>0</v>
+      </c>
+      <c r="N7" s="26">
+        <v>0</v>
+      </c>
+      <c r="O7" s="26">
+        <v>1</v>
+      </c>
+      <c r="P7" s="26">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>4</v>
+      </c>
+      <c r="R7" s="26">
+        <v>0</v>
+      </c>
+      <c r="S7" s="26">
+        <v>0</v>
+      </c>
+      <c r="T7" s="26">
+        <v>0</v>
+      </c>
+      <c r="U7" s="26">
+        <v>1</v>
+      </c>
+      <c r="V7" s="26">
+        <v>0</v>
+      </c>
+      <c r="W7" s="26">
+        <v>0</v>
+      </c>
+      <c r="X7" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="27">
-        <v>1</v>
-      </c>
-      <c r="B7" s="27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="26">
         <v>6</v>
       </c>
-      <c r="C7" s="27">
-        <v>2</v>
-      </c>
-      <c r="F7" s="30" t="str">
+      <c r="D8" s="26">
+        <v>3</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G7" s="27" t="e">
-        <f>VLOOKUP(D7,Cards!A$2:G$15,6)</f>
+      <c r="J8" s="26" t="e">
+        <f t="array" ref="J8">INDEX([1]combat_sim_results!A7:'[1]combat_sim_results'!E10005, MATCH(1, ([1]combat_sim_results!C7:'[1]combat_sim_results'!C10005=H8)*([1]combat_sim_results!D7:'[1]combat_sim_results'!D10005=I8)*([1]combat_sim_results!A7:'[1]combat_sim_results'!A10005=P7)*([1]combat_sim_results!B7:'[1]combat_sim_results'!B10005=O7), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H7" s="27" t="e">
-        <f>VLOOKUP(D7,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I7" s="27" t="e">
-        <f t="array" ref="I7">INDEX([1]combat_sim_results!A6:'[1]combat_sim_results'!E10004, MATCH(1, ([1]combat_sim_results!C6:'[1]combat_sim_results'!C10004=G7)* ([1]combat_sim_results!D6:'[1]combat_sim_results'!D10004=H7), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X7" s="27">
+      <c r="K8" s="26">
+        <v>6</v>
+      </c>
+      <c r="L8" s="26">
+        <v>0</v>
+      </c>
+      <c r="M8" s="26">
+        <v>0</v>
+      </c>
+      <c r="N8" s="26">
+        <v>0</v>
+      </c>
+      <c r="O8" s="26">
+        <v>1</v>
+      </c>
+      <c r="P8" s="26">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>4</v>
+      </c>
+      <c r="R8" s="26">
+        <v>0</v>
+      </c>
+      <c r="S8" s="26">
+        <v>0</v>
+      </c>
+      <c r="T8" s="26">
+        <v>0</v>
+      </c>
+      <c r="U8" s="26">
+        <v>1</v>
+      </c>
+      <c r="V8" s="26">
+        <v>0</v>
+      </c>
+      <c r="W8" s="26">
+        <v>1</v>
+      </c>
+      <c r="X8" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
-        <v>1</v>
-      </c>
-      <c r="B8" s="27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26">
+        <v>5</v>
+      </c>
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="27">
-        <v>3</v>
-      </c>
-      <c r="F8" s="30" t="str">
+      <c r="G9" s="29">
+        <f t="shared" si="1"/>
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="H9" s="26">
+        <v>8</v>
+      </c>
+      <c r="I9" s="26">
+        <v>4</v>
+      </c>
+      <c r="J9" s="26">
+        <f t="array" ref="J9">INDEX([1]combat_sim_results!A8:'[1]combat_sim_results'!E10006, MATCH(1, ([1]combat_sim_results!C8:'[1]combat_sim_results'!C10006=H9)*([1]combat_sim_results!D8:'[1]combat_sim_results'!D10006=I9)*([1]combat_sim_results!A8:'[1]combat_sim_results'!A10006=P8)*([1]combat_sim_results!B8:'[1]combat_sim_results'!B10006=O8), 0),5)</f>
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="K9" s="26">
+        <v>13</v>
+      </c>
+      <c r="L9" s="26">
+        <v>0</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>1</v>
+      </c>
+      <c r="P9" s="26">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>5</v>
+      </c>
+      <c r="R9" s="26">
+        <v>0</v>
+      </c>
+      <c r="S9" s="26">
+        <v>0</v>
+      </c>
+      <c r="T9" s="26">
+        <v>0</v>
+      </c>
+      <c r="U9" s="26">
+        <v>1</v>
+      </c>
+      <c r="V9" s="26">
+        <v>0</v>
+      </c>
+      <c r="W9" s="26">
+        <v>0</v>
+      </c>
+      <c r="X9" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="26">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="26">
+        <v>1</v>
+      </c>
+      <c r="C10" s="26">
+        <v>5</v>
+      </c>
+      <c r="D10" s="26">
+        <v>2</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G8" s="27" t="e">
-        <f>VLOOKUP(D8,Cards!A$2:G$15,6)</f>
+      <c r="J10" s="26" t="e">
+        <f t="array" ref="J10">INDEX([1]combat_sim_results!A9:'[1]combat_sim_results'!E10007, MATCH(1, ([1]combat_sim_results!C9:'[1]combat_sim_results'!C10007=H10)*([1]combat_sim_results!D9:'[1]combat_sim_results'!D10007=I10)*([1]combat_sim_results!A9:'[1]combat_sim_results'!A10007=P9)*([1]combat_sim_results!B9:'[1]combat_sim_results'!B10007=O9), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H8" s="27" t="e">
-        <f>VLOOKUP(D8,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I8" s="27" t="e">
-        <f t="array" ref="I8">INDEX([1]combat_sim_results!A7:'[1]combat_sim_results'!E10005, MATCH(1, ([1]combat_sim_results!C7:'[1]combat_sim_results'!C10005=G8)* ([1]combat_sim_results!D7:'[1]combat_sim_results'!D10005=H8), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X8" s="27">
+      <c r="K10" s="26">
+        <v>9</v>
+      </c>
+      <c r="L10" s="26">
+        <v>3</v>
+      </c>
+      <c r="M10" s="26">
+        <v>2</v>
+      </c>
+      <c r="N10" s="26">
+        <v>0</v>
+      </c>
+      <c r="O10" s="26">
+        <v>1</v>
+      </c>
+      <c r="P10" s="26">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>5</v>
+      </c>
+      <c r="R10" s="26">
+        <v>0</v>
+      </c>
+      <c r="S10" s="26">
+        <v>0</v>
+      </c>
+      <c r="T10" s="26">
+        <v>0</v>
+      </c>
+      <c r="U10" s="26">
+        <v>1</v>
+      </c>
+      <c r="V10" s="26">
+        <v>0</v>
+      </c>
+      <c r="W10" s="26">
+        <v>0</v>
+      </c>
+      <c r="X10" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
-        <v>1</v>
-      </c>
-      <c r="B9" s="27">
-        <v>5</v>
-      </c>
-      <c r="C9" s="27">
-        <v>1</v>
-      </c>
-      <c r="F9" s="30" t="str">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B11" s="26">
+        <v>1</v>
+      </c>
+      <c r="C11" s="26">
+        <v>5</v>
+      </c>
+      <c r="D11" s="26">
+        <v>3</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G9" s="27" t="e">
-        <f>VLOOKUP(D9,Cards!A$2:G$15,6)</f>
+      <c r="J11" s="26" t="e">
+        <f t="array" ref="J11">INDEX([1]combat_sim_results!A10:'[1]combat_sim_results'!E10008, MATCH(1, ([1]combat_sim_results!C10:'[1]combat_sim_results'!C10008=H11)*([1]combat_sim_results!D10:'[1]combat_sim_results'!D10008=I11)*([1]combat_sim_results!A10:'[1]combat_sim_results'!A10008=P10)*([1]combat_sim_results!B10:'[1]combat_sim_results'!B10008=O10), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H9" s="27" t="e">
-        <f>VLOOKUP(D9,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I9" s="27" t="e">
-        <f t="array" ref="I9">INDEX([1]combat_sim_results!A8:'[1]combat_sim_results'!E10006, MATCH(1, ([1]combat_sim_results!C8:'[1]combat_sim_results'!C10006=G9)* ([1]combat_sim_results!D8:'[1]combat_sim_results'!D10006=H9), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X9" s="27">
+      <c r="K11" s="26">
+        <v>7</v>
+      </c>
+      <c r="L11" s="26">
+        <v>6</v>
+      </c>
+      <c r="M11" s="26">
+        <v>2</v>
+      </c>
+      <c r="N11" s="26">
+        <v>0</v>
+      </c>
+      <c r="O11" s="26">
+        <v>1</v>
+      </c>
+      <c r="P11" s="26">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>5</v>
+      </c>
+      <c r="R11" s="26">
+        <v>0</v>
+      </c>
+      <c r="S11" s="26">
+        <v>0</v>
+      </c>
+      <c r="T11" s="26">
+        <v>0</v>
+      </c>
+      <c r="U11" s="26">
+        <v>1</v>
+      </c>
+      <c r="V11" s="26">
+        <v>0</v>
+      </c>
+      <c r="W11" s="26">
+        <v>0</v>
+      </c>
+      <c r="X11" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
-        <v>1</v>
-      </c>
-      <c r="B10" s="27">
-        <v>5</v>
-      </c>
-      <c r="C10" s="27">
-        <v>2</v>
-      </c>
-      <c r="F10" s="30" t="str">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B12" s="26">
+        <v>1</v>
+      </c>
+      <c r="C12" s="26">
+        <v>4</v>
+      </c>
+      <c r="D12" s="26">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G10" s="27" t="e">
-        <f>VLOOKUP(D10,Cards!A$2:G$15,6)</f>
+      <c r="J12" s="26" t="e">
+        <f t="array" ref="J12">INDEX([1]combat_sim_results!A11:'[1]combat_sim_results'!E10009, MATCH(1, ([1]combat_sim_results!C11:'[1]combat_sim_results'!C10009=H12)*([1]combat_sim_results!D11:'[1]combat_sim_results'!D10009=I12)*([1]combat_sim_results!A11:'[1]combat_sim_results'!A10009=P11)*([1]combat_sim_results!B11:'[1]combat_sim_results'!B10009=O11), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H10" s="27" t="e">
-        <f>VLOOKUP(D10,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I10" s="27" t="e">
-        <f t="array" ref="I10">INDEX([1]combat_sim_results!A9:'[1]combat_sim_results'!E10007, MATCH(1, ([1]combat_sim_results!C9:'[1]combat_sim_results'!C10007=G10)* ([1]combat_sim_results!D9:'[1]combat_sim_results'!D10007=H10), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X10" s="27">
+      <c r="K12" s="26">
+        <v>9</v>
+      </c>
+      <c r="L12" s="26">
+        <v>6</v>
+      </c>
+      <c r="M12" s="26">
+        <v>0</v>
+      </c>
+      <c r="N12" s="26">
+        <v>0</v>
+      </c>
+      <c r="O12" s="26">
+        <v>1</v>
+      </c>
+      <c r="P12" s="26">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="26">
+        <v>5</v>
+      </c>
+      <c r="R12" s="26">
+        <v>0</v>
+      </c>
+      <c r="S12" s="26">
+        <v>0</v>
+      </c>
+      <c r="T12" s="26">
+        <v>0</v>
+      </c>
+      <c r="U12" s="26">
+        <v>1</v>
+      </c>
+      <c r="V12" s="26">
+        <v>0</v>
+      </c>
+      <c r="W12" s="26">
+        <v>0</v>
+      </c>
+      <c r="X12" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
-        <v>1</v>
-      </c>
-      <c r="B11" s="27">
-        <v>5</v>
-      </c>
-      <c r="C11" s="27">
-        <v>3</v>
-      </c>
-      <c r="F11" s="30" t="str">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B13" s="26">
+        <v>1</v>
+      </c>
+      <c r="C13" s="26">
+        <v>4</v>
+      </c>
+      <c r="D13" s="26">
+        <v>2</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G11" s="27" t="e">
-        <f>VLOOKUP(D11,Cards!A$2:G$15,6)</f>
+      <c r="J13" s="26" t="e">
+        <f t="array" ref="J13">INDEX([1]combat_sim_results!A12:'[1]combat_sim_results'!E10010, MATCH(1, ([1]combat_sim_results!C12:'[1]combat_sim_results'!C10010=H13)*([1]combat_sim_results!D12:'[1]combat_sim_results'!D10010=I13)*([1]combat_sim_results!A12:'[1]combat_sim_results'!A10010=P12)*([1]combat_sim_results!B12:'[1]combat_sim_results'!B10010=O12), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="27" t="e">
-        <f>VLOOKUP(D11,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I11" s="27" t="e">
-        <f t="array" ref="I11">INDEX([1]combat_sim_results!A10:'[1]combat_sim_results'!E10008, MATCH(1, ([1]combat_sim_results!C10:'[1]combat_sim_results'!C10008=G11)* ([1]combat_sim_results!D10:'[1]combat_sim_results'!D10008=H11), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X11" s="27">
+      <c r="K13" s="26">
+        <v>6</v>
+      </c>
+      <c r="L13" s="26">
+        <v>6</v>
+      </c>
+      <c r="M13" s="26">
+        <v>2</v>
+      </c>
+      <c r="N13" s="26">
+        <v>0</v>
+      </c>
+      <c r="O13" s="26">
+        <v>1</v>
+      </c>
+      <c r="P13" s="26">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>5</v>
+      </c>
+      <c r="R13" s="26">
+        <v>0</v>
+      </c>
+      <c r="S13" s="26">
+        <v>0</v>
+      </c>
+      <c r="T13" s="26">
+        <v>0</v>
+      </c>
+      <c r="U13" s="26">
+        <v>1</v>
+      </c>
+      <c r="V13" s="26">
+        <v>0</v>
+      </c>
+      <c r="W13" s="26">
+        <v>0</v>
+      </c>
+      <c r="X13" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
-        <v>1</v>
-      </c>
-      <c r="B12" s="27">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B14" s="26">
+        <v>1</v>
+      </c>
+      <c r="C14" s="26">
         <v>4</v>
       </c>
-      <c r="C12" s="27">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30" t="str">
+      <c r="D14" s="26">
+        <v>3</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G12" s="27" t="e">
-        <f>VLOOKUP(D12,Cards!A$2:G$15,6)</f>
+      <c r="J14" s="26" t="e">
+        <f t="array" ref="J14">INDEX([1]combat_sim_results!A13:'[1]combat_sim_results'!E10011, MATCH(1, ([1]combat_sim_results!C13:'[1]combat_sim_results'!C10011=H14)*([1]combat_sim_results!D13:'[1]combat_sim_results'!D10011=I14)*([1]combat_sim_results!A13:'[1]combat_sim_results'!A10011=P13)*([1]combat_sim_results!B13:'[1]combat_sim_results'!B10011=O13), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H12" s="27" t="e">
-        <f>VLOOKUP(D12,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I12" s="27" t="e">
-        <f t="array" ref="I12">INDEX([1]combat_sim_results!A11:'[1]combat_sim_results'!E10009, MATCH(1, ([1]combat_sim_results!C11:'[1]combat_sim_results'!C10009=G12)* ([1]combat_sim_results!D11:'[1]combat_sim_results'!D10009=H12), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X12" s="27">
+      <c r="K14" s="26">
+        <v>2</v>
+      </c>
+      <c r="L14" s="26">
+        <v>6</v>
+      </c>
+      <c r="M14" s="26">
+        <v>2</v>
+      </c>
+      <c r="N14" s="26">
+        <v>1</v>
+      </c>
+      <c r="O14" s="26">
+        <v>1</v>
+      </c>
+      <c r="P14" s="26">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>5</v>
+      </c>
+      <c r="R14" s="26">
+        <v>0</v>
+      </c>
+      <c r="S14" s="26">
+        <v>0</v>
+      </c>
+      <c r="T14" s="26">
+        <v>0</v>
+      </c>
+      <c r="U14" s="26">
+        <v>1</v>
+      </c>
+      <c r="V14" s="26">
+        <v>0</v>
+      </c>
+      <c r="W14" s="26">
+        <v>0</v>
+      </c>
+      <c r="X14" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
-        <v>1</v>
-      </c>
-      <c r="B13" s="27">
-        <v>4</v>
-      </c>
-      <c r="C13" s="27">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B15" s="26">
+        <v>1</v>
+      </c>
+      <c r="C15" s="26">
+        <v>3</v>
+      </c>
+      <c r="D15" s="26">
+        <v>1</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="1"/>
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H15" s="26">
+        <v>12</v>
+      </c>
+      <c r="I15" s="26">
         <v>2</v>
       </c>
-      <c r="F13" s="30" t="str">
+      <c r="J15" s="26">
+        <f t="array" ref="J15">INDEX([1]combat_sim_results!A14:'[1]combat_sim_results'!E10012, MATCH(1, ([1]combat_sim_results!C14:'[1]combat_sim_results'!C10012=H15)*([1]combat_sim_results!D14:'[1]combat_sim_results'!D10012=I15)*([1]combat_sim_results!A14:'[1]combat_sim_results'!A10012=P14)*([1]combat_sim_results!B14:'[1]combat_sim_results'!B10012=O14), 0),5)</f>
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="K15" s="26">
+        <v>9</v>
+      </c>
+      <c r="L15" s="26">
+        <v>6</v>
+      </c>
+      <c r="M15" s="26">
+        <v>3</v>
+      </c>
+      <c r="N15" s="26">
+        <v>1</v>
+      </c>
+      <c r="O15" s="26">
+        <v>1</v>
+      </c>
+      <c r="P15" s="26">
+        <v>7</v>
+      </c>
+      <c r="Q15" s="26">
+        <v>5</v>
+      </c>
+      <c r="R15" s="26">
+        <v>0</v>
+      </c>
+      <c r="S15" s="26">
+        <v>0</v>
+      </c>
+      <c r="T15" s="26">
+        <v>0</v>
+      </c>
+      <c r="U15" s="26">
+        <v>0</v>
+      </c>
+      <c r="V15" s="26">
+        <v>0</v>
+      </c>
+      <c r="W15" s="26">
+        <v>0</v>
+      </c>
+      <c r="X15" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="26">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1</v>
+      </c>
+      <c r="C16" s="26">
+        <v>3</v>
+      </c>
+      <c r="D16" s="26">
+        <v>2</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G13" s="27" t="e">
-        <f>VLOOKUP(D13,Cards!A$2:G$15,6)</f>
+      <c r="J16" s="26" t="e">
+        <f t="array" ref="J16">INDEX([1]combat_sim_results!A15:'[1]combat_sim_results'!E10013, MATCH(1, ([1]combat_sim_results!C15:'[1]combat_sim_results'!C10013=H16)*([1]combat_sim_results!D15:'[1]combat_sim_results'!D10013=I16)*([1]combat_sim_results!A15:'[1]combat_sim_results'!A10013=P15)*([1]combat_sim_results!B15:'[1]combat_sim_results'!B10013=O15), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H13" s="27" t="e">
-        <f>VLOOKUP(D13,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I13" s="27" t="e">
-        <f t="array" ref="I13">INDEX([1]combat_sim_results!A12:'[1]combat_sim_results'!E10010, MATCH(1, ([1]combat_sim_results!C12:'[1]combat_sim_results'!C10010=G13)* ([1]combat_sim_results!D12:'[1]combat_sim_results'!D10010=H13), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X13" s="27">
+      <c r="K16" s="26">
+        <v>9</v>
+      </c>
+      <c r="L16" s="26">
+        <v>5</v>
+      </c>
+      <c r="M16" s="26">
+        <v>3</v>
+      </c>
+      <c r="N16" s="26">
+        <v>0</v>
+      </c>
+      <c r="O16" s="26">
+        <v>1</v>
+      </c>
+      <c r="P16" s="26">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="26">
+        <v>5</v>
+      </c>
+      <c r="R16" s="26">
+        <v>1</v>
+      </c>
+      <c r="S16" s="26">
+        <v>0</v>
+      </c>
+      <c r="T16" s="26">
+        <v>0</v>
+      </c>
+      <c r="U16" s="26">
+        <v>0</v>
+      </c>
+      <c r="V16" s="26">
+        <v>0</v>
+      </c>
+      <c r="W16" s="26">
+        <v>0</v>
+      </c>
+      <c r="X16" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
-        <v>1</v>
-      </c>
-      <c r="B14" s="27">
+        <v>5.416666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B17" s="26">
+        <v>1</v>
+      </c>
+      <c r="C17" s="26">
+        <v>3</v>
+      </c>
+      <c r="D17" s="26">
+        <v>3</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="H17" s="26">
+        <v>11</v>
+      </c>
+      <c r="I17" s="26">
         <v>4</v>
       </c>
-      <c r="C14" s="27">
-        <v>3</v>
-      </c>
-      <c r="F14" s="30" t="str">
+      <c r="J17" s="26">
+        <f t="array" ref="J17">INDEX([1]combat_sim_results!A16:'[1]combat_sim_results'!E10014, MATCH(1, ([1]combat_sim_results!C16:'[1]combat_sim_results'!C10014=H17)*([1]combat_sim_results!D16:'[1]combat_sim_results'!D10014=I17)*([1]combat_sim_results!A16:'[1]combat_sim_results'!A10014=P16)*([1]combat_sim_results!B16:'[1]combat_sim_results'!B10014=O16), 0),5)</f>
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="K17" s="26">
+        <v>14</v>
+      </c>
+      <c r="L17" s="26">
+        <v>6</v>
+      </c>
+      <c r="M17" s="26">
+        <v>4</v>
+      </c>
+      <c r="N17" s="26">
+        <v>0</v>
+      </c>
+      <c r="O17" s="26">
+        <v>1</v>
+      </c>
+      <c r="P17" s="26">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="26">
+        <v>5</v>
+      </c>
+      <c r="R17" s="26">
+        <v>1</v>
+      </c>
+      <c r="S17" s="26">
+        <v>0</v>
+      </c>
+      <c r="T17" s="26">
+        <v>0</v>
+      </c>
+      <c r="U17" s="26">
+        <v>0</v>
+      </c>
+      <c r="V17" s="26">
+        <v>0</v>
+      </c>
+      <c r="W17" s="26">
+        <v>0</v>
+      </c>
+      <c r="X17" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="26">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="Z17" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B18" s="26">
+        <v>1</v>
+      </c>
+      <c r="C18" s="26">
+        <v>2</v>
+      </c>
+      <c r="D18" s="26">
+        <v>1</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G14" s="27" t="e">
-        <f>VLOOKUP(D14,Cards!A$2:G$15,6)</f>
+      <c r="J18" s="26" t="e">
+        <f t="array" ref="J18">INDEX([1]combat_sim_results!A17:'[1]combat_sim_results'!E10015, MATCH(1, ([1]combat_sim_results!C17:'[1]combat_sim_results'!C10015=H18)*([1]combat_sim_results!D17:'[1]combat_sim_results'!D10015=I18)*([1]combat_sim_results!A17:'[1]combat_sim_results'!A10015=P17)*([1]combat_sim_results!B17:'[1]combat_sim_results'!B10015=O17), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H14" s="27" t="e">
-        <f>VLOOKUP(D14,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I14" s="27" t="e">
-        <f t="array" ref="I14">INDEX([1]combat_sim_results!A13:'[1]combat_sim_results'!E10011, MATCH(1, ([1]combat_sim_results!C13:'[1]combat_sim_results'!C10011=G14)* ([1]combat_sim_results!D13:'[1]combat_sim_results'!D10011=H14), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X14" s="27">
+      <c r="K18" s="26">
+        <v>6</v>
+      </c>
+      <c r="L18" s="26">
+        <v>18</v>
+      </c>
+      <c r="M18" s="26">
+        <v>4</v>
+      </c>
+      <c r="N18" s="26">
+        <v>0</v>
+      </c>
+      <c r="O18" s="26">
+        <v>1</v>
+      </c>
+      <c r="P18" s="26">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>5</v>
+      </c>
+      <c r="R18" s="26">
+        <v>1</v>
+      </c>
+      <c r="S18" s="26">
+        <v>0</v>
+      </c>
+      <c r="T18" s="26">
+        <v>0</v>
+      </c>
+      <c r="U18" s="26">
+        <v>0</v>
+      </c>
+      <c r="V18" s="26">
+        <v>0</v>
+      </c>
+      <c r="W18" s="26">
+        <v>0</v>
+      </c>
+      <c r="X18" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
-        <v>1</v>
-      </c>
-      <c r="B15" s="27">
-        <v>3</v>
-      </c>
-      <c r="C15" s="27">
-        <v>1</v>
-      </c>
-      <c r="F15" s="30" t="str">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B19" s="26">
+        <v>1</v>
+      </c>
+      <c r="C19" s="26">
+        <v>2</v>
+      </c>
+      <c r="D19" s="26">
+        <v>2</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G15" s="27" t="e">
-        <f>VLOOKUP(D15,Cards!A$2:G$15,6)</f>
+      <c r="J19" s="26" t="e">
+        <f t="array" ref="J19">INDEX([1]combat_sim_results!A18:'[1]combat_sim_results'!E10016, MATCH(1, ([1]combat_sim_results!C18:'[1]combat_sim_results'!C10016=H19)*([1]combat_sim_results!D18:'[1]combat_sim_results'!D10016=I19)*([1]combat_sim_results!A18:'[1]combat_sim_results'!A10016=P18)*([1]combat_sim_results!B18:'[1]combat_sim_results'!B10016=O18), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H15" s="27" t="e">
-        <f>VLOOKUP(D15,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I15" s="27" t="e">
-        <f t="array" ref="I15">INDEX([1]combat_sim_results!A14:'[1]combat_sim_results'!E10012, MATCH(1, ([1]combat_sim_results!C14:'[1]combat_sim_results'!C10012=G15)* ([1]combat_sim_results!D14:'[1]combat_sim_results'!D10012=H15), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X15" s="27">
+      <c r="K19" s="26">
+        <v>6</v>
+      </c>
+      <c r="L19" s="26">
+        <v>12</v>
+      </c>
+      <c r="M19" s="26">
+        <v>4</v>
+      </c>
+      <c r="N19" s="26">
+        <v>0</v>
+      </c>
+      <c r="O19" s="26">
+        <v>1</v>
+      </c>
+      <c r="P19" s="26">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>5</v>
+      </c>
+      <c r="R19" s="26">
+        <v>1</v>
+      </c>
+      <c r="S19" s="26">
+        <v>0</v>
+      </c>
+      <c r="T19" s="26">
+        <v>0</v>
+      </c>
+      <c r="U19" s="26">
+        <v>0</v>
+      </c>
+      <c r="V19" s="26">
+        <v>0</v>
+      </c>
+      <c r="W19" s="26">
+        <v>0</v>
+      </c>
+      <c r="X19" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
-        <v>1</v>
-      </c>
-      <c r="B16" s="27">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B20" s="26">
+        <v>1</v>
+      </c>
+      <c r="C20" s="26">
+        <v>2</v>
+      </c>
+      <c r="D20" s="26">
         <v>3</v>
       </c>
-      <c r="C16" s="27">
-        <v>2</v>
-      </c>
-      <c r="F16" s="30" t="str">
+      <c r="E20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G16" s="27" t="e">
-        <f>VLOOKUP(D16,Cards!A$2:G$15,6)</f>
+      <c r="J20" s="26" t="e">
+        <f t="array" ref="J20">INDEX([1]combat_sim_results!A19:'[1]combat_sim_results'!E10017, MATCH(1, ([1]combat_sim_results!C19:'[1]combat_sim_results'!C10017=H20)*([1]combat_sim_results!D19:'[1]combat_sim_results'!D10017=I20)*([1]combat_sim_results!A19:'[1]combat_sim_results'!A10017=P19)*([1]combat_sim_results!B19:'[1]combat_sim_results'!B10017=O19), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H16" s="27" t="e">
-        <f>VLOOKUP(D16,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I16" s="27" t="e">
-        <f t="array" ref="I16">INDEX([1]combat_sim_results!A15:'[1]combat_sim_results'!E10013, MATCH(1, ([1]combat_sim_results!C15:'[1]combat_sim_results'!C10013=G16)* ([1]combat_sim_results!D15:'[1]combat_sim_results'!D10013=H16), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X16" s="27">
+      <c r="K20" s="26">
+        <v>6</v>
+      </c>
+      <c r="L20" s="26">
+        <v>6</v>
+      </c>
+      <c r="M20" s="26">
+        <v>4</v>
+      </c>
+      <c r="N20" s="26">
+        <v>3</v>
+      </c>
+      <c r="O20" s="26">
+        <v>1</v>
+      </c>
+      <c r="P20" s="26">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="26">
+        <v>5</v>
+      </c>
+      <c r="R20" s="26">
+        <v>1</v>
+      </c>
+      <c r="S20" s="26">
+        <v>0</v>
+      </c>
+      <c r="T20" s="26">
+        <v>0</v>
+      </c>
+      <c r="U20" s="26">
+        <v>0</v>
+      </c>
+      <c r="V20" s="26">
+        <v>0</v>
+      </c>
+      <c r="W20" s="26">
+        <v>0</v>
+      </c>
+      <c r="X20" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
-        <v>1</v>
-      </c>
-      <c r="B17" s="27">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B21" s="26">
+        <v>1</v>
+      </c>
+      <c r="C21" s="26">
+        <v>1</v>
+      </c>
+      <c r="D21" s="26">
+        <v>1</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="29">
+        <f t="shared" si="1"/>
+        <v>0.999</v>
+      </c>
+      <c r="H21" s="26">
+        <v>8</v>
+      </c>
+      <c r="I21" s="26">
+        <v>2</v>
+      </c>
+      <c r="J21" s="26">
+        <v>0.999</v>
+      </c>
+      <c r="K21" s="26">
+        <v>7</v>
+      </c>
+      <c r="L21" s="26">
+        <v>6</v>
+      </c>
+      <c r="M21" s="26">
+        <v>5</v>
+      </c>
+      <c r="N21" s="26">
         <v>3</v>
       </c>
-      <c r="C17" s="27">
-        <v>3</v>
-      </c>
-      <c r="F17" s="30" t="str">
+      <c r="O21" s="26">
+        <v>1</v>
+      </c>
+      <c r="P21" s="26">
+        <v>25</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>5</v>
+      </c>
+      <c r="R21" s="26">
+        <v>1</v>
+      </c>
+      <c r="S21" s="26">
+        <v>0</v>
+      </c>
+      <c r="T21" s="26">
+        <v>0</v>
+      </c>
+      <c r="U21" s="26">
+        <v>0</v>
+      </c>
+      <c r="V21" s="26">
+        <v>0</v>
+      </c>
+      <c r="W21" s="26">
+        <v>0</v>
+      </c>
+      <c r="X21" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="26">
+        <f t="shared" si="0"/>
+        <v>9.25</v>
+      </c>
+      <c r="Z21" s="26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B22" s="26">
+        <v>1</v>
+      </c>
+      <c r="C22" s="26">
+        <v>1</v>
+      </c>
+      <c r="D22" s="26">
+        <v>2</v>
+      </c>
+      <c r="G22" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G17" s="27" t="e">
-        <f>VLOOKUP(D17,Cards!A$2:G$15,6)</f>
+      <c r="J22" s="26" t="e">
+        <f t="array" ref="J22">INDEX([1]combat_sim_results!A21:'[1]combat_sim_results'!E10019, MATCH(1, ([1]combat_sim_results!C21:'[1]combat_sim_results'!C10019=H22)*([1]combat_sim_results!D21:'[1]combat_sim_results'!D10019=I22)*([1]combat_sim_results!A21:'[1]combat_sim_results'!A10019=P21)*([1]combat_sim_results!B21:'[1]combat_sim_results'!B10019=O21), 0),5)</f>
         <v>#N/A</v>
       </c>
-      <c r="H17" s="27" t="e">
-        <f>VLOOKUP(D17,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I17" s="27" t="e">
-        <f t="array" ref="I17">INDEX([1]combat_sim_results!A16:'[1]combat_sim_results'!E10014, MATCH(1, ([1]combat_sim_results!C16:'[1]combat_sim_results'!C10014=G17)* ([1]combat_sim_results!D16:'[1]combat_sim_results'!D10014=H17), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X17" s="27">
+      <c r="Y22" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
-        <v>1</v>
-      </c>
-      <c r="B18" s="27">
-        <v>2</v>
-      </c>
-      <c r="C18" s="27">
-        <v>1</v>
-      </c>
-      <c r="F18" s="30" t="str">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B23" s="26">
+        <v>1</v>
+      </c>
+      <c r="C23" s="26">
+        <v>1</v>
+      </c>
+      <c r="D23" s="26">
+        <v>3</v>
+      </c>
+      <c r="G23" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G18" s="27" t="e">
-        <f>VLOOKUP(D18,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H18" s="27" t="e">
-        <f>VLOOKUP(D18,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I18" s="27" t="e">
-        <f t="array" ref="I18">INDEX([1]combat_sim_results!A17:'[1]combat_sim_results'!E10015, MATCH(1, ([1]combat_sim_results!C17:'[1]combat_sim_results'!C10015=G18)* ([1]combat_sim_results!D17:'[1]combat_sim_results'!D10015=H18), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X18" s="27">
+      <c r="J23" s="26">
+        <f t="array" ref="J23">INDEX([1]combat_sim_results!A22:'[1]combat_sim_results'!E10020, MATCH(1, ([1]combat_sim_results!C22:'[1]combat_sim_results'!C10020=H23)*([1]combat_sim_results!D22:'[1]combat_sim_results'!D10020=I23)*([1]combat_sim_results!A22:'[1]combat_sim_results'!A10020=P22)*([1]combat_sim_results!B22:'[1]combat_sim_results'!B10020=O22), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
-        <v>1</v>
-      </c>
-      <c r="B19" s="27">
-        <v>2</v>
-      </c>
-      <c r="C19" s="27">
-        <v>2</v>
-      </c>
-      <c r="F19" s="30" t="str">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B24" s="26">
+        <v>1</v>
+      </c>
+      <c r="C24" s="26">
+        <v>0</v>
+      </c>
+      <c r="D24" s="26">
+        <v>1</v>
+      </c>
+      <c r="G24" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G19" s="27" t="e">
-        <f>VLOOKUP(D19,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H19" s="27" t="e">
-        <f>VLOOKUP(D19,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I19" s="27" t="e">
-        <f t="array" ref="I19">INDEX([1]combat_sim_results!A18:'[1]combat_sim_results'!E10016, MATCH(1, ([1]combat_sim_results!C18:'[1]combat_sim_results'!C10016=G19)* ([1]combat_sim_results!D18:'[1]combat_sim_results'!D10016=H19), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X19" s="27">
+      <c r="J24" s="26">
+        <f t="array" ref="J24">INDEX([1]combat_sim_results!A23:'[1]combat_sim_results'!E10021, MATCH(1, ([1]combat_sim_results!C23:'[1]combat_sim_results'!C10021=H24)*([1]combat_sim_results!D23:'[1]combat_sim_results'!D10021=I24)*([1]combat_sim_results!A23:'[1]combat_sim_results'!A10021=P23)*([1]combat_sim_results!B23:'[1]combat_sim_results'!B10021=O23), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
-        <v>1</v>
-      </c>
-      <c r="B20" s="27">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B25" s="26">
+        <v>1</v>
+      </c>
+      <c r="C25" s="26">
+        <v>0</v>
+      </c>
+      <c r="D25" s="26">
         <v>2</v>
       </c>
-      <c r="C20" s="27">
-        <v>3</v>
-      </c>
-      <c r="F20" s="30" t="str">
+      <c r="G25" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G20" s="27" t="e">
-        <f>VLOOKUP(D20,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H20" s="27" t="e">
-        <f>VLOOKUP(D20,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I20" s="27" t="e">
-        <f t="array" ref="I20">INDEX([1]combat_sim_results!A19:'[1]combat_sim_results'!E10017, MATCH(1, ([1]combat_sim_results!C19:'[1]combat_sim_results'!C10017=G20)* ([1]combat_sim_results!D19:'[1]combat_sim_results'!D10017=H20), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X20" s="27">
+      <c r="J25" s="26">
+        <f t="array" ref="J25">INDEX([1]combat_sim_results!A24:'[1]combat_sim_results'!E10022, MATCH(1, ([1]combat_sim_results!C24:'[1]combat_sim_results'!C10022=H25)*([1]combat_sim_results!D24:'[1]combat_sim_results'!D10022=I25)*([1]combat_sim_results!A24:'[1]combat_sim_results'!A10022=P24)*([1]combat_sim_results!B24:'[1]combat_sim_results'!B10022=O24), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
-        <v>1</v>
-      </c>
-      <c r="B21" s="27">
-        <v>1</v>
-      </c>
-      <c r="C21" s="27">
-        <v>1</v>
-      </c>
-      <c r="F21" s="30" t="str">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="B26" s="26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="26">
+        <v>3</v>
+      </c>
+      <c r="G26" s="29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G21" s="27" t="e">
-        <f>VLOOKUP(D21,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H21" s="27" t="e">
-        <f>VLOOKUP(D21,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I21" s="27" t="e">
-        <f t="array" ref="I21">INDEX([1]combat_sim_results!A20:'[1]combat_sim_results'!E10018, MATCH(1, ([1]combat_sim_results!C20:'[1]combat_sim_results'!C10018=G21)* ([1]combat_sim_results!D20:'[1]combat_sim_results'!D10018=H21), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X21" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
-        <v>1</v>
-      </c>
-      <c r="B22" s="27">
-        <v>1</v>
-      </c>
-      <c r="C22" s="27">
-        <v>2</v>
-      </c>
-      <c r="F22" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G22" s="27" t="e">
-        <f>VLOOKUP(D22,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H22" s="27" t="e">
-        <f>VLOOKUP(D22,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I22" s="27" t="e">
-        <f t="array" ref="I22">INDEX([1]combat_sim_results!A21:'[1]combat_sim_results'!E10019, MATCH(1, ([1]combat_sim_results!C21:'[1]combat_sim_results'!C10019=G22)* ([1]combat_sim_results!D21:'[1]combat_sim_results'!D10019=H22), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X22" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
-        <v>1</v>
-      </c>
-      <c r="B23" s="27">
-        <v>1</v>
-      </c>
-      <c r="C23" s="27">
-        <v>3</v>
-      </c>
-      <c r="F23" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G23" s="27" t="e">
-        <f>VLOOKUP(D23,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H23" s="27" t="e">
-        <f>VLOOKUP(D23,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I23" s="27" t="e">
-        <f t="array" ref="I23">INDEX([1]combat_sim_results!A22:'[1]combat_sim_results'!E10020, MATCH(1, ([1]combat_sim_results!C22:'[1]combat_sim_results'!C10020=G23)* ([1]combat_sim_results!D22:'[1]combat_sim_results'!D10020=H23), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X23" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
-        <v>1</v>
-      </c>
-      <c r="B24" s="27">
-        <v>0</v>
-      </c>
-      <c r="C24" s="27">
-        <v>1</v>
-      </c>
-      <c r="F24" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G24" s="27" t="e">
-        <f>VLOOKUP(D24,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H24" s="27" t="e">
-        <f>VLOOKUP(D24,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I24" s="27" t="e">
-        <f t="array" ref="I24">INDEX([1]combat_sim_results!A23:'[1]combat_sim_results'!E10021, MATCH(1, ([1]combat_sim_results!C23:'[1]combat_sim_results'!C10021=G24)* ([1]combat_sim_results!D23:'[1]combat_sim_results'!D10021=H24), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X24" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
-        <v>1</v>
-      </c>
-      <c r="B25" s="27">
-        <v>0</v>
-      </c>
-      <c r="C25" s="27">
-        <v>2</v>
-      </c>
-      <c r="F25" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G25" s="27" t="e">
-        <f>VLOOKUP(D25,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H25" s="27" t="e">
-        <f>VLOOKUP(D25,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I25" s="27" t="e">
-        <f t="array" ref="I25">INDEX([1]combat_sim_results!A24:'[1]combat_sim_results'!E10022, MATCH(1, ([1]combat_sim_results!C24:'[1]combat_sim_results'!C10022=G25)* ([1]combat_sim_results!D24:'[1]combat_sim_results'!D10022=H25), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X25" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
-        <v>1</v>
-      </c>
-      <c r="B26" s="27">
-        <v>0</v>
-      </c>
-      <c r="C26" s="27">
-        <v>3</v>
-      </c>
-      <c r="F26" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G26" s="27" t="e">
-        <f>VLOOKUP(D26,Cards!A$2:G$15,6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H26" s="27" t="e">
-        <f>VLOOKUP(D26,Cards!A$2:G$15,7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I26" s="27" t="e">
-        <f t="array" ref="I26">INDEX([1]combat_sim_results!A25:'[1]combat_sim_results'!E10023, MATCH(1, ([1]combat_sim_results!C25:'[1]combat_sim_results'!C10023=G26)* ([1]combat_sim_results!D25:'[1]combat_sim_results'!D10023=H26), 0),5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X26" s="27">
+      <c r="J26" s="26">
+        <f t="array" ref="J26">INDEX([1]combat_sim_results!A25:'[1]combat_sim_results'!E10023, MATCH(1, ([1]combat_sim_results!C25:'[1]combat_sim_results'!C10023=H26)*([1]combat_sim_results!D25:'[1]combat_sim_results'!D10023=I26)*([1]combat_sim_results!A25:'[1]combat_sim_results'!A10023=P25)*([1]combat_sim_results!B25:'[1]combat_sim_results'!B10023=O25), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3125,22 +4023,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F3" formula="1"/>
+    <ignoredError sqref="G3" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Cards!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D3</xm:sqref>
+          <xm:sqref>E3:E26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Playtest Options'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E26</xm:sqref>
+          <xm:sqref>F3:F26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
playtest: another round in the spreadsheet
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>Built zeppelin! Beat him pretty easily even with 1 ATK. Soooo many HP.</t>
+  </si>
+  <si>
+    <t>Took the risk because I had oil and bandages. Needed 6 extra HP to get through it.</t>
+  </si>
+  <si>
+    <t>Insta-slaughter</t>
+  </si>
+  <si>
+    <t>I messed up my records here a little bit</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -517,7 +529,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -606,10 +618,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -959,6 +974,370 @@
           </cell>
           <cell r="D25">
             <v>5</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>1</v>
+          </cell>
+          <cell r="B26">
+            <v>0</v>
+          </cell>
+          <cell r="C26">
+            <v>7</v>
+          </cell>
+          <cell r="D26">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>1</v>
+          </cell>
+          <cell r="B27">
+            <v>0</v>
+          </cell>
+          <cell r="C27">
+            <v>7</v>
+          </cell>
+          <cell r="D27">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>1</v>
+          </cell>
+          <cell r="B28">
+            <v>0</v>
+          </cell>
+          <cell r="C28">
+            <v>7</v>
+          </cell>
+          <cell r="D28">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>1</v>
+          </cell>
+          <cell r="B29">
+            <v>0</v>
+          </cell>
+          <cell r="C29">
+            <v>7</v>
+          </cell>
+          <cell r="D29">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>1</v>
+          </cell>
+          <cell r="B30">
+            <v>0</v>
+          </cell>
+          <cell r="C30">
+            <v>8</v>
+          </cell>
+          <cell r="D30">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>1</v>
+          </cell>
+          <cell r="B31">
+            <v>0</v>
+          </cell>
+          <cell r="C31">
+            <v>8</v>
+          </cell>
+          <cell r="D31">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>1</v>
+          </cell>
+          <cell r="B32">
+            <v>0</v>
+          </cell>
+          <cell r="C32">
+            <v>8</v>
+          </cell>
+          <cell r="D32">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>1</v>
+          </cell>
+          <cell r="B33">
+            <v>0</v>
+          </cell>
+          <cell r="C33">
+            <v>8</v>
+          </cell>
+          <cell r="D33">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>1</v>
+          </cell>
+          <cell r="B34">
+            <v>0</v>
+          </cell>
+          <cell r="C34">
+            <v>9</v>
+          </cell>
+          <cell r="D34">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>1</v>
+          </cell>
+          <cell r="B35">
+            <v>0</v>
+          </cell>
+          <cell r="C35">
+            <v>9</v>
+          </cell>
+          <cell r="D35">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>1</v>
+          </cell>
+          <cell r="B36">
+            <v>0</v>
+          </cell>
+          <cell r="C36">
+            <v>9</v>
+          </cell>
+          <cell r="D36">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>1</v>
+          </cell>
+          <cell r="B37">
+            <v>0</v>
+          </cell>
+          <cell r="C37">
+            <v>9</v>
+          </cell>
+          <cell r="D37">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>1</v>
+          </cell>
+          <cell r="B38">
+            <v>0</v>
+          </cell>
+          <cell r="C38">
+            <v>10</v>
+          </cell>
+          <cell r="D38">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>1</v>
+          </cell>
+          <cell r="B39">
+            <v>0</v>
+          </cell>
+          <cell r="C39">
+            <v>10</v>
+          </cell>
+          <cell r="D39">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>1</v>
+          </cell>
+          <cell r="B40">
+            <v>0</v>
+          </cell>
+          <cell r="C40">
+            <v>10</v>
+          </cell>
+          <cell r="D40">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>1</v>
+          </cell>
+          <cell r="B41">
+            <v>0</v>
+          </cell>
+          <cell r="C41">
+            <v>10</v>
+          </cell>
+          <cell r="D41">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>1</v>
+          </cell>
+          <cell r="B42">
+            <v>0</v>
+          </cell>
+          <cell r="C42">
+            <v>11</v>
+          </cell>
+          <cell r="D42">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>1</v>
+          </cell>
+          <cell r="B43">
+            <v>0</v>
+          </cell>
+          <cell r="C43">
+            <v>11</v>
+          </cell>
+          <cell r="D43">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>1</v>
+          </cell>
+          <cell r="B44">
+            <v>0</v>
+          </cell>
+          <cell r="C44">
+            <v>11</v>
+          </cell>
+          <cell r="D44">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>1</v>
+          </cell>
+          <cell r="B45">
+            <v>0</v>
+          </cell>
+          <cell r="C45">
+            <v>11</v>
+          </cell>
+          <cell r="D45">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>1</v>
+          </cell>
+          <cell r="B46">
+            <v>0</v>
+          </cell>
+          <cell r="C46">
+            <v>12</v>
+          </cell>
+          <cell r="D46">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>1</v>
+          </cell>
+          <cell r="B47">
+            <v>0</v>
+          </cell>
+          <cell r="C47">
+            <v>12</v>
+          </cell>
+          <cell r="D47">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>1</v>
+          </cell>
+          <cell r="B48">
+            <v>0</v>
+          </cell>
+          <cell r="C48">
+            <v>12</v>
+          </cell>
+          <cell r="D48">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>1</v>
+          </cell>
+          <cell r="B49">
+            <v>0</v>
+          </cell>
+          <cell r="C49">
+            <v>12</v>
+          </cell>
+          <cell r="D49">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>1</v>
+          </cell>
+          <cell r="B50">
+            <v>0</v>
+          </cell>
+          <cell r="C50">
+            <v>13</v>
+          </cell>
+          <cell r="D50">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>1</v>
+          </cell>
+          <cell r="B51">
+            <v>0</v>
+          </cell>
+          <cell r="C51">
+            <v>13</v>
+          </cell>
+          <cell r="D51">
+            <v>3</v>
           </cell>
         </row>
         <row r="10000">
@@ -2112,12 +2491,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -2275,10 +2654,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,11 +2685,11 @@
     <col min="23" max="23" width="8.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.140625" style="26" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" style="30" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>120</v>
       </c>
@@ -2386,11 +2765,11 @@
       <c r="Y1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26">
         <v>1</v>
       </c>
@@ -2444,11 +2823,11 @@
         <f>K2/4+L2/3+M2/2+N2</f>
         <v>2.5</v>
       </c>
-      <c r="Z2" s="26" t="s">
+      <c r="Z2" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>6.1</v>
       </c>
@@ -2522,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>6.1</v>
       </c>
@@ -2596,7 +2975,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>6.1</v>
       </c>
@@ -2670,7 +3049,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>6.1</v>
       </c>
@@ -2750,7 +3129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>6.1</v>
       </c>
@@ -2824,7 +3203,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
         <v>6.1</v>
       </c>
@@ -2898,7 +3277,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>6.1</v>
       </c>
@@ -2978,7 +3357,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
         <v>6.1</v>
       </c>
@@ -3052,7 +3431,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26">
         <v>6.1</v>
       </c>
@@ -3126,7 +3505,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>6.1</v>
       </c>
@@ -3200,7 +3579,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <v>6.1</v>
       </c>
@@ -3274,7 +3653,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>6.1</v>
       </c>
@@ -3348,7 +3727,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26">
         <v>6.1</v>
       </c>
@@ -3428,7 +3807,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26">
         <v>6.1</v>
       </c>
@@ -3502,7 +3881,7 @@
         <v>5.416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26">
         <v>6.1</v>
       </c>
@@ -3581,11 +3960,11 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="Z17" s="31" t="s">
+      <c r="Z17" s="30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <v>6.1</v>
       </c>
@@ -3659,7 +4038,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26">
         <v>6.1</v>
       </c>
@@ -3733,7 +4112,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26">
         <v>6.1</v>
       </c>
@@ -3807,7 +4186,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26">
         <v>6.1</v>
       </c>
@@ -3885,11 +4264,11 @@
         <f t="shared" si="0"/>
         <v>9.25</v>
       </c>
-      <c r="Z21" s="26" t="s">
+      <c r="Z21" s="30" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26">
         <v>6.1</v>
       </c>
@@ -3915,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26">
         <v>6.1</v>
       </c>
@@ -3929,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G23:G52" si="2">IF(F23="Battle",J23,"")</f>
         <v/>
       </c>
       <c r="J23" s="26">
@@ -3941,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26">
         <v>6.1</v>
       </c>
@@ -3955,7 +4334,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J24" s="26">
@@ -3967,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26">
         <v>6.1</v>
       </c>
@@ -3981,7 +4360,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J25" s="26">
@@ -3993,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26">
         <v>6.1</v>
       </c>
@@ -4007,7 +4386,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J26" s="26">
@@ -4016,6 +4395,1515 @@
       </c>
       <c r="Y26" s="26">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J27" s="26">
+        <f t="array" ref="J27">INDEX([1]combat_sim_results!A26:'[1]combat_sim_results'!E10024, MATCH(1, ([1]combat_sim_results!C26:'[1]combat_sim_results'!C10024=H27)*([1]combat_sim_results!D26:'[1]combat_sim_results'!D10024=I27)*([1]combat_sim_results!A26:'[1]combat_sim_results'!A10024=P26)*([1]combat_sim_results!B26:'[1]combat_sim_results'!B10024=O26), 0),5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="G28" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J28" s="26">
+        <f t="array" ref="J28">INDEX([1]combat_sim_results!A27:'[1]combat_sim_results'!E10025, MATCH(1, ([1]combat_sim_results!C27:'[1]combat_sim_results'!C10025=H28)*([1]combat_sim_results!D27:'[1]combat_sim_results'!D10025=I28)*([1]combat_sim_results!A27:'[1]combat_sim_results'!A10025=P27)*([1]combat_sim_results!B27:'[1]combat_sim_results'!B10025=O27), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="26">
+        <v>4</v>
+      </c>
+      <c r="L28" s="26">
+        <v>3</v>
+      </c>
+      <c r="M28" s="26">
+        <v>1</v>
+      </c>
+      <c r="N28" s="26">
+        <v>0</v>
+      </c>
+      <c r="O28" s="26">
+        <v>0</v>
+      </c>
+      <c r="P28" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="26">
+        <v>3</v>
+      </c>
+      <c r="R28" s="26">
+        <v>0</v>
+      </c>
+      <c r="S28" s="26">
+        <v>0</v>
+      </c>
+      <c r="T28" s="26">
+        <v>0</v>
+      </c>
+      <c r="U28" s="26">
+        <v>0</v>
+      </c>
+      <c r="V28" s="26">
+        <v>0</v>
+      </c>
+      <c r="W28" s="26">
+        <v>0</v>
+      </c>
+      <c r="X28" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="26">
+        <f>K28/4+L28/3+M28/2+N28</f>
+        <v>2.5</v>
+      </c>
+      <c r="Z28" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C29" s="26">
+        <v>7</v>
+      </c>
+      <c r="D29" s="26">
+        <v>1</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J29" s="26" t="e">
+        <f t="array" ref="J29">INDEX([1]combat_sim_results!A28:'[1]combat_sim_results'!E10026, MATCH(1, ([1]combat_sim_results!C28:'[1]combat_sim_results'!C10026=H29)*([1]combat_sim_results!D28:'[1]combat_sim_results'!D10026=I29)*([1]combat_sim_results!A28:'[1]combat_sim_results'!A10026=P28)*([1]combat_sim_results!B28:'[1]combat_sim_results'!B10026=O28), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K29" s="26">
+        <v>0</v>
+      </c>
+      <c r="L29" s="26">
+        <v>3</v>
+      </c>
+      <c r="M29" s="26">
+        <v>1</v>
+      </c>
+      <c r="N29" s="26">
+        <v>1</v>
+      </c>
+      <c r="O29" s="26">
+        <v>0</v>
+      </c>
+      <c r="P29" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="26">
+        <v>3</v>
+      </c>
+      <c r="R29" s="26">
+        <v>0</v>
+      </c>
+      <c r="S29" s="26">
+        <v>0</v>
+      </c>
+      <c r="T29" s="26">
+        <v>0</v>
+      </c>
+      <c r="U29" s="26">
+        <v>0</v>
+      </c>
+      <c r="V29" s="26">
+        <v>0</v>
+      </c>
+      <c r="W29" s="26">
+        <v>0</v>
+      </c>
+      <c r="X29" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="26">
+        <f t="shared" ref="Y29:Y52" si="3">K29/4+L29/3+M29/2+N29</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C30" s="26">
+        <v>7</v>
+      </c>
+      <c r="D30" s="26">
+        <v>2</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J30" s="26" t="e">
+        <f t="array" ref="J30">INDEX([1]combat_sim_results!A29:'[1]combat_sim_results'!E10027, MATCH(1, ([1]combat_sim_results!C29:'[1]combat_sim_results'!C10027=H30)*([1]combat_sim_results!D29:'[1]combat_sim_results'!D10027=I30)*([1]combat_sim_results!A29:'[1]combat_sim_results'!A10027=P29)*([1]combat_sim_results!B29:'[1]combat_sim_results'!B10027=O29), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K30" s="26">
+        <v>3</v>
+      </c>
+      <c r="L30" s="26">
+        <v>3</v>
+      </c>
+      <c r="M30" s="26">
+        <v>0</v>
+      </c>
+      <c r="N30" s="26">
+        <v>1</v>
+      </c>
+      <c r="O30" s="26">
+        <v>0</v>
+      </c>
+      <c r="P30" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="26">
+        <v>3</v>
+      </c>
+      <c r="R30" s="26">
+        <v>0</v>
+      </c>
+      <c r="S30" s="26">
+        <v>0</v>
+      </c>
+      <c r="T30" s="26">
+        <v>0</v>
+      </c>
+      <c r="U30" s="26">
+        <v>0</v>
+      </c>
+      <c r="V30" s="26">
+        <v>0</v>
+      </c>
+      <c r="W30" s="26">
+        <v>0</v>
+      </c>
+      <c r="X30" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="26">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C31" s="26">
+        <v>7</v>
+      </c>
+      <c r="D31" s="26">
+        <v>3</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J31" s="26" t="e">
+        <f t="array" ref="J31">INDEX([1]combat_sim_results!A30:'[1]combat_sim_results'!E10028, MATCH(1, ([1]combat_sim_results!C30:'[1]combat_sim_results'!C10028=H31)*([1]combat_sim_results!D30:'[1]combat_sim_results'!D10028=I31)*([1]combat_sim_results!A30:'[1]combat_sim_results'!A10028=P30)*([1]combat_sim_results!B30:'[1]combat_sim_results'!B10028=O30), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K31" s="26">
+        <v>3</v>
+      </c>
+      <c r="L31" s="26">
+        <v>0</v>
+      </c>
+      <c r="M31" s="26">
+        <v>0</v>
+      </c>
+      <c r="N31" s="26">
+        <v>1</v>
+      </c>
+      <c r="O31" s="26">
+        <v>0</v>
+      </c>
+      <c r="P31" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="26">
+        <v>3</v>
+      </c>
+      <c r="R31" s="26">
+        <v>0</v>
+      </c>
+      <c r="S31" s="26">
+        <v>0</v>
+      </c>
+      <c r="T31" s="26">
+        <v>0</v>
+      </c>
+      <c r="U31" s="26">
+        <v>0</v>
+      </c>
+      <c r="V31" s="26">
+        <v>0</v>
+      </c>
+      <c r="W31" s="26">
+        <v>1</v>
+      </c>
+      <c r="X31" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="26">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C32" s="26">
+        <v>6</v>
+      </c>
+      <c r="D32" s="26">
+        <v>1</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J32" s="26" t="e">
+        <f t="array" ref="J32">INDEX([1]combat_sim_results!A31:'[1]combat_sim_results'!E10029, MATCH(1, ([1]combat_sim_results!C31:'[1]combat_sim_results'!C10029=H32)*([1]combat_sim_results!D31:'[1]combat_sim_results'!D10029=I32)*([1]combat_sim_results!A31:'[1]combat_sim_results'!A10029=P31)*([1]combat_sim_results!B31:'[1]combat_sim_results'!B10029=O31), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K32" s="26">
+        <v>1</v>
+      </c>
+      <c r="L32" s="26">
+        <v>3</v>
+      </c>
+      <c r="M32" s="26">
+        <v>0</v>
+      </c>
+      <c r="N32" s="26">
+        <v>1</v>
+      </c>
+      <c r="O32" s="26">
+        <v>0</v>
+      </c>
+      <c r="P32" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="26">
+        <v>4</v>
+      </c>
+      <c r="R32" s="26">
+        <v>0</v>
+      </c>
+      <c r="S32" s="26">
+        <v>0</v>
+      </c>
+      <c r="T32" s="26">
+        <v>0</v>
+      </c>
+      <c r="U32" s="26">
+        <v>0</v>
+      </c>
+      <c r="V32" s="26">
+        <v>0</v>
+      </c>
+      <c r="W32" s="26">
+        <v>0</v>
+      </c>
+      <c r="X32" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="26">
+        <f t="shared" si="3"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C33" s="26">
+        <v>6</v>
+      </c>
+      <c r="D33" s="26">
+        <v>2</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J33" s="26" t="e">
+        <f t="array" ref="J33">INDEX([1]combat_sim_results!A32:'[1]combat_sim_results'!E10030, MATCH(1, ([1]combat_sim_results!C32:'[1]combat_sim_results'!C10030=H33)*([1]combat_sim_results!D32:'[1]combat_sim_results'!D10030=I33)*([1]combat_sim_results!A32:'[1]combat_sim_results'!A10030=P32)*([1]combat_sim_results!B32:'[1]combat_sim_results'!B10030=O32), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K33" s="26">
+        <v>1</v>
+      </c>
+      <c r="L33" s="26">
+        <v>2</v>
+      </c>
+      <c r="M33" s="26">
+        <v>0</v>
+      </c>
+      <c r="N33" s="26">
+        <v>0</v>
+      </c>
+      <c r="O33" s="26">
+        <v>0</v>
+      </c>
+      <c r="P33" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q33" s="26">
+        <v>4</v>
+      </c>
+      <c r="R33" s="26">
+        <v>1</v>
+      </c>
+      <c r="S33" s="26">
+        <v>0</v>
+      </c>
+      <c r="T33" s="26">
+        <v>0</v>
+      </c>
+      <c r="U33" s="26">
+        <v>0</v>
+      </c>
+      <c r="V33" s="26">
+        <v>0</v>
+      </c>
+      <c r="W33" s="26">
+        <v>0</v>
+      </c>
+      <c r="X33" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="26">
+        <f t="shared" si="3"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C34" s="26">
+        <v>6</v>
+      </c>
+      <c r="D34" s="26">
+        <v>3</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H34" s="26">
+        <v>8</v>
+      </c>
+      <c r="I34" s="26">
+        <v>2</v>
+      </c>
+      <c r="J34" s="26">
+        <f t="array" ref="J34">INDEX([1]combat_sim_results!A33:'[1]combat_sim_results'!E10031, MATCH(1, ([1]combat_sim_results!C33:'[1]combat_sim_results'!C10031=H34)*([1]combat_sim_results!D33:'[1]combat_sim_results'!D10031=I34)*([1]combat_sim_results!A33:'[1]combat_sim_results'!A10031=P33)*([1]combat_sim_results!B33:'[1]combat_sim_results'!B10031=O33), 0),5)</f>
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="K34" s="26">
+        <v>3</v>
+      </c>
+      <c r="L34" s="26">
+        <v>2</v>
+      </c>
+      <c r="M34" s="26">
+        <v>3</v>
+      </c>
+      <c r="N34" s="26">
+        <v>0</v>
+      </c>
+      <c r="O34" s="26">
+        <v>0</v>
+      </c>
+      <c r="P34" s="26">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="26">
+        <v>4</v>
+      </c>
+      <c r="R34" s="26">
+        <v>1</v>
+      </c>
+      <c r="S34" s="26">
+        <v>0</v>
+      </c>
+      <c r="T34" s="26">
+        <v>0</v>
+      </c>
+      <c r="U34" s="26">
+        <v>0</v>
+      </c>
+      <c r="V34" s="26">
+        <v>0</v>
+      </c>
+      <c r="W34" s="26">
+        <v>0</v>
+      </c>
+      <c r="X34" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="26">
+        <f t="shared" si="3"/>
+        <v>2.9166666666666665</v>
+      </c>
+    </row>
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C35" s="26">
+        <v>5</v>
+      </c>
+      <c r="D35" s="26">
+        <v>1</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J35" s="26" t="e">
+        <f t="array" ref="J35">INDEX([1]combat_sim_results!A34:'[1]combat_sim_results'!E10032, MATCH(1, ([1]combat_sim_results!C34:'[1]combat_sim_results'!C10032=H35)*([1]combat_sim_results!D34:'[1]combat_sim_results'!D10032=I35)*([1]combat_sim_results!A34:'[1]combat_sim_results'!A10032=P34)*([1]combat_sim_results!B34:'[1]combat_sim_results'!B10032=O34), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K35" s="26">
+        <v>1</v>
+      </c>
+      <c r="L35" s="26">
+        <v>5</v>
+      </c>
+      <c r="M35" s="26">
+        <v>3</v>
+      </c>
+      <c r="N35" s="26">
+        <v>0</v>
+      </c>
+      <c r="O35" s="26">
+        <v>0</v>
+      </c>
+      <c r="P35" s="26">
+        <v>8</v>
+      </c>
+      <c r="Q35" s="26">
+        <v>4</v>
+      </c>
+      <c r="R35" s="26">
+        <v>1</v>
+      </c>
+      <c r="S35" s="26">
+        <v>0</v>
+      </c>
+      <c r="T35" s="26">
+        <v>0</v>
+      </c>
+      <c r="U35" s="26">
+        <v>0</v>
+      </c>
+      <c r="V35" s="26">
+        <v>0</v>
+      </c>
+      <c r="W35" s="26">
+        <v>0</v>
+      </c>
+      <c r="X35" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="26">
+        <f t="shared" si="3"/>
+        <v>3.416666666666667</v>
+      </c>
+    </row>
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C36" s="26">
+        <v>5</v>
+      </c>
+      <c r="D36" s="26">
+        <v>2</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="29">
+        <f t="shared" si="2"/>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="H36" s="26">
+        <v>10</v>
+      </c>
+      <c r="I36" s="26">
+        <v>3</v>
+      </c>
+      <c r="J36" s="26">
+        <f t="array" ref="J36">INDEX([1]combat_sim_results!A35:'[1]combat_sim_results'!E10033, MATCH(1, ([1]combat_sim_results!C35:'[1]combat_sim_results'!C10033=H36)*([1]combat_sim_results!D35:'[1]combat_sim_results'!D10033=I36)*([1]combat_sim_results!A35:'[1]combat_sim_results'!A10033=P35)*([1]combat_sim_results!B35:'[1]combat_sim_results'!B10033=O35), 0),5)</f>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="K36" s="26">
+        <v>5</v>
+      </c>
+      <c r="L36" s="26">
+        <v>9</v>
+      </c>
+      <c r="M36" s="26">
+        <v>3</v>
+      </c>
+      <c r="N36" s="26">
+        <v>0</v>
+      </c>
+      <c r="O36" s="26">
+        <v>0</v>
+      </c>
+      <c r="P36" s="26">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="26">
+        <v>5</v>
+      </c>
+      <c r="R36" s="26">
+        <v>1</v>
+      </c>
+      <c r="S36" s="26">
+        <v>0</v>
+      </c>
+      <c r="T36" s="26">
+        <v>0</v>
+      </c>
+      <c r="U36" s="26">
+        <v>0</v>
+      </c>
+      <c r="V36" s="26">
+        <v>0</v>
+      </c>
+      <c r="W36" s="26">
+        <v>0</v>
+      </c>
+      <c r="X36" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="26">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+      <c r="Z36" s="30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C37" s="26">
+        <v>5</v>
+      </c>
+      <c r="D37" s="26">
+        <v>3</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J37" s="26" t="e">
+        <f t="array" ref="J37">INDEX([1]combat_sim_results!A36:'[1]combat_sim_results'!E10034, MATCH(1, ([1]combat_sim_results!C36:'[1]combat_sim_results'!C10034=H37)*([1]combat_sim_results!D36:'[1]combat_sim_results'!D10034=I37)*([1]combat_sim_results!A36:'[1]combat_sim_results'!A10034=P36)*([1]combat_sim_results!B36:'[1]combat_sim_results'!B10034=O36), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K37" s="26">
+        <v>3</v>
+      </c>
+      <c r="L37" s="26">
+        <v>9</v>
+      </c>
+      <c r="M37" s="26">
+        <v>3</v>
+      </c>
+      <c r="N37" s="26">
+        <v>0</v>
+      </c>
+      <c r="O37" s="26">
+        <v>0</v>
+      </c>
+      <c r="P37" s="26">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="26">
+        <v>5</v>
+      </c>
+      <c r="R37" s="26">
+        <v>1</v>
+      </c>
+      <c r="S37" s="26">
+        <v>0</v>
+      </c>
+      <c r="T37" s="26">
+        <v>0</v>
+      </c>
+      <c r="U37" s="26">
+        <v>1</v>
+      </c>
+      <c r="V37" s="26">
+        <v>0</v>
+      </c>
+      <c r="W37" s="26">
+        <v>0</v>
+      </c>
+      <c r="X37" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="26">
+        <f t="shared" si="3"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C38" s="26">
+        <v>4</v>
+      </c>
+      <c r="D38" s="26">
+        <v>1</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J38" s="26" t="e">
+        <f t="array" ref="J38">INDEX([1]combat_sim_results!A37:'[1]combat_sim_results'!E10035, MATCH(1, ([1]combat_sim_results!C37:'[1]combat_sim_results'!C10035=H38)*([1]combat_sim_results!D37:'[1]combat_sim_results'!D10035=I38)*([1]combat_sim_results!A37:'[1]combat_sim_results'!A10035=P37)*([1]combat_sim_results!B37:'[1]combat_sim_results'!B10035=O37), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K38" s="26">
+        <v>5</v>
+      </c>
+      <c r="L38" s="26">
+        <v>5</v>
+      </c>
+      <c r="M38" s="26">
+        <v>3</v>
+      </c>
+      <c r="N38" s="26">
+        <v>0</v>
+      </c>
+      <c r="O38" s="26">
+        <v>0</v>
+      </c>
+      <c r="P38" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q38" s="26">
+        <v>5</v>
+      </c>
+      <c r="R38" s="26">
+        <v>1</v>
+      </c>
+      <c r="S38" s="26">
+        <v>0</v>
+      </c>
+      <c r="T38" s="26">
+        <v>0</v>
+      </c>
+      <c r="U38" s="26">
+        <v>1</v>
+      </c>
+      <c r="V38" s="26">
+        <v>0</v>
+      </c>
+      <c r="W38" s="26">
+        <v>0</v>
+      </c>
+      <c r="X38" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="26">
+        <f t="shared" si="3"/>
+        <v>4.416666666666667</v>
+      </c>
+    </row>
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C39" s="26">
+        <v>4</v>
+      </c>
+      <c r="D39" s="26">
+        <v>2</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J39" s="26" t="e">
+        <f t="array" ref="J39">INDEX([1]combat_sim_results!A38:'[1]combat_sim_results'!E10036, MATCH(1, ([1]combat_sim_results!C38:'[1]combat_sim_results'!C10036=H39)*([1]combat_sim_results!D38:'[1]combat_sim_results'!D10036=I39)*([1]combat_sim_results!A38:'[1]combat_sim_results'!A10036=P38)*([1]combat_sim_results!B38:'[1]combat_sim_results'!B10036=O38), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K39" s="26">
+        <v>5</v>
+      </c>
+      <c r="L39" s="26">
+        <v>2</v>
+      </c>
+      <c r="M39" s="26">
+        <v>3</v>
+      </c>
+      <c r="N39" s="26">
+        <v>0</v>
+      </c>
+      <c r="O39" s="26">
+        <v>0</v>
+      </c>
+      <c r="P39" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q39" s="26">
+        <v>6</v>
+      </c>
+      <c r="R39" s="26">
+        <v>1</v>
+      </c>
+      <c r="S39" s="26">
+        <v>0</v>
+      </c>
+      <c r="T39" s="26">
+        <v>0</v>
+      </c>
+      <c r="U39" s="26">
+        <v>1</v>
+      </c>
+      <c r="V39" s="26">
+        <v>0</v>
+      </c>
+      <c r="W39" s="26">
+        <v>0</v>
+      </c>
+      <c r="X39" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="26">
+        <f t="shared" si="3"/>
+        <v>3.4166666666666665</v>
+      </c>
+    </row>
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C40" s="26">
+        <v>4</v>
+      </c>
+      <c r="D40" s="26">
+        <v>3</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J40" s="26" t="e">
+        <f t="array" ref="J40">INDEX([1]combat_sim_results!A39:'[1]combat_sim_results'!E10037, MATCH(1, ([1]combat_sim_results!C39:'[1]combat_sim_results'!C10037=H40)*([1]combat_sim_results!D39:'[1]combat_sim_results'!D10037=I40)*([1]combat_sim_results!A39:'[1]combat_sim_results'!A10037=P39)*([1]combat_sim_results!B39:'[1]combat_sim_results'!B10037=O39), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K40" s="26">
+        <v>1</v>
+      </c>
+      <c r="L40" s="26">
+        <v>2</v>
+      </c>
+      <c r="M40" s="26">
+        <v>3</v>
+      </c>
+      <c r="N40" s="26">
+        <v>0</v>
+      </c>
+      <c r="O40" s="26">
+        <v>1</v>
+      </c>
+      <c r="P40" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q40" s="26">
+        <v>6</v>
+      </c>
+      <c r="R40" s="26">
+        <v>1</v>
+      </c>
+      <c r="S40" s="26">
+        <v>0</v>
+      </c>
+      <c r="T40" s="26">
+        <v>0</v>
+      </c>
+      <c r="U40" s="26">
+        <v>1</v>
+      </c>
+      <c r="V40" s="26">
+        <v>0</v>
+      </c>
+      <c r="W40" s="26">
+        <v>0</v>
+      </c>
+      <c r="X40" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="26">
+        <f t="shared" si="3"/>
+        <v>2.4166666666666665</v>
+      </c>
+    </row>
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C41" s="26">
+        <v>3</v>
+      </c>
+      <c r="D41" s="26">
+        <v>1</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J41" s="26" t="e">
+        <f t="array" ref="J41">INDEX([1]combat_sim_results!A40:'[1]combat_sim_results'!E10038, MATCH(1, ([1]combat_sim_results!C40:'[1]combat_sim_results'!C10038=H41)*([1]combat_sim_results!D40:'[1]combat_sim_results'!D10038=I41)*([1]combat_sim_results!A40:'[1]combat_sim_results'!A10038=P40)*([1]combat_sim_results!B40:'[1]combat_sim_results'!B10038=O40), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K41" s="26">
+        <v>1</v>
+      </c>
+      <c r="L41" s="26">
+        <v>2</v>
+      </c>
+      <c r="M41" s="26">
+        <v>3</v>
+      </c>
+      <c r="N41" s="26">
+        <v>0</v>
+      </c>
+      <c r="O41" s="26">
+        <v>1</v>
+      </c>
+      <c r="P41" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q41" s="26">
+        <v>6</v>
+      </c>
+      <c r="R41" s="26">
+        <v>1</v>
+      </c>
+      <c r="S41" s="26">
+        <v>0</v>
+      </c>
+      <c r="T41" s="26">
+        <v>0</v>
+      </c>
+      <c r="U41" s="26">
+        <v>1</v>
+      </c>
+      <c r="V41" s="26">
+        <v>0</v>
+      </c>
+      <c r="W41" s="26">
+        <v>0</v>
+      </c>
+      <c r="X41" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="26">
+        <f t="shared" si="3"/>
+        <v>2.4166666666666665</v>
+      </c>
+    </row>
+    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C42" s="26">
+        <v>3</v>
+      </c>
+      <c r="D42" s="26">
+        <v>2</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="29">
+        <f t="shared" si="2"/>
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="H42" s="26">
+        <v>8</v>
+      </c>
+      <c r="I42" s="26">
+        <v>4</v>
+      </c>
+      <c r="J42" s="26">
+        <f t="array" ref="J42">INDEX([1]combat_sim_results!A41:'[1]combat_sim_results'!E10039, MATCH(1, ([1]combat_sim_results!C41:'[1]combat_sim_results'!C10039=H42)*([1]combat_sim_results!D41:'[1]combat_sim_results'!D10039=I42)*([1]combat_sim_results!A41:'[1]combat_sim_results'!A10039=P41)*([1]combat_sim_results!B41:'[1]combat_sim_results'!B10039=O41), 0),5)</f>
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="K42" s="26">
+        <v>6</v>
+      </c>
+      <c r="L42" s="26">
+        <v>2</v>
+      </c>
+      <c r="M42" s="26">
+        <v>5</v>
+      </c>
+      <c r="N42" s="26">
+        <v>0</v>
+      </c>
+      <c r="O42" s="26">
+        <v>2</v>
+      </c>
+      <c r="P42" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q42" s="26">
+        <v>6</v>
+      </c>
+      <c r="R42" s="26">
+        <v>1</v>
+      </c>
+      <c r="S42" s="26">
+        <v>0</v>
+      </c>
+      <c r="T42" s="26">
+        <v>0</v>
+      </c>
+      <c r="U42" s="26">
+        <v>1</v>
+      </c>
+      <c r="V42" s="26">
+        <v>0</v>
+      </c>
+      <c r="W42" s="26">
+        <v>0</v>
+      </c>
+      <c r="X42" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="26">
+        <f t="shared" si="3"/>
+        <v>4.6666666666666661</v>
+      </c>
+      <c r="Z42" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C43" s="26">
+        <v>3</v>
+      </c>
+      <c r="D43" s="26">
+        <v>3</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J43" s="26" t="e">
+        <f t="array" ref="J43">INDEX([1]combat_sim_results!A42:'[1]combat_sim_results'!E10040, MATCH(1, ([1]combat_sim_results!C42:'[1]combat_sim_results'!C10040=H43)*([1]combat_sim_results!D42:'[1]combat_sim_results'!D10040=I43)*([1]combat_sim_results!A42:'[1]combat_sim_results'!A10040=P42)*([1]combat_sim_results!B42:'[1]combat_sim_results'!B10040=O42), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K43" s="26">
+        <v>6</v>
+      </c>
+      <c r="L43" s="26">
+        <v>5</v>
+      </c>
+      <c r="M43" s="26">
+        <v>5</v>
+      </c>
+      <c r="N43" s="26">
+        <v>0</v>
+      </c>
+      <c r="O43" s="26">
+        <v>2</v>
+      </c>
+      <c r="P43" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q43" s="26">
+        <v>6</v>
+      </c>
+      <c r="R43" s="26">
+        <v>1</v>
+      </c>
+      <c r="S43" s="26">
+        <v>0</v>
+      </c>
+      <c r="T43" s="26">
+        <v>0</v>
+      </c>
+      <c r="U43" s="26">
+        <v>1</v>
+      </c>
+      <c r="V43" s="26">
+        <v>0</v>
+      </c>
+      <c r="W43" s="26">
+        <v>0</v>
+      </c>
+      <c r="X43" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="26">
+        <f t="shared" si="3"/>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C44" s="26">
+        <v>2</v>
+      </c>
+      <c r="D44" s="26">
+        <v>1</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J44" s="26" t="e">
+        <f t="array" ref="J44">INDEX([1]combat_sim_results!A43:'[1]combat_sim_results'!E10041, MATCH(1, ([1]combat_sim_results!C43:'[1]combat_sim_results'!C10041=H44)*([1]combat_sim_results!D43:'[1]combat_sim_results'!D10041=I44)*([1]combat_sim_results!A43:'[1]combat_sim_results'!A10041=P43)*([1]combat_sim_results!B43:'[1]combat_sim_results'!B10041=O43), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K44" s="26">
+        <v>6</v>
+      </c>
+      <c r="L44" s="26">
+        <v>5</v>
+      </c>
+      <c r="M44" s="26">
+        <v>5</v>
+      </c>
+      <c r="N44" s="26">
+        <v>2</v>
+      </c>
+      <c r="O44" s="26">
+        <v>2</v>
+      </c>
+      <c r="P44" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q44" s="26">
+        <v>6</v>
+      </c>
+      <c r="R44" s="26">
+        <v>1</v>
+      </c>
+      <c r="S44" s="26">
+        <v>0</v>
+      </c>
+      <c r="T44" s="26">
+        <v>0</v>
+      </c>
+      <c r="U44" s="26">
+        <v>0</v>
+      </c>
+      <c r="V44" s="26">
+        <v>0</v>
+      </c>
+      <c r="W44" s="26">
+        <v>0</v>
+      </c>
+      <c r="X44" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="26">
+        <f t="shared" si="3"/>
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C45" s="26">
+        <v>2</v>
+      </c>
+      <c r="D45" s="26">
+        <v>2</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J45" s="26" t="e">
+        <f t="array" ref="J45">INDEX([1]combat_sim_results!A44:'[1]combat_sim_results'!E10042, MATCH(1, ([1]combat_sim_results!C44:'[1]combat_sim_results'!C10042=H45)*([1]combat_sim_results!D44:'[1]combat_sim_results'!D10042=I45)*([1]combat_sim_results!A44:'[1]combat_sim_results'!A10042=P44)*([1]combat_sim_results!B44:'[1]combat_sim_results'!B10042=O44), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K45" s="26">
+        <v>6</v>
+      </c>
+      <c r="L45" s="26">
+        <v>5</v>
+      </c>
+      <c r="M45" s="26">
+        <v>5</v>
+      </c>
+      <c r="N45" s="26">
+        <v>2</v>
+      </c>
+      <c r="O45" s="26">
+        <v>2</v>
+      </c>
+      <c r="P45" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q45" s="26">
+        <v>6</v>
+      </c>
+      <c r="R45" s="26">
+        <v>1</v>
+      </c>
+      <c r="S45" s="26">
+        <v>0</v>
+      </c>
+      <c r="T45" s="26">
+        <v>0</v>
+      </c>
+      <c r="U45" s="26">
+        <v>0</v>
+      </c>
+      <c r="V45" s="26">
+        <v>0</v>
+      </c>
+      <c r="W45" s="26">
+        <v>0</v>
+      </c>
+      <c r="X45" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="26">
+        <f t="shared" si="3"/>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="Z45" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C46" s="26">
+        <v>2</v>
+      </c>
+      <c r="D46" s="26">
+        <v>3</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J46" s="26" t="e">
+        <f t="array" ref="J46">INDEX([1]combat_sim_results!A45:'[1]combat_sim_results'!E10043, MATCH(1, ([1]combat_sim_results!C45:'[1]combat_sim_results'!C10043=H46)*([1]combat_sim_results!D45:'[1]combat_sim_results'!D10043=I46)*([1]combat_sim_results!A45:'[1]combat_sim_results'!A10043=P45)*([1]combat_sim_results!B45:'[1]combat_sim_results'!B10043=O45), 0),5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K46" s="26">
+        <v>6</v>
+      </c>
+      <c r="L46" s="26">
+        <v>1</v>
+      </c>
+      <c r="M46" s="26">
+        <v>5</v>
+      </c>
+      <c r="N46" s="26">
+        <v>4</v>
+      </c>
+      <c r="O46" s="26">
+        <v>2</v>
+      </c>
+      <c r="P46" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q46" s="26">
+        <v>6</v>
+      </c>
+      <c r="R46" s="26">
+        <v>1</v>
+      </c>
+      <c r="S46" s="26">
+        <v>0</v>
+      </c>
+      <c r="T46" s="26">
+        <v>0</v>
+      </c>
+      <c r="U46" s="26">
+        <v>0</v>
+      </c>
+      <c r="V46" s="26">
+        <v>0</v>
+      </c>
+      <c r="W46" s="26">
+        <v>0</v>
+      </c>
+      <c r="X46" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="26">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333321</v>
+      </c>
+    </row>
+    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C47" s="26">
+        <v>1</v>
+      </c>
+      <c r="D47" s="26">
+        <v>1</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="29">
+        <f t="shared" si="2"/>
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="H47" s="26">
+        <v>11</v>
+      </c>
+      <c r="I47" s="26">
+        <v>4</v>
+      </c>
+      <c r="J47" s="26">
+        <f t="array" ref="J47">INDEX([1]combat_sim_results!A46:'[1]combat_sim_results'!E10044, MATCH(1, ([1]combat_sim_results!C46:'[1]combat_sim_results'!C10044=H47)*([1]combat_sim_results!D46:'[1]combat_sim_results'!D10044=I47)*([1]combat_sim_results!A46:'[1]combat_sim_results'!A10044=P46)*([1]combat_sim_results!B46:'[1]combat_sim_results'!B10044=O46), 0),5)</f>
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="K47" s="26">
+        <v>7</v>
+      </c>
+      <c r="L47" s="26">
+        <v>2</v>
+      </c>
+      <c r="M47" s="26">
+        <v>5</v>
+      </c>
+      <c r="N47" s="26">
+        <v>4</v>
+      </c>
+      <c r="O47" s="26">
+        <v>3</v>
+      </c>
+      <c r="P47" s="26">
+        <v>15</v>
+      </c>
+      <c r="Q47" s="26">
+        <v>6</v>
+      </c>
+      <c r="R47" s="26">
+        <v>1</v>
+      </c>
+      <c r="S47" s="26">
+        <v>0</v>
+      </c>
+      <c r="T47" s="26">
+        <v>0</v>
+      </c>
+      <c r="U47" s="26">
+        <v>0</v>
+      </c>
+      <c r="V47" s="26">
+        <v>0</v>
+      </c>
+      <c r="W47" s="26">
+        <v>0</v>
+      </c>
+      <c r="X47" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="26">
+        <f t="shared" si="3"/>
+        <v>8.9166666666666661</v>
+      </c>
+      <c r="Z47" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C48" s="26">
+        <v>1</v>
+      </c>
+      <c r="D48" s="26">
+        <v>2</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="29">
+        <f t="shared" si="2"/>
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H48" s="26">
+        <v>15</v>
+      </c>
+      <c r="I48" s="26">
+        <v>4</v>
+      </c>
+      <c r="J48" s="26">
+        <f t="array" ref="J48">INDEX([1]combat_sim_results!A47:'[1]combat_sim_results'!E10045, MATCH(1, ([1]combat_sim_results!C47:'[1]combat_sim_results'!C10045=H48)*([1]combat_sim_results!D47:'[1]combat_sim_results'!D10045=I48)*([1]combat_sim_results!A47:'[1]combat_sim_results'!A10045=P47)*([1]combat_sim_results!B47:'[1]combat_sim_results'!B10045=O47), 0),5)</f>
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="Y48" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z48" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C49" s="26">
+        <v>1</v>
+      </c>
+      <c r="D49" s="26">
+        <v>3</v>
+      </c>
+      <c r="G49" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J49" s="26">
+        <f t="array" ref="J49">INDEX([1]combat_sim_results!A48:'[1]combat_sim_results'!E10046, MATCH(1, ([1]combat_sim_results!C48:'[1]combat_sim_results'!C10046=H49)*([1]combat_sim_results!D48:'[1]combat_sim_results'!D10046=I49)*([1]combat_sim_results!A48:'[1]combat_sim_results'!A10046=P48)*([1]combat_sim_results!B48:'[1]combat_sim_results'!B10046=O48), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y49" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C50" s="26">
+        <v>0</v>
+      </c>
+      <c r="D50" s="26">
+        <v>1</v>
+      </c>
+      <c r="G50" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J50" s="26">
+        <f t="array" ref="J50">INDEX([1]combat_sim_results!A49:'[1]combat_sim_results'!E10047, MATCH(1, ([1]combat_sim_results!C49:'[1]combat_sim_results'!C10047=H50)*([1]combat_sim_results!D49:'[1]combat_sim_results'!D10047=I50)*([1]combat_sim_results!A49:'[1]combat_sim_results'!A10047=P49)*([1]combat_sim_results!B49:'[1]combat_sim_results'!B10047=O49), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y50" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C51" s="26">
+        <v>0</v>
+      </c>
+      <c r="D51" s="26">
+        <v>2</v>
+      </c>
+      <c r="G51" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J51" s="26">
+        <f t="array" ref="J51">INDEX([1]combat_sim_results!A50:'[1]combat_sim_results'!E10048, MATCH(1, ([1]combat_sim_results!C50:'[1]combat_sim_results'!C10048=H51)*([1]combat_sim_results!D50:'[1]combat_sim_results'!D10048=I51)*([1]combat_sim_results!A50:'[1]combat_sim_results'!A10048=P50)*([1]combat_sim_results!B50:'[1]combat_sim_results'!B10048=O50), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y51" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C52" s="26">
+        <v>0</v>
+      </c>
+      <c r="D52" s="26">
+        <v>3</v>
+      </c>
+      <c r="G52" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J52" s="26">
+        <f t="array" ref="J52">INDEX([1]combat_sim_results!A51:'[1]combat_sim_results'!E10049, MATCH(1, ([1]combat_sim_results!C51:'[1]combat_sim_results'!C10049=H52)*([1]combat_sim_results!D51:'[1]combat_sim_results'!D10049=I52)*([1]combat_sim_results!A51:'[1]combat_sim_results'!A10049=P51)*([1]combat_sim_results!B51:'[1]combat_sim_results'!B10049=O51), 0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y52" s="26">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4027,18 +5915,18 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Cards!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E26</xm:sqref>
+          <xm:sqref>E44:E52 E3:E42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Playtest Options'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F26</xm:sqref>
+          <xm:sqref>F3:F52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Balance update for v7.0
* Tape Dispensor is actually useful now!
* Oil Rag is easier to get, which makes Minor Ductwork a tad less ominous
* Ugly Sweater Ghost gives a nice defeat bonus (let's see more Sprocket Snake!)
* Ugly Sweater Ghost got a Barter nerf too
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Use for +1 Carry</t>
   </si>
   <si>
-    <t>15 HP. 2 ATK.</t>
-  </si>
-  <si>
     <t>+1 ATK for 1 Oil</t>
   </si>
   <si>
@@ -198,10 +195,6 @@
 for 2 Metal, 1 Oil</t>
   </si>
   <si>
-    <t>Tape Dispensor
-for 3 Metal, 1 Oil</t>
-  </si>
-  <si>
     <t>8 HP. 2 ATK.</t>
   </si>
   <si>
@@ -216,14 +209,6 @@
     <t>Use in battle for -5 Creature HP</t>
   </si>
   <si>
-    <t>Oil Pan
-for 3 Metal, 1 Duct Tape</t>
-  </si>
-  <si>
-    <t>Oil Pan
-for 2 Metal, 1 Duct Tape</t>
-  </si>
-  <si>
     <t xml:space="preserve">17 HP. 4 ATK. </t>
   </si>
   <si>
@@ -258,9 +243,6 @@
   </si>
   <si>
     <t>Duct tape dealer, but with oil.</t>
-  </si>
-  <si>
-    <t>2:3 Metal:Fabric</t>
   </si>
   <si>
     <t>Oil to both Metal and Fabric</t>
@@ -356,9 +338,6 @@
     <t>Oil Rag</t>
   </si>
   <si>
-    <t>Gain 1 Duct Tape at first encounter each round</t>
-  </si>
-  <si>
     <t>10 HP. 3 ATK.
 +1 Carry upon Defeat</t>
   </si>
@@ -447,6 +426,20 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>Oil Rag
+for 3 Fabric</t>
+  </si>
+  <si>
+    <t>15 HP. 2 ATK.
++3 HP upon Defeat</t>
+  </si>
+  <si>
+    <t>Gain 2 Metal, 2 Fabric,  and 1 Oil for 1 Duct Tape, any time</t>
+  </si>
+  <si>
+    <t>2:2 Metal:Fabric</t>
   </si>
 </sst>
 </file>
@@ -622,10 +615,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1673,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,10 +1706,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -1728,16 +1721,16 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1763,13 +1756,13 @@
         <v>2</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K2" s="8">
         <v>1</v>
@@ -1779,7 +1772,7 @@
         <v>1.75</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N2" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K2,K$9:K$15,0))</f>
@@ -1788,7 +1781,7 @@
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -1809,13 +1802,13 @@
         <v>2</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" s="8">
         <v>2</v>
@@ -1825,7 +1818,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="N3" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K3,K$9:K$15,0))</f>
@@ -1855,10 +1848,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>10</v>
@@ -1871,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N4" s="7" t="str">
         <f t="shared" ref="N4:N7" si="1">INDEX(A$9:A$15,MATCH(K4,K$9:K$15,0))</f>
@@ -1901,13 +1894,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K5" s="8">
         <v>4</v>
@@ -1917,7 +1910,7 @@
         <v>2.25</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N5" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1926,7 +1919,7 @@
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -1949,11 +1942,11 @@
       <c r="H6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>54</v>
+      <c r="I6" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="K6" s="8">
         <v>5</v>
@@ -1963,7 +1956,7 @@
         <v>3.333333333333333</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="N6" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1993,13 +1986,13 @@
         <v>4</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="K7" s="8">
         <v>6</v>
@@ -2009,7 +2002,7 @@
         <v>2.25</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="N7" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2018,7 +2011,7 @@
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -2039,13 +2032,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>36</v>
+      <c r="J8" s="23" t="s">
+        <v>122</v>
       </c>
       <c r="K8" s="8">
         <v>7</v>
@@ -2055,7 +2048,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N8" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K8,K$9:K$15,0))</f>
@@ -2064,7 +2057,7 @@
     </row>
     <row r="9" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>13</v>
@@ -2085,13 +2078,13 @@
         <v>3</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K9" s="14">
         <v>7</v>
@@ -2101,7 +2094,7 @@
         <v>5.416666666666667</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="N9" s="13" t="str">
         <f>INDEX(A$2:A$8,MATCH(K9,K$2:K$8,0))</f>
@@ -2134,10 +2127,10 @@
         <v>34</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K10" s="14">
         <v>1</v>
@@ -2147,7 +2140,7 @@
         <v>2.5</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N10" s="13" t="str">
         <f t="shared" ref="N10:N15" si="2">INDEX(A$2:A$8,MATCH(K10,K$2:K$8,0))</f>
@@ -2177,13 +2170,13 @@
         <v>3</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="14">
         <v>2</v>
@@ -2193,7 +2186,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N11" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2223,13 +2216,13 @@
         <v>4</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K12" s="14">
         <v>4</v>
@@ -2239,7 +2232,7 @@
         <v>5.166666666666667</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N12" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2248,7 +2241,7 @@
     </row>
     <row r="13" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>13</v>
@@ -2269,13 +2262,13 @@
         <v>4</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K13" s="14">
         <v>3</v>
@@ -2285,7 +2278,7 @@
         <v>4.5</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N13" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2315,13 +2308,13 @@
         <v>4</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="K14" s="14">
         <v>5</v>
@@ -2331,7 +2324,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N14" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2361,13 +2354,13 @@
         <v>4</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K15" s="14">
         <v>6</v>
@@ -2377,7 +2370,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N15" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2395,13 +2388,13 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2418,7 +2411,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2426,15 +2419,15 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2442,7 +2435,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2450,7 +2443,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2491,12 +2484,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -2577,7 +2570,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" s="24">
         <f>B3/SUM($B3:$D3)</f>
@@ -2594,7 +2587,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B7" s="24">
         <f>B4/SUM($B4:$D4)</f>
@@ -2611,7 +2604,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B8" s="24">
         <f>B5/SUM($B5:$D5)</f>
@@ -2628,7 +2621,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" s="24">
         <f>4/9</f>
@@ -2656,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2691,34 +2684,34 @@
   <sheetData>
     <row r="1" spans="1:26" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>116</v>
-      </c>
       <c r="H1" s="27" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>2</v>
@@ -2733,13 +2726,13 @@
         <v>16</v>
       </c>
       <c r="O1" s="27" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="27" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="R1" s="25" t="s">
         <v>22</v>
@@ -2748,7 +2741,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="U1" s="25" t="s">
         <v>21</v>
@@ -2763,10 +2756,10 @@
         <v>28</v>
       </c>
       <c r="Y1" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z1" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="Z1" s="31" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -2824,7 +2817,7 @@
         <v>2.5</v>
       </c>
       <c r="Z2" s="30" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -2852,7 +2845,7 @@
       </c>
       <c r="J3" s="26" t="e">
         <f t="array" ref="J3">INDEX([1]combat_sim_results!A2:'[1]combat_sim_results'!E10000, MATCH(1, ([1]combat_sim_results!C2:'[1]combat_sim_results'!C10000=H3)*([1]combat_sim_results!D2:'[1]combat_sim_results'!D10000=I3)*([1]combat_sim_results!A2:'[1]combat_sim_results'!A10000=P2)*([1]combat_sim_results!B2:'[1]combat_sim_results'!B10000=O2), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K3" s="26">
         <v>4</v>
@@ -2921,12 +2914,12 @@
         <v>18</v>
       </c>
       <c r="G4" s="29" t="str">
-        <f t="shared" ref="G4:G26" si="1">IF(F4="Battle",J4,"")</f>
+        <f t="shared" ref="G4:G22" si="1">IF(F4="Battle",J4,"")</f>
         <v/>
       </c>
       <c r="J4" s="26" t="e">
         <f t="array" ref="J4">INDEX([1]combat_sim_results!A3:'[1]combat_sim_results'!E10001, MATCH(1, ([1]combat_sim_results!C3:'[1]combat_sim_results'!C10001=H4)*([1]combat_sim_results!D3:'[1]combat_sim_results'!D10001=I4)*([1]combat_sim_results!A3:'[1]combat_sim_results'!A10001=P3)*([1]combat_sim_results!B3:'[1]combat_sim_results'!B10001=O3), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K4" s="26">
         <v>1</v>
@@ -2989,7 +2982,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>18</v>
@@ -3000,7 +2993,7 @@
       </c>
       <c r="J5" s="26" t="e">
         <f t="array" ref="J5">INDEX([1]combat_sim_results!A4:'[1]combat_sim_results'!E10002, MATCH(1, ([1]combat_sim_results!C4:'[1]combat_sim_results'!C10002=H5)*([1]combat_sim_results!D4:'[1]combat_sim_results'!D10002=I5)*([1]combat_sim_results!A4:'[1]combat_sim_results'!A10002=P4)*([1]combat_sim_results!B4:'[1]combat_sim_results'!B10002=O4), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K5" s="26">
         <v>1</v>
@@ -3068,9 +3061,9 @@
       <c r="F6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="H6" s="26">
         <v>14</v>
@@ -3078,9 +3071,9 @@
       <c r="I6" s="26">
         <v>2</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="26" t="e">
         <f t="array" ref="J6">INDEX([1]combat_sim_results!A5:'[1]combat_sim_results'!E10003, MATCH(1, ([1]combat_sim_results!C5:'[1]combat_sim_results'!C10003=H6)*([1]combat_sim_results!D5:'[1]combat_sim_results'!D10003=I6)*([1]combat_sim_results!A5:'[1]combat_sim_results'!A10003=P5)*([1]combat_sim_results!B5:'[1]combat_sim_results'!B10003=O5), 0),5)</f>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="K6" s="26">
         <v>6</v>
@@ -3154,7 +3147,7 @@
       </c>
       <c r="J7" s="26" t="e">
         <f t="array" ref="J7">INDEX([1]combat_sim_results!A6:'[1]combat_sim_results'!E10004, MATCH(1, ([1]combat_sim_results!C6:'[1]combat_sim_results'!C10004=H7)*([1]combat_sim_results!D6:'[1]combat_sim_results'!D10004=I7)*([1]combat_sim_results!A6:'[1]combat_sim_results'!A10004=P6)*([1]combat_sim_results!B6:'[1]combat_sim_results'!B10004=O6), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K7" s="26">
         <v>6</v>
@@ -3217,7 +3210,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>18</v>
@@ -3228,7 +3221,7 @@
       </c>
       <c r="J8" s="26" t="e">
         <f t="array" ref="J8">INDEX([1]combat_sim_results!A7:'[1]combat_sim_results'!E10005, MATCH(1, ([1]combat_sim_results!C7:'[1]combat_sim_results'!C10005=H8)*([1]combat_sim_results!D7:'[1]combat_sim_results'!D10005=I8)*([1]combat_sim_results!A7:'[1]combat_sim_results'!A10005=P7)*([1]combat_sim_results!B7:'[1]combat_sim_results'!B10005=O7), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K8" s="26">
         <v>6</v>
@@ -3296,9 +3289,9 @@
       <c r="F9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.88600000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="H9" s="26">
         <v>8</v>
@@ -3306,9 +3299,9 @@
       <c r="I9" s="26">
         <v>4</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="26" t="e">
         <f t="array" ref="J9">INDEX([1]combat_sim_results!A8:'[1]combat_sim_results'!E10006, MATCH(1, ([1]combat_sim_results!C8:'[1]combat_sim_results'!C10006=H9)*([1]combat_sim_results!D8:'[1]combat_sim_results'!D10006=I9)*([1]combat_sim_results!A8:'[1]combat_sim_results'!A10006=P8)*([1]combat_sim_results!B8:'[1]combat_sim_results'!B10006=O8), 0),5)</f>
-        <v>0.88600000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="K9" s="26">
         <v>13</v>
@@ -3371,7 +3364,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>5</v>
@@ -3382,7 +3375,7 @@
       </c>
       <c r="J10" s="26" t="e">
         <f t="array" ref="J10">INDEX([1]combat_sim_results!A9:'[1]combat_sim_results'!E10007, MATCH(1, ([1]combat_sim_results!C9:'[1]combat_sim_results'!C10007=H10)*([1]combat_sim_results!D9:'[1]combat_sim_results'!D10007=I10)*([1]combat_sim_results!A9:'[1]combat_sim_results'!A10007=P9)*([1]combat_sim_results!B9:'[1]combat_sim_results'!B10007=O9), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K10" s="26">
         <v>9</v>
@@ -3445,7 +3438,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F11" s="26" t="s">
         <v>5</v>
@@ -3456,7 +3449,7 @@
       </c>
       <c r="J11" s="26" t="e">
         <f t="array" ref="J11">INDEX([1]combat_sim_results!A10:'[1]combat_sim_results'!E10008, MATCH(1, ([1]combat_sim_results!C10:'[1]combat_sim_results'!C10008=H11)*([1]combat_sim_results!D10:'[1]combat_sim_results'!D10008=I11)*([1]combat_sim_results!A10:'[1]combat_sim_results'!A10008=P10)*([1]combat_sim_results!B10:'[1]combat_sim_results'!B10008=O10), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K11" s="26">
         <v>7</v>
@@ -3530,7 +3523,7 @@
       </c>
       <c r="J12" s="26" t="e">
         <f t="array" ref="J12">INDEX([1]combat_sim_results!A11:'[1]combat_sim_results'!E10009, MATCH(1, ([1]combat_sim_results!C11:'[1]combat_sim_results'!C10009=H12)*([1]combat_sim_results!D11:'[1]combat_sim_results'!D10009=I12)*([1]combat_sim_results!A11:'[1]combat_sim_results'!A10009=P11)*([1]combat_sim_results!B11:'[1]combat_sim_results'!B10009=O11), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K12" s="26">
         <v>9</v>
@@ -3593,7 +3586,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>5</v>
@@ -3604,7 +3597,7 @@
       </c>
       <c r="J13" s="26" t="e">
         <f t="array" ref="J13">INDEX([1]combat_sim_results!A12:'[1]combat_sim_results'!E10010, MATCH(1, ([1]combat_sim_results!C12:'[1]combat_sim_results'!C10010=H13)*([1]combat_sim_results!D12:'[1]combat_sim_results'!D10010=I13)*([1]combat_sim_results!A12:'[1]combat_sim_results'!A10010=P12)*([1]combat_sim_results!B12:'[1]combat_sim_results'!B10010=O12), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K13" s="26">
         <v>6</v>
@@ -3667,7 +3660,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F14" s="26" t="s">
         <v>5</v>
@@ -3678,7 +3671,7 @@
       </c>
       <c r="J14" s="26" t="e">
         <f t="array" ref="J14">INDEX([1]combat_sim_results!A13:'[1]combat_sim_results'!E10011, MATCH(1, ([1]combat_sim_results!C13:'[1]combat_sim_results'!C10011=H14)*([1]combat_sim_results!D13:'[1]combat_sim_results'!D10011=I14)*([1]combat_sim_results!A13:'[1]combat_sim_results'!A10011=P13)*([1]combat_sim_results!B13:'[1]combat_sim_results'!B10011=O13), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K14" s="26">
         <v>2</v>
@@ -3746,9 +3739,9 @@
       <c r="F15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.98599999999999999</v>
+        <v>#REF!</v>
       </c>
       <c r="H15" s="26">
         <v>12</v>
@@ -3756,9 +3749,9 @@
       <c r="I15" s="26">
         <v>2</v>
       </c>
-      <c r="J15" s="26">
+      <c r="J15" s="26" t="e">
         <f t="array" ref="J15">INDEX([1]combat_sim_results!A14:'[1]combat_sim_results'!E10012, MATCH(1, ([1]combat_sim_results!C14:'[1]combat_sim_results'!C10012=H15)*([1]combat_sim_results!D14:'[1]combat_sim_results'!D10012=I15)*([1]combat_sim_results!A14:'[1]combat_sim_results'!A10012=P14)*([1]combat_sim_results!B14:'[1]combat_sim_results'!B10012=O14), 0),5)</f>
-        <v>0.98599999999999999</v>
+        <v>#REF!</v>
       </c>
       <c r="K15" s="26">
         <v>9</v>
@@ -3832,7 +3825,7 @@
       </c>
       <c r="J16" s="26" t="e">
         <f t="array" ref="J16">INDEX([1]combat_sim_results!A15:'[1]combat_sim_results'!E10013, MATCH(1, ([1]combat_sim_results!C15:'[1]combat_sim_results'!C10013=H16)*([1]combat_sim_results!D15:'[1]combat_sim_results'!D10013=I16)*([1]combat_sim_results!A15:'[1]combat_sim_results'!A10013=P15)*([1]combat_sim_results!B15:'[1]combat_sim_results'!B10013=O15), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K16" s="26">
         <v>9</v>
@@ -3900,9 +3893,9 @@
       <c r="F17" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.33400000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="H17" s="26">
         <v>11</v>
@@ -3910,9 +3903,9 @@
       <c r="I17" s="26">
         <v>4</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="26" t="e">
         <f t="array" ref="J17">INDEX([1]combat_sim_results!A16:'[1]combat_sim_results'!E10014, MATCH(1, ([1]combat_sim_results!C16:'[1]combat_sim_results'!C10014=H17)*([1]combat_sim_results!D16:'[1]combat_sim_results'!D10014=I17)*([1]combat_sim_results!A16:'[1]combat_sim_results'!A10014=P16)*([1]combat_sim_results!B16:'[1]combat_sim_results'!B10014=O16), 0),5)</f>
-        <v>0.33400000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="K17" s="26">
         <v>14</v>
@@ -3961,7 +3954,7 @@
         <v>7.5</v>
       </c>
       <c r="Z17" s="30" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -3978,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>5</v>
@@ -3989,7 +3982,7 @@
       </c>
       <c r="J18" s="26" t="e">
         <f t="array" ref="J18">INDEX([1]combat_sim_results!A17:'[1]combat_sim_results'!E10015, MATCH(1, ([1]combat_sim_results!C17:'[1]combat_sim_results'!C10015=H18)*([1]combat_sim_results!D17:'[1]combat_sim_results'!D10015=I18)*([1]combat_sim_results!A17:'[1]combat_sim_results'!A10015=P17)*([1]combat_sim_results!B17:'[1]combat_sim_results'!B10015=O17), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K18" s="26">
         <v>6</v>
@@ -4052,7 +4045,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>5</v>
@@ -4063,7 +4056,7 @@
       </c>
       <c r="J19" s="26" t="e">
         <f t="array" ref="J19">INDEX([1]combat_sim_results!A18:'[1]combat_sim_results'!E10016, MATCH(1, ([1]combat_sim_results!C18:'[1]combat_sim_results'!C10016=H19)*([1]combat_sim_results!D18:'[1]combat_sim_results'!D10016=I19)*([1]combat_sim_results!A18:'[1]combat_sim_results'!A10016=P18)*([1]combat_sim_results!B18:'[1]combat_sim_results'!B10016=O18), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K19" s="26">
         <v>6</v>
@@ -4137,7 +4130,7 @@
       </c>
       <c r="J20" s="26" t="e">
         <f t="array" ref="J20">INDEX([1]combat_sim_results!A19:'[1]combat_sim_results'!E10017, MATCH(1, ([1]combat_sim_results!C19:'[1]combat_sim_results'!C10017=H20)*([1]combat_sim_results!D19:'[1]combat_sim_results'!D10017=I20)*([1]combat_sim_results!A19:'[1]combat_sim_results'!A10017=P19)*([1]combat_sim_results!B19:'[1]combat_sim_results'!B10017=O19), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K20" s="26">
         <v>6</v>
@@ -4200,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>6</v>
@@ -4265,7 +4258,7 @@
         <v>9.25</v>
       </c>
       <c r="Z21" s="30" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -4287,7 +4280,7 @@
       </c>
       <c r="J22" s="26" t="e">
         <f t="array" ref="J22">INDEX([1]combat_sim_results!A21:'[1]combat_sim_results'!E10019, MATCH(1, ([1]combat_sim_results!C21:'[1]combat_sim_results'!C10019=H22)*([1]combat_sim_results!D21:'[1]combat_sim_results'!D10019=I22)*([1]combat_sim_results!A21:'[1]combat_sim_results'!A10019=P21)*([1]combat_sim_results!B21:'[1]combat_sim_results'!B10019=O21), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="Y22" s="26">
         <f t="shared" si="0"/>
@@ -4311,9 +4304,9 @@
         <f t="shared" ref="G23:G52" si="2">IF(F23="Battle",J23,"")</f>
         <v/>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="26" t="e">
         <f t="array" ref="J23">INDEX([1]combat_sim_results!A22:'[1]combat_sim_results'!E10020, MATCH(1, ([1]combat_sim_results!C22:'[1]combat_sim_results'!C10020=H23)*([1]combat_sim_results!D22:'[1]combat_sim_results'!D10020=I23)*([1]combat_sim_results!A22:'[1]combat_sim_results'!A10020=P22)*([1]combat_sim_results!B22:'[1]combat_sim_results'!B10020=O22), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y23" s="26">
         <f t="shared" si="0"/>
@@ -4337,9 +4330,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J24" s="26">
+      <c r="J24" s="26" t="e">
         <f t="array" ref="J24">INDEX([1]combat_sim_results!A23:'[1]combat_sim_results'!E10021, MATCH(1, ([1]combat_sim_results!C23:'[1]combat_sim_results'!C10021=H24)*([1]combat_sim_results!D23:'[1]combat_sim_results'!D10021=I24)*([1]combat_sim_results!A23:'[1]combat_sim_results'!A10021=P23)*([1]combat_sim_results!B23:'[1]combat_sim_results'!B10021=O23), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y24" s="26">
         <f t="shared" si="0"/>
@@ -4363,9 +4356,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J25" s="26">
+      <c r="J25" s="26" t="e">
         <f t="array" ref="J25">INDEX([1]combat_sim_results!A24:'[1]combat_sim_results'!E10022, MATCH(1, ([1]combat_sim_results!C24:'[1]combat_sim_results'!C10022=H25)*([1]combat_sim_results!D24:'[1]combat_sim_results'!D10022=I25)*([1]combat_sim_results!A24:'[1]combat_sim_results'!A10022=P24)*([1]combat_sim_results!B24:'[1]combat_sim_results'!B10022=O24), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y25" s="26">
         <f t="shared" si="0"/>
@@ -4389,9 +4382,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J26" s="26">
+      <c r="J26" s="26" t="e">
         <f t="array" ref="J26">INDEX([1]combat_sim_results!A25:'[1]combat_sim_results'!E10023, MATCH(1, ([1]combat_sim_results!C25:'[1]combat_sim_results'!C10023=H26)*([1]combat_sim_results!D25:'[1]combat_sim_results'!D10023=I26)*([1]combat_sim_results!A25:'[1]combat_sim_results'!A10023=P25)*([1]combat_sim_results!B25:'[1]combat_sim_results'!B10023=O25), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y26" s="26">
         <f t="shared" si="0"/>
@@ -4403,9 +4396,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J27" s="26">
+      <c r="J27" s="26" t="e">
         <f t="array" ref="J27">INDEX([1]combat_sim_results!A26:'[1]combat_sim_results'!E10024, MATCH(1, ([1]combat_sim_results!C26:'[1]combat_sim_results'!C10024=H27)*([1]combat_sim_results!D26:'[1]combat_sim_results'!D10024=I27)*([1]combat_sim_results!A26:'[1]combat_sim_results'!A10024=P26)*([1]combat_sim_results!B26:'[1]combat_sim_results'!B10024=O26), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -4413,9 +4406,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="26" t="e">
         <f t="array" ref="J28">INDEX([1]combat_sim_results!A27:'[1]combat_sim_results'!E10025, MATCH(1, ([1]combat_sim_results!C27:'[1]combat_sim_results'!C10025=H28)*([1]combat_sim_results!D27:'[1]combat_sim_results'!D10025=I28)*([1]combat_sim_results!A27:'[1]combat_sim_results'!A10025=P27)*([1]combat_sim_results!B27:'[1]combat_sim_results'!B10025=O27), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="K28" s="26">
         <v>4</v>
@@ -4464,7 +4457,7 @@
         <v>2.5</v>
       </c>
       <c r="Z28" s="30" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -4475,7 +4468,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F29" s="26" t="s">
         <v>5</v>
@@ -4486,7 +4479,7 @@
       </c>
       <c r="J29" s="26" t="e">
         <f t="array" ref="J29">INDEX([1]combat_sim_results!A28:'[1]combat_sim_results'!E10026, MATCH(1, ([1]combat_sim_results!C28:'[1]combat_sim_results'!C10026=H29)*([1]combat_sim_results!D28:'[1]combat_sim_results'!D10026=I29)*([1]combat_sim_results!A28:'[1]combat_sim_results'!A10026=P28)*([1]combat_sim_results!B28:'[1]combat_sim_results'!B10026=O28), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K29" s="26">
         <v>0</v>
@@ -4554,7 +4547,7 @@
       </c>
       <c r="J30" s="26" t="e">
         <f t="array" ref="J30">INDEX([1]combat_sim_results!A29:'[1]combat_sim_results'!E10027, MATCH(1, ([1]combat_sim_results!C29:'[1]combat_sim_results'!C10027=H30)*([1]combat_sim_results!D29:'[1]combat_sim_results'!D10027=I30)*([1]combat_sim_results!A29:'[1]combat_sim_results'!A10027=P29)*([1]combat_sim_results!B29:'[1]combat_sim_results'!B10027=O29), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K30" s="26">
         <v>3</v>
@@ -4611,7 +4604,7 @@
         <v>3</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F31" s="26" t="s">
         <v>18</v>
@@ -4622,7 +4615,7 @@
       </c>
       <c r="J31" s="26" t="e">
         <f t="array" ref="J31">INDEX([1]combat_sim_results!A30:'[1]combat_sim_results'!E10028, MATCH(1, ([1]combat_sim_results!C30:'[1]combat_sim_results'!C10028=H31)*([1]combat_sim_results!D30:'[1]combat_sim_results'!D10028=I31)*([1]combat_sim_results!A30:'[1]combat_sim_results'!A10028=P30)*([1]combat_sim_results!B30:'[1]combat_sim_results'!B10028=O30), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K31" s="26">
         <v>3</v>
@@ -4679,7 +4672,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>5</v>
@@ -4690,7 +4683,7 @@
       </c>
       <c r="J32" s="26" t="e">
         <f t="array" ref="J32">INDEX([1]combat_sim_results!A31:'[1]combat_sim_results'!E10029, MATCH(1, ([1]combat_sim_results!C31:'[1]combat_sim_results'!C10029=H32)*([1]combat_sim_results!D31:'[1]combat_sim_results'!D10029=I32)*([1]combat_sim_results!A31:'[1]combat_sim_results'!A10029=P31)*([1]combat_sim_results!B31:'[1]combat_sim_results'!B10029=O31), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K32" s="26">
         <v>1</v>
@@ -4758,7 +4751,7 @@
       </c>
       <c r="J33" s="26" t="e">
         <f t="array" ref="J33">INDEX([1]combat_sim_results!A32:'[1]combat_sim_results'!E10030, MATCH(1, ([1]combat_sim_results!C32:'[1]combat_sim_results'!C10030=H33)*([1]combat_sim_results!D32:'[1]combat_sim_results'!D10030=I33)*([1]combat_sim_results!A32:'[1]combat_sim_results'!A10030=P32)*([1]combat_sim_results!B32:'[1]combat_sim_results'!B10030=O32), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K33" s="26">
         <v>1</v>
@@ -4815,7 +4808,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F34" s="26" t="s">
         <v>18</v>
@@ -4830,9 +4823,9 @@
       <c r="I34" s="26">
         <v>2</v>
       </c>
-      <c r="J34" s="26">
+      <c r="J34" s="26" t="e">
         <f t="array" ref="J34">INDEX([1]combat_sim_results!A33:'[1]combat_sim_results'!E10031, MATCH(1, ([1]combat_sim_results!C33:'[1]combat_sim_results'!C10031=H34)*([1]combat_sim_results!D33:'[1]combat_sim_results'!D10031=I34)*([1]combat_sim_results!A33:'[1]combat_sim_results'!A10031=P33)*([1]combat_sim_results!B33:'[1]combat_sim_results'!B10031=O33), 0),5)</f>
-        <v>0.97299999999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="K34" s="26">
         <v>3</v>
@@ -4889,7 +4882,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F35" s="26" t="s">
         <v>5</v>
@@ -4900,7 +4893,7 @@
       </c>
       <c r="J35" s="26" t="e">
         <f t="array" ref="J35">INDEX([1]combat_sim_results!A34:'[1]combat_sim_results'!E10032, MATCH(1, ([1]combat_sim_results!C34:'[1]combat_sim_results'!C10032=H35)*([1]combat_sim_results!D34:'[1]combat_sim_results'!D10032=I35)*([1]combat_sim_results!A34:'[1]combat_sim_results'!A10032=P34)*([1]combat_sim_results!B34:'[1]combat_sim_results'!B10032=O34), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K35" s="26">
         <v>1</v>
@@ -4957,14 +4950,14 @@
         <v>2</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.59099999999999997</v>
+        <v>#REF!</v>
       </c>
       <c r="H36" s="26">
         <v>10</v>
@@ -4972,9 +4965,9 @@
       <c r="I36" s="26">
         <v>3</v>
       </c>
-      <c r="J36" s="26">
+      <c r="J36" s="26" t="e">
         <f t="array" ref="J36">INDEX([1]combat_sim_results!A35:'[1]combat_sim_results'!E10033, MATCH(1, ([1]combat_sim_results!C35:'[1]combat_sim_results'!C10033=H36)*([1]combat_sim_results!D35:'[1]combat_sim_results'!D10033=I36)*([1]combat_sim_results!A35:'[1]combat_sim_results'!A10033=P35)*([1]combat_sim_results!B35:'[1]combat_sim_results'!B10033=O35), 0),5)</f>
-        <v>0.59099999999999997</v>
+        <v>#REF!</v>
       </c>
       <c r="K36" s="26">
         <v>5</v>
@@ -5023,7 +5016,7 @@
         <v>5.75</v>
       </c>
       <c r="Z36" s="30" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="3:26" x14ac:dyDescent="0.25">
@@ -5045,7 +5038,7 @@
       </c>
       <c r="J37" s="26" t="e">
         <f t="array" ref="J37">INDEX([1]combat_sim_results!A36:'[1]combat_sim_results'!E10034, MATCH(1, ([1]combat_sim_results!C36:'[1]combat_sim_results'!C10034=H37)*([1]combat_sim_results!D36:'[1]combat_sim_results'!D10034=I37)*([1]combat_sim_results!A36:'[1]combat_sim_results'!A10034=P36)*([1]combat_sim_results!B36:'[1]combat_sim_results'!B10034=O36), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K37" s="26">
         <v>3</v>
@@ -5113,7 +5106,7 @@
       </c>
       <c r="J38" s="26" t="e">
         <f t="array" ref="J38">INDEX([1]combat_sim_results!A37:'[1]combat_sim_results'!E10035, MATCH(1, ([1]combat_sim_results!C37:'[1]combat_sim_results'!C10035=H38)*([1]combat_sim_results!D37:'[1]combat_sim_results'!D10035=I38)*([1]combat_sim_results!A37:'[1]combat_sim_results'!A10035=P37)*([1]combat_sim_results!B37:'[1]combat_sim_results'!B10035=O37), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K38" s="26">
         <v>5</v>
@@ -5170,7 +5163,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F39" s="26" t="s">
         <v>18</v>
@@ -5181,7 +5174,7 @@
       </c>
       <c r="J39" s="26" t="e">
         <f t="array" ref="J39">INDEX([1]combat_sim_results!A38:'[1]combat_sim_results'!E10036, MATCH(1, ([1]combat_sim_results!C38:'[1]combat_sim_results'!C10036=H39)*([1]combat_sim_results!D38:'[1]combat_sim_results'!D10036=I39)*([1]combat_sim_results!A38:'[1]combat_sim_results'!A10036=P38)*([1]combat_sim_results!B38:'[1]combat_sim_results'!B10036=O38), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K39" s="26">
         <v>5</v>
@@ -5249,7 +5242,7 @@
       </c>
       <c r="J40" s="26" t="e">
         <f t="array" ref="J40">INDEX([1]combat_sim_results!A39:'[1]combat_sim_results'!E10037, MATCH(1, ([1]combat_sim_results!C39:'[1]combat_sim_results'!C10037=H40)*([1]combat_sim_results!D39:'[1]combat_sim_results'!D10037=I40)*([1]combat_sim_results!A39:'[1]combat_sim_results'!A10037=P39)*([1]combat_sim_results!B39:'[1]combat_sim_results'!B10037=O39), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K40" s="26">
         <v>1</v>
@@ -5317,7 +5310,7 @@
       </c>
       <c r="J41" s="26" t="e">
         <f t="array" ref="J41">INDEX([1]combat_sim_results!A40:'[1]combat_sim_results'!E10038, MATCH(1, ([1]combat_sim_results!C40:'[1]combat_sim_results'!C10038=H41)*([1]combat_sim_results!D40:'[1]combat_sim_results'!D10038=I41)*([1]combat_sim_results!A40:'[1]combat_sim_results'!A10038=P40)*([1]combat_sim_results!B40:'[1]combat_sim_results'!B10038=O40), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K41" s="26">
         <v>1</v>
@@ -5379,9 +5372,9 @@
       <c r="F42" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.89100000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="H42" s="26">
         <v>8</v>
@@ -5389,9 +5382,9 @@
       <c r="I42" s="26">
         <v>4</v>
       </c>
-      <c r="J42" s="26">
+      <c r="J42" s="26" t="e">
         <f t="array" ref="J42">INDEX([1]combat_sim_results!A41:'[1]combat_sim_results'!E10039, MATCH(1, ([1]combat_sim_results!C41:'[1]combat_sim_results'!C10039=H42)*([1]combat_sim_results!D41:'[1]combat_sim_results'!D10039=I42)*([1]combat_sim_results!A41:'[1]combat_sim_results'!A10039=P41)*([1]combat_sim_results!B41:'[1]combat_sim_results'!B10039=O41), 0),5)</f>
-        <v>0.89100000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="K42" s="26">
         <v>6</v>
@@ -5440,7 +5433,7 @@
         <v>4.6666666666666661</v>
       </c>
       <c r="Z42" s="30" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
@@ -5459,7 +5452,7 @@
       </c>
       <c r="J43" s="26" t="e">
         <f t="array" ref="J43">INDEX([1]combat_sim_results!A42:'[1]combat_sim_results'!E10040, MATCH(1, ([1]combat_sim_results!C42:'[1]combat_sim_results'!C10040=H43)*([1]combat_sim_results!D42:'[1]combat_sim_results'!D10040=I43)*([1]combat_sim_results!A42:'[1]combat_sim_results'!A10040=P42)*([1]combat_sim_results!B42:'[1]combat_sim_results'!B10040=O42), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K43" s="26">
         <v>6</v>
@@ -5516,7 +5509,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F44" s="26" t="s">
         <v>5</v>
@@ -5527,7 +5520,7 @@
       </c>
       <c r="J44" s="26" t="e">
         <f t="array" ref="J44">INDEX([1]combat_sim_results!A43:'[1]combat_sim_results'!E10041, MATCH(1, ([1]combat_sim_results!C43:'[1]combat_sim_results'!C10041=H44)*([1]combat_sim_results!D43:'[1]combat_sim_results'!D10041=I44)*([1]combat_sim_results!A43:'[1]combat_sim_results'!A10041=P43)*([1]combat_sim_results!B43:'[1]combat_sim_results'!B10041=O43), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K44" s="26">
         <v>6</v>
@@ -5595,7 +5588,7 @@
       </c>
       <c r="J45" s="26" t="e">
         <f t="array" ref="J45">INDEX([1]combat_sim_results!A44:'[1]combat_sim_results'!E10042, MATCH(1, ([1]combat_sim_results!C44:'[1]combat_sim_results'!C10042=H45)*([1]combat_sim_results!D44:'[1]combat_sim_results'!D10042=I45)*([1]combat_sim_results!A44:'[1]combat_sim_results'!A10042=P44)*([1]combat_sim_results!B44:'[1]combat_sim_results'!B10042=O44), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K45" s="26">
         <v>6</v>
@@ -5644,7 +5637,7 @@
         <v>7.666666666666667</v>
       </c>
       <c r="Z45" s="30" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.25">
@@ -5666,7 +5659,7 @@
       </c>
       <c r="J46" s="26" t="e">
         <f t="array" ref="J46">INDEX([1]combat_sim_results!A45:'[1]combat_sim_results'!E10043, MATCH(1, ([1]combat_sim_results!C45:'[1]combat_sim_results'!C10043=H46)*([1]combat_sim_results!D45:'[1]combat_sim_results'!D10043=I46)*([1]combat_sim_results!A45:'[1]combat_sim_results'!A10043=P45)*([1]combat_sim_results!B45:'[1]combat_sim_results'!B10043=O45), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K46" s="26">
         <v>6</v>
@@ -5728,9 +5721,9 @@
       <c r="F47" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.80300000000000005</v>
+        <v>#REF!</v>
       </c>
       <c r="H47" s="26">
         <v>11</v>
@@ -5738,9 +5731,9 @@
       <c r="I47" s="26">
         <v>4</v>
       </c>
-      <c r="J47" s="26">
+      <c r="J47" s="26" t="e">
         <f t="array" ref="J47">INDEX([1]combat_sim_results!A46:'[1]combat_sim_results'!E10044, MATCH(1, ([1]combat_sim_results!C46:'[1]combat_sim_results'!C10044=H47)*([1]combat_sim_results!D46:'[1]combat_sim_results'!D10044=I47)*([1]combat_sim_results!A46:'[1]combat_sim_results'!A10044=P46)*([1]combat_sim_results!B46:'[1]combat_sim_results'!B10044=O46), 0),5)</f>
-        <v>0.80300000000000005</v>
+        <v>#REF!</v>
       </c>
       <c r="K47" s="26">
         <v>7</v>
@@ -5789,7 +5782,7 @@
         <v>8.9166666666666661</v>
       </c>
       <c r="Z47" s="30" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="3:26" x14ac:dyDescent="0.25">
@@ -5805,9 +5798,9 @@
       <c r="F48" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G48" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="H48" s="26">
         <v>15</v>
@@ -5815,16 +5808,16 @@
       <c r="I48" s="26">
         <v>4</v>
       </c>
-      <c r="J48" s="26">
+      <c r="J48" s="26" t="e">
         <f t="array" ref="J48">INDEX([1]combat_sim_results!A47:'[1]combat_sim_results'!E10045, MATCH(1, ([1]combat_sim_results!C47:'[1]combat_sim_results'!C10045=H48)*([1]combat_sim_results!D47:'[1]combat_sim_results'!D10045=I48)*([1]combat_sim_results!A47:'[1]combat_sim_results'!A10045=P47)*([1]combat_sim_results!B47:'[1]combat_sim_results'!B10045=O47), 0),5)</f>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="Y48" s="26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z48" s="30" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="3:25" x14ac:dyDescent="0.25">
@@ -5838,9 +5831,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J49" s="26">
+      <c r="J49" s="26" t="e">
         <f t="array" ref="J49">INDEX([1]combat_sim_results!A48:'[1]combat_sim_results'!E10046, MATCH(1, ([1]combat_sim_results!C48:'[1]combat_sim_results'!C10046=H49)*([1]combat_sim_results!D48:'[1]combat_sim_results'!D10046=I49)*([1]combat_sim_results!A48:'[1]combat_sim_results'!A10046=P48)*([1]combat_sim_results!B48:'[1]combat_sim_results'!B10046=O48), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y49" s="26">
         <f t="shared" si="3"/>
@@ -5858,9 +5851,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J50" s="26">
+      <c r="J50" s="26" t="e">
         <f t="array" ref="J50">INDEX([1]combat_sim_results!A49:'[1]combat_sim_results'!E10047, MATCH(1, ([1]combat_sim_results!C49:'[1]combat_sim_results'!C10047=H50)*([1]combat_sim_results!D49:'[1]combat_sim_results'!D10047=I50)*([1]combat_sim_results!A49:'[1]combat_sim_results'!A10047=P49)*([1]combat_sim_results!B49:'[1]combat_sim_results'!B10047=O49), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y50" s="26">
         <f t="shared" si="3"/>
@@ -5878,9 +5871,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J51" s="26">
+      <c r="J51" s="26" t="e">
         <f t="array" ref="J51">INDEX([1]combat_sim_results!A50:'[1]combat_sim_results'!E10048, MATCH(1, ([1]combat_sim_results!C50:'[1]combat_sim_results'!C10048=H51)*([1]combat_sim_results!D50:'[1]combat_sim_results'!D10048=I51)*([1]combat_sim_results!A50:'[1]combat_sim_results'!A10048=P50)*([1]combat_sim_results!B50:'[1]combat_sim_results'!B10048=O50), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y51" s="26">
         <f t="shared" si="3"/>
@@ -5898,9 +5891,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J52" s="26">
+      <c r="J52" s="26" t="e">
         <f t="array" ref="J52">INDEX([1]combat_sim_results!A51:'[1]combat_sim_results'!E10049, MATCH(1, ([1]combat_sim_results!C51:'[1]combat_sim_results'!C10049=H52)*([1]combat_sim_results!D51:'[1]combat_sim_results'!D10049=I52)*([1]combat_sim_results!A51:'[1]combat_sim_results'!A10049=P51)*([1]combat_sim_results!B51:'[1]combat_sim_results'!B10049=O51), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y52" s="26">
         <f t="shared" si="3"/>
@@ -5915,7 +5908,7 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Cards!$A$2:$A$15</xm:f>
@@ -5946,7 +5939,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
balancing: battling & big creatures are better
* Tape dispensor just wasn't cutting it. Replaced with Shiny Shiv to represent a more aggressive battle-heavy strategy
* Boosted HP of some creatures since Shiny Shiv allows for better battling
* Ugly Sweater Ghost lowered HP to give people a reason to battle him
* Made some Big creatures more tantalizing, like Sprocket Snake and Tap Spider
* Nerfed a few "Have" powers like the Strong Magnet and Whacking Plank
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Oil Nymph</t>
-  </si>
-  <si>
-    <t>6 HP. 1 ATK.</t>
   </si>
   <si>
     <t>Minor Ductwork</t>
@@ -161,26 +158,16 @@
 for 2/4 Fabric</t>
   </si>
   <si>
-    <t>1:2 Metal:Fabric</t>
-  </si>
-  <si>
     <t>20 HP. 4 ATK.</t>
   </si>
   <si>
     <t>Est. Value</t>
   </si>
   <si>
-    <t>16 HP. 3 ATK.
- ⃠ Have Strong Magnet</t>
-  </si>
-  <si>
     <t>+1 ATK for 4 Metal</t>
   </si>
   <si>
     <t xml:space="preserve">+2 Duct Tape for Disassembling 1 Tool </t>
-  </si>
-  <si>
-    <t>+2 Metal and +2 Fabric for 2 Oil</t>
   </si>
   <si>
     <t>Bandages
@@ -191,13 +178,6 @@
 for 1 Fabric, 1 Oil</t>
   </si>
   <si>
-    <t>Tape Dispensor
-for 2 Metal, 1 Oil</t>
-  </si>
-  <si>
-    <t>8 HP. 2 ATK.</t>
-  </si>
-  <si>
     <t>12 HP. 2 ATK. 
  ⃠ Have Tote Bag</t>
   </si>
@@ -212,9 +192,6 @@
     <t xml:space="preserve">17 HP. 4 ATK. </t>
   </si>
   <si>
-    <t>5:3 Metal:Fabric</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -249,10 +226,6 @@
   </si>
   <si>
     <t>Metal dealer, but you need lots of fabric. Or lots of Metal.</t>
-  </si>
-  <si>
-    <t>11 HP. 4 ATK
-⃠ Have Whacking Plank</t>
   </si>
   <si>
     <t>Friendly Can of Lube</t>
@@ -432,14 +405,45 @@
 for 3 Fabric</t>
   </si>
   <si>
-    <t>15 HP. 2 ATK.
+    <t>2:2 Metal:Fabric</t>
+  </si>
+  <si>
+    <t>Shiny Shiv
+for 2 Metal, 1 Oil</t>
+  </si>
+  <si>
+    <t>Shiny Shiv</t>
+  </si>
+  <si>
+    <t>Creatures start with 2HP fewer each battle</t>
+  </si>
+  <si>
+    <t>10 HP. 2 ATK.</t>
+  </si>
+  <si>
+    <t>7 HP. 1 ATK.</t>
+  </si>
+  <si>
+    <t>13 HP. 2 ATK.
 +3 HP upon Defeat</t>
   </si>
   <si>
-    <t>Gain 2 Metal, 2 Fabric,  and 1 Oil for 1 Duct Tape, any time</t>
-  </si>
-  <si>
-    <t>2:2 Metal:Fabric</t>
+    <t>11 HP. 4 ATK
+⃠ Ditch Whacking Plank</t>
+  </si>
+  <si>
+    <t>16 HP. 3 ATK.
+ ⃠ Ditch Strong Magnet</t>
+  </si>
+  <si>
+    <t>2:3 Metal:Fabric</t>
+  </si>
+  <si>
+    <t>2:2 Metal:Oil
+or 1:1 Fabric:Oil</t>
+  </si>
+  <si>
+    <t>+1 ATK for -1 Carry</t>
   </si>
 </sst>
 </file>
@@ -522,7 +526,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1666,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,31 +1713,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1756,13 +1763,13 @@
         <v>2</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>49</v>
+        <v>66</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="K2" s="8">
         <v>1</v>
@@ -1772,7 +1779,7 @@
         <v>1.75</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="N2" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K2,K$9:K$15,0))</f>
@@ -1781,7 +1788,7 @@
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -1802,13 +1809,13 @@
         <v>2</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="K3" s="8">
         <v>2</v>
@@ -1818,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="N3" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K3,K$9:K$15,0))</f>
@@ -1827,7 +1834,7 @@
     </row>
     <row r="4" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
@@ -1848,13 +1855,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="K4" s="8">
         <v>3</v>
@@ -1864,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="N4" s="7" t="str">
         <f t="shared" ref="N4:N7" si="1">INDEX(A$9:A$15,MATCH(K4,K$9:K$15,0))</f>
@@ -1873,7 +1880,7 @@
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>8</v>
@@ -1894,13 +1901,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K5" s="8">
         <v>4</v>
@@ -1910,7 +1917,7 @@
         <v>2.25</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="N5" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1919,7 +1926,7 @@
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -1940,13 +1947,13 @@
         <v>3</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K6" s="8">
         <v>5</v>
@@ -1956,7 +1963,7 @@
         <v>3.333333333333333</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="N6" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1965,7 +1972,7 @@
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>8</v>
@@ -1986,13 +1993,13 @@
         <v>4</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="K7" s="8">
         <v>6</v>
@@ -2002,7 +2009,7 @@
         <v>2.25</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N7" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2011,7 +2018,7 @@
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -2032,13 +2039,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K8" s="8">
         <v>7</v>
@@ -2048,7 +2055,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="N8" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K8,K$9:K$15,0))</f>
@@ -2057,10 +2064,10 @@
     </row>
     <row r="9" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="14">
         <v>5</v>
@@ -2077,14 +2084,14 @@
       <c r="G9" s="14">
         <v>3</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>53</v>
+      <c r="H9" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="K9" s="14">
         <v>7</v>
@@ -2094,7 +2101,7 @@
         <v>5.416666666666667</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="N9" s="13" t="str">
         <f>INDEX(A$2:A$8,MATCH(K9,K$2:K$8,0))</f>
@@ -2106,7 +2113,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="14">
         <v>0</v>
@@ -2124,13 +2131,13 @@
         <v>3</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="K10" s="14">
         <v>1</v>
@@ -2140,7 +2147,7 @@
         <v>2.5</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="N10" s="13" t="str">
         <f t="shared" ref="N10:N15" si="2">INDEX(A$2:A$8,MATCH(K10,K$2:K$8,0))</f>
@@ -2149,10 +2156,10 @@
     </row>
     <row r="11" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="14">
         <v>7</v>
@@ -2170,13 +2177,13 @@
         <v>3</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="K11" s="14">
         <v>2</v>
@@ -2186,7 +2193,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="N11" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2195,10 +2202,10 @@
     </row>
     <row r="12" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="14">
         <v>8</v>
@@ -2216,13 +2223,13 @@
         <v>4</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K12" s="14">
         <v>4</v>
@@ -2232,7 +2239,7 @@
         <v>5.166666666666667</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="N12" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2241,10 +2248,10 @@
     </row>
     <row r="13" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="14">
         <v>6</v>
@@ -2261,14 +2268,14 @@
       <c r="G13" s="14">
         <v>4</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>38</v>
+      <c r="H13" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K13" s="14">
         <v>3</v>
@@ -2278,7 +2285,7 @@
         <v>4.5</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="N13" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2287,10 +2294,10 @@
     </row>
     <row r="14" spans="1:14" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="14">
         <v>8</v>
@@ -2308,13 +2315,13 @@
         <v>4</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="K14" s="14">
         <v>5</v>
@@ -2324,7 +2331,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="N14" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2333,10 +2340,10 @@
     </row>
     <row r="15" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="14">
         <v>5</v>
@@ -2353,14 +2360,14 @@
       <c r="G15" s="14">
         <v>4</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>44</v>
+      <c r="H15" s="33" t="s">
+        <v>125</v>
       </c>
       <c r="I15" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>66</v>
       </c>
       <c r="K15" s="14">
         <v>6</v>
@@ -2370,7 +2377,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="N15" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2388,7 +2395,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,66 +2407,66 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2485,7 +2492,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
@@ -2502,7 +2509,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2528,7 +2535,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <f>SUM(Cards!C9:C15)</f>
@@ -2549,7 +2556,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>
@@ -2570,7 +2577,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B6" s="24">
         <f>B3/SUM($B3:$D3)</f>
@@ -2587,7 +2594,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B7" s="24">
         <f>B4/SUM($B4:$D4)</f>
@@ -2604,7 +2611,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B8" s="24">
         <f>B5/SUM($B5:$D5)</f>
@@ -2621,7 +2628,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B9" s="24">
         <f>4/9</f>
@@ -2684,34 +2691,34 @@
   <sheetData>
     <row r="1" spans="1:26" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F1" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>112</v>
-      </c>
       <c r="J1" s="27" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>2</v>
@@ -2723,43 +2730,43 @@
         <v>4</v>
       </c>
       <c r="N1" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="R1" s="25" t="s">
+      <c r="T1" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="U1" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="25" t="s">
+      <c r="X1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="25" t="s">
-        <v>28</v>
-      </c>
       <c r="Y1" s="25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="Z1" s="31" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -2817,7 +2824,7 @@
         <v>2.5</v>
       </c>
       <c r="Z2" s="30" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -2834,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>5</v>
@@ -2845,7 +2852,7 @@
       </c>
       <c r="J3" s="26" t="e">
         <f t="array" ref="J3">INDEX([1]combat_sim_results!A2:'[1]combat_sim_results'!E10000, MATCH(1, ([1]combat_sim_results!C2:'[1]combat_sim_results'!C10000=H3)*([1]combat_sim_results!D2:'[1]combat_sim_results'!D10000=I3)*([1]combat_sim_results!A2:'[1]combat_sim_results'!A10000=P2)*([1]combat_sim_results!B2:'[1]combat_sim_results'!B10000=O2), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K3" s="26">
         <v>4</v>
@@ -2911,7 +2918,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="29" t="str">
         <f t="shared" ref="G4:G22" si="1">IF(F4="Battle",J4,"")</f>
@@ -2919,7 +2926,7 @@
       </c>
       <c r="J4" s="26" t="e">
         <f t="array" ref="J4">INDEX([1]combat_sim_results!A3:'[1]combat_sim_results'!E10001, MATCH(1, ([1]combat_sim_results!C3:'[1]combat_sim_results'!C10001=H4)*([1]combat_sim_results!D3:'[1]combat_sim_results'!D10001=I4)*([1]combat_sim_results!A3:'[1]combat_sim_results'!A10001=P3)*([1]combat_sim_results!B3:'[1]combat_sim_results'!B10001=O3), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K4" s="26">
         <v>1</v>
@@ -2982,10 +2989,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -2993,7 +3000,7 @@
       </c>
       <c r="J5" s="26" t="e">
         <f t="array" ref="J5">INDEX([1]combat_sim_results!A4:'[1]combat_sim_results'!E10002, MATCH(1, ([1]combat_sim_results!C4:'[1]combat_sim_results'!C10002=H5)*([1]combat_sim_results!D4:'[1]combat_sim_results'!D10002=I5)*([1]combat_sim_results!A4:'[1]combat_sim_results'!A10002=P4)*([1]combat_sim_results!B4:'[1]combat_sim_results'!B10002=O4), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K5" s="26">
         <v>1</v>
@@ -3056,14 +3063,14 @@
         <v>1</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="29" t="e">
+      <c r="G6" s="29">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="H6" s="26">
         <v>14</v>
@@ -3071,9 +3078,9 @@
       <c r="I6" s="26">
         <v>2</v>
       </c>
-      <c r="J6" s="26" t="e">
+      <c r="J6" s="26">
         <f t="array" ref="J6">INDEX([1]combat_sim_results!A5:'[1]combat_sim_results'!E10003, MATCH(1, ([1]combat_sim_results!C5:'[1]combat_sim_results'!C10003=H6)*([1]combat_sim_results!D5:'[1]combat_sim_results'!D10003=I6)*([1]combat_sim_results!A5:'[1]combat_sim_results'!A10003=P5)*([1]combat_sim_results!B5:'[1]combat_sim_results'!B10003=O5), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="K6" s="26">
         <v>6</v>
@@ -3136,7 +3143,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>5</v>
@@ -3147,7 +3154,7 @@
       </c>
       <c r="J7" s="26" t="e">
         <f t="array" ref="J7">INDEX([1]combat_sim_results!A6:'[1]combat_sim_results'!E10004, MATCH(1, ([1]combat_sim_results!C6:'[1]combat_sim_results'!C10004=H7)*([1]combat_sim_results!D6:'[1]combat_sim_results'!D10004=I7)*([1]combat_sim_results!A6:'[1]combat_sim_results'!A10004=P6)*([1]combat_sim_results!B6:'[1]combat_sim_results'!B10004=O6), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K7" s="26">
         <v>6</v>
@@ -3210,10 +3217,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3221,7 +3228,7 @@
       </c>
       <c r="J8" s="26" t="e">
         <f t="array" ref="J8">INDEX([1]combat_sim_results!A7:'[1]combat_sim_results'!E10005, MATCH(1, ([1]combat_sim_results!C7:'[1]combat_sim_results'!C10005=H8)*([1]combat_sim_results!D7:'[1]combat_sim_results'!D10005=I8)*([1]combat_sim_results!A7:'[1]combat_sim_results'!A10005=P7)*([1]combat_sim_results!B7:'[1]combat_sim_results'!B10005=O7), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K8" s="26">
         <v>6</v>
@@ -3284,14 +3291,14 @@
         <v>1</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="29" t="e">
+      <c r="G9" s="29">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="H9" s="26">
         <v>8</v>
@@ -3299,9 +3306,9 @@
       <c r="I9" s="26">
         <v>4</v>
       </c>
-      <c r="J9" s="26" t="e">
+      <c r="J9" s="26">
         <f t="array" ref="J9">INDEX([1]combat_sim_results!A8:'[1]combat_sim_results'!E10006, MATCH(1, ([1]combat_sim_results!C8:'[1]combat_sim_results'!C10006=H9)*([1]combat_sim_results!D8:'[1]combat_sim_results'!D10006=I9)*([1]combat_sim_results!A8:'[1]combat_sim_results'!A10006=P8)*([1]combat_sim_results!B8:'[1]combat_sim_results'!B10006=O8), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="K9" s="26">
         <v>13</v>
@@ -3364,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>5</v>
@@ -3375,7 +3382,7 @@
       </c>
       <c r="J10" s="26" t="e">
         <f t="array" ref="J10">INDEX([1]combat_sim_results!A9:'[1]combat_sim_results'!E10007, MATCH(1, ([1]combat_sim_results!C9:'[1]combat_sim_results'!C10007=H10)*([1]combat_sim_results!D9:'[1]combat_sim_results'!D10007=I10)*([1]combat_sim_results!A9:'[1]combat_sim_results'!A10007=P9)*([1]combat_sim_results!B9:'[1]combat_sim_results'!B10007=O9), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K10" s="26">
         <v>9</v>
@@ -3438,7 +3445,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F11" s="26" t="s">
         <v>5</v>
@@ -3449,7 +3456,7 @@
       </c>
       <c r="J11" s="26" t="e">
         <f t="array" ref="J11">INDEX([1]combat_sim_results!A10:'[1]combat_sim_results'!E10008, MATCH(1, ([1]combat_sim_results!C10:'[1]combat_sim_results'!C10008=H11)*([1]combat_sim_results!D10:'[1]combat_sim_results'!D10008=I11)*([1]combat_sim_results!A10:'[1]combat_sim_results'!A10008=P10)*([1]combat_sim_results!B10:'[1]combat_sim_results'!B10008=O10), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K11" s="26">
         <v>7</v>
@@ -3512,7 +3519,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="26" t="s">
         <v>5</v>
@@ -3523,7 +3530,7 @@
       </c>
       <c r="J12" s="26" t="e">
         <f t="array" ref="J12">INDEX([1]combat_sim_results!A11:'[1]combat_sim_results'!E10009, MATCH(1, ([1]combat_sim_results!C11:'[1]combat_sim_results'!C10009=H12)*([1]combat_sim_results!D11:'[1]combat_sim_results'!D10009=I12)*([1]combat_sim_results!A11:'[1]combat_sim_results'!A10009=P11)*([1]combat_sim_results!B11:'[1]combat_sim_results'!B10009=O11), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K12" s="26">
         <v>9</v>
@@ -3586,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>5</v>
@@ -3597,7 +3604,7 @@
       </c>
       <c r="J13" s="26" t="e">
         <f t="array" ref="J13">INDEX([1]combat_sim_results!A12:'[1]combat_sim_results'!E10010, MATCH(1, ([1]combat_sim_results!C12:'[1]combat_sim_results'!C10010=H13)*([1]combat_sim_results!D12:'[1]combat_sim_results'!D10010=I13)*([1]combat_sim_results!A12:'[1]combat_sim_results'!A10010=P12)*([1]combat_sim_results!B12:'[1]combat_sim_results'!B10010=O12), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K13" s="26">
         <v>6</v>
@@ -3660,7 +3667,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F14" s="26" t="s">
         <v>5</v>
@@ -3671,7 +3678,7 @@
       </c>
       <c r="J14" s="26" t="e">
         <f t="array" ref="J14">INDEX([1]combat_sim_results!A13:'[1]combat_sim_results'!E10011, MATCH(1, ([1]combat_sim_results!C13:'[1]combat_sim_results'!C10011=H14)*([1]combat_sim_results!D13:'[1]combat_sim_results'!D10011=I14)*([1]combat_sim_results!A13:'[1]combat_sim_results'!A10011=P13)*([1]combat_sim_results!B13:'[1]combat_sim_results'!B10011=O13), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K14" s="26">
         <v>2</v>
@@ -3739,9 +3746,9 @@
       <c r="F15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="29" t="e">
+      <c r="G15" s="29">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="H15" s="26">
         <v>12</v>
@@ -3749,9 +3756,9 @@
       <c r="I15" s="26">
         <v>2</v>
       </c>
-      <c r="J15" s="26" t="e">
+      <c r="J15" s="26">
         <f t="array" ref="J15">INDEX([1]combat_sim_results!A14:'[1]combat_sim_results'!E10012, MATCH(1, ([1]combat_sim_results!C14:'[1]combat_sim_results'!C10012=H15)*([1]combat_sim_results!D14:'[1]combat_sim_results'!D10012=I15)*([1]combat_sim_results!A14:'[1]combat_sim_results'!A10012=P14)*([1]combat_sim_results!B14:'[1]combat_sim_results'!B10012=O14), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="K15" s="26">
         <v>9</v>
@@ -3814,10 +3821,10 @@
         <v>2</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="29" t="str">
         <f t="shared" si="1"/>
@@ -3825,7 +3832,7 @@
       </c>
       <c r="J16" s="26" t="e">
         <f t="array" ref="J16">INDEX([1]combat_sim_results!A15:'[1]combat_sim_results'!E10013, MATCH(1, ([1]combat_sim_results!C15:'[1]combat_sim_results'!C10013=H16)*([1]combat_sim_results!D15:'[1]combat_sim_results'!D10013=I16)*([1]combat_sim_results!A15:'[1]combat_sim_results'!A10013=P15)*([1]combat_sim_results!B15:'[1]combat_sim_results'!B10013=O15), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K16" s="26">
         <v>9</v>
@@ -3888,14 +3895,14 @@
         <v>3</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="29" t="e">
+      <c r="G17" s="29">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="H17" s="26">
         <v>11</v>
@@ -3903,9 +3910,9 @@
       <c r="I17" s="26">
         <v>4</v>
       </c>
-      <c r="J17" s="26" t="e">
+      <c r="J17" s="26">
         <f t="array" ref="J17">INDEX([1]combat_sim_results!A16:'[1]combat_sim_results'!E10014, MATCH(1, ([1]combat_sim_results!C16:'[1]combat_sim_results'!C10014=H17)*([1]combat_sim_results!D16:'[1]combat_sim_results'!D10014=I17)*([1]combat_sim_results!A16:'[1]combat_sim_results'!A10014=P16)*([1]combat_sim_results!B16:'[1]combat_sim_results'!B10014=O16), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="K17" s="26">
         <v>14</v>
@@ -3954,7 +3961,7 @@
         <v>7.5</v>
       </c>
       <c r="Z17" s="30" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -3971,7 +3978,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>5</v>
@@ -3982,7 +3989,7 @@
       </c>
       <c r="J18" s="26" t="e">
         <f t="array" ref="J18">INDEX([1]combat_sim_results!A17:'[1]combat_sim_results'!E10015, MATCH(1, ([1]combat_sim_results!C17:'[1]combat_sim_results'!C10015=H18)*([1]combat_sim_results!D17:'[1]combat_sim_results'!D10015=I18)*([1]combat_sim_results!A17:'[1]combat_sim_results'!A10015=P17)*([1]combat_sim_results!B17:'[1]combat_sim_results'!B10015=O17), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K18" s="26">
         <v>6</v>
@@ -4045,7 +4052,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>5</v>
@@ -4056,7 +4063,7 @@
       </c>
       <c r="J19" s="26" t="e">
         <f t="array" ref="J19">INDEX([1]combat_sim_results!A18:'[1]combat_sim_results'!E10016, MATCH(1, ([1]combat_sim_results!C18:'[1]combat_sim_results'!C10016=H19)*([1]combat_sim_results!D18:'[1]combat_sim_results'!D10016=I19)*([1]combat_sim_results!A18:'[1]combat_sim_results'!A10016=P18)*([1]combat_sim_results!B18:'[1]combat_sim_results'!B10016=O18), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K19" s="26">
         <v>6</v>
@@ -4119,7 +4126,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>5</v>
@@ -4130,7 +4137,7 @@
       </c>
       <c r="J20" s="26" t="e">
         <f t="array" ref="J20">INDEX([1]combat_sim_results!A19:'[1]combat_sim_results'!E10017, MATCH(1, ([1]combat_sim_results!C19:'[1]combat_sim_results'!C10017=H20)*([1]combat_sim_results!D19:'[1]combat_sim_results'!D10017=I20)*([1]combat_sim_results!A19:'[1]combat_sim_results'!A10017=P19)*([1]combat_sim_results!B19:'[1]combat_sim_results'!B10017=O19), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K20" s="26">
         <v>6</v>
@@ -4193,7 +4200,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>6</v>
@@ -4258,7 +4265,7 @@
         <v>9.25</v>
       </c>
       <c r="Z21" s="30" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -4280,7 +4287,7 @@
       </c>
       <c r="J22" s="26" t="e">
         <f t="array" ref="J22">INDEX([1]combat_sim_results!A21:'[1]combat_sim_results'!E10019, MATCH(1, ([1]combat_sim_results!C21:'[1]combat_sim_results'!C10019=H22)*([1]combat_sim_results!D21:'[1]combat_sim_results'!D10019=I22)*([1]combat_sim_results!A21:'[1]combat_sim_results'!A10019=P21)*([1]combat_sim_results!B21:'[1]combat_sim_results'!B10019=O21), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="Y22" s="26">
         <f t="shared" si="0"/>
@@ -4304,9 +4311,9 @@
         <f t="shared" ref="G23:G52" si="2">IF(F23="Battle",J23,"")</f>
         <v/>
       </c>
-      <c r="J23" s="26" t="e">
+      <c r="J23" s="26">
         <f t="array" ref="J23">INDEX([1]combat_sim_results!A22:'[1]combat_sim_results'!E10020, MATCH(1, ([1]combat_sim_results!C22:'[1]combat_sim_results'!C10020=H23)*([1]combat_sim_results!D22:'[1]combat_sim_results'!D10020=I23)*([1]combat_sim_results!A22:'[1]combat_sim_results'!A10020=P22)*([1]combat_sim_results!B22:'[1]combat_sim_results'!B10020=O22), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="26">
         <f t="shared" si="0"/>
@@ -4330,9 +4337,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J24" s="26" t="e">
+      <c r="J24" s="26">
         <f t="array" ref="J24">INDEX([1]combat_sim_results!A23:'[1]combat_sim_results'!E10021, MATCH(1, ([1]combat_sim_results!C23:'[1]combat_sim_results'!C10021=H24)*([1]combat_sim_results!D23:'[1]combat_sim_results'!D10021=I24)*([1]combat_sim_results!A23:'[1]combat_sim_results'!A10021=P23)*([1]combat_sim_results!B23:'[1]combat_sim_results'!B10021=O23), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="26">
         <f t="shared" si="0"/>
@@ -4356,9 +4363,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J25" s="26" t="e">
+      <c r="J25" s="26">
         <f t="array" ref="J25">INDEX([1]combat_sim_results!A24:'[1]combat_sim_results'!E10022, MATCH(1, ([1]combat_sim_results!C24:'[1]combat_sim_results'!C10022=H25)*([1]combat_sim_results!D24:'[1]combat_sim_results'!D10022=I25)*([1]combat_sim_results!A24:'[1]combat_sim_results'!A10022=P24)*([1]combat_sim_results!B24:'[1]combat_sim_results'!B10022=O24), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y25" s="26">
         <f t="shared" si="0"/>
@@ -4382,9 +4389,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J26" s="26" t="e">
+      <c r="J26" s="26">
         <f t="array" ref="J26">INDEX([1]combat_sim_results!A25:'[1]combat_sim_results'!E10023, MATCH(1, ([1]combat_sim_results!C25:'[1]combat_sim_results'!C10023=H26)*([1]combat_sim_results!D25:'[1]combat_sim_results'!D10023=I26)*([1]combat_sim_results!A25:'[1]combat_sim_results'!A10023=P25)*([1]combat_sim_results!B25:'[1]combat_sim_results'!B10023=O25), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="26">
         <f t="shared" si="0"/>
@@ -4396,9 +4403,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J27" s="26" t="e">
+      <c r="J27" s="26">
         <f t="array" ref="J27">INDEX([1]combat_sim_results!A26:'[1]combat_sim_results'!E10024, MATCH(1, ([1]combat_sim_results!C26:'[1]combat_sim_results'!C10024=H27)*([1]combat_sim_results!D26:'[1]combat_sim_results'!D10024=I27)*([1]combat_sim_results!A26:'[1]combat_sim_results'!A10024=P26)*([1]combat_sim_results!B26:'[1]combat_sim_results'!B10024=O26), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -4406,9 +4413,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J28" s="26" t="e">
+      <c r="J28" s="26">
         <f t="array" ref="J28">INDEX([1]combat_sim_results!A27:'[1]combat_sim_results'!E10025, MATCH(1, ([1]combat_sim_results!C27:'[1]combat_sim_results'!C10025=H28)*([1]combat_sim_results!D27:'[1]combat_sim_results'!D10025=I28)*([1]combat_sim_results!A27:'[1]combat_sim_results'!A10025=P27)*([1]combat_sim_results!B27:'[1]combat_sim_results'!B10025=O27), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="K28" s="26">
         <v>4</v>
@@ -4457,7 +4464,7 @@
         <v>2.5</v>
       </c>
       <c r="Z28" s="30" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -4468,7 +4475,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F29" s="26" t="s">
         <v>5</v>
@@ -4479,7 +4486,7 @@
       </c>
       <c r="J29" s="26" t="e">
         <f t="array" ref="J29">INDEX([1]combat_sim_results!A28:'[1]combat_sim_results'!E10026, MATCH(1, ([1]combat_sim_results!C28:'[1]combat_sim_results'!C10026=H29)*([1]combat_sim_results!D28:'[1]combat_sim_results'!D10026=I29)*([1]combat_sim_results!A28:'[1]combat_sim_results'!A10026=P28)*([1]combat_sim_results!B28:'[1]combat_sim_results'!B10026=O28), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K29" s="26">
         <v>0</v>
@@ -4547,7 +4554,7 @@
       </c>
       <c r="J30" s="26" t="e">
         <f t="array" ref="J30">INDEX([1]combat_sim_results!A29:'[1]combat_sim_results'!E10027, MATCH(1, ([1]combat_sim_results!C29:'[1]combat_sim_results'!C10027=H30)*([1]combat_sim_results!D29:'[1]combat_sim_results'!D10027=I30)*([1]combat_sim_results!A29:'[1]combat_sim_results'!A10027=P29)*([1]combat_sim_results!B29:'[1]combat_sim_results'!B10027=O29), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K30" s="26">
         <v>3</v>
@@ -4604,10 +4611,10 @@
         <v>3</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" s="29" t="str">
         <f t="shared" si="2"/>
@@ -4615,7 +4622,7 @@
       </c>
       <c r="J31" s="26" t="e">
         <f t="array" ref="J31">INDEX([1]combat_sim_results!A30:'[1]combat_sim_results'!E10028, MATCH(1, ([1]combat_sim_results!C30:'[1]combat_sim_results'!C10028=H31)*([1]combat_sim_results!D30:'[1]combat_sim_results'!D10028=I31)*([1]combat_sim_results!A30:'[1]combat_sim_results'!A10028=P30)*([1]combat_sim_results!B30:'[1]combat_sim_results'!B10028=O30), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K31" s="26">
         <v>3</v>
@@ -4672,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>5</v>
@@ -4683,7 +4690,7 @@
       </c>
       <c r="J32" s="26" t="e">
         <f t="array" ref="J32">INDEX([1]combat_sim_results!A31:'[1]combat_sim_results'!E10029, MATCH(1, ([1]combat_sim_results!C31:'[1]combat_sim_results'!C10029=H32)*([1]combat_sim_results!D31:'[1]combat_sim_results'!D10029=I32)*([1]combat_sim_results!A31:'[1]combat_sim_results'!A10029=P31)*([1]combat_sim_results!B31:'[1]combat_sim_results'!B10029=O31), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K32" s="26">
         <v>1</v>
@@ -4740,10 +4747,10 @@
         <v>2</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G33" s="29" t="str">
         <f t="shared" si="2"/>
@@ -4751,7 +4758,7 @@
       </c>
       <c r="J33" s="26" t="e">
         <f t="array" ref="J33">INDEX([1]combat_sim_results!A32:'[1]combat_sim_results'!E10030, MATCH(1, ([1]combat_sim_results!C32:'[1]combat_sim_results'!C10030=H33)*([1]combat_sim_results!D32:'[1]combat_sim_results'!D10030=I33)*([1]combat_sim_results!A32:'[1]combat_sim_results'!A10030=P32)*([1]combat_sim_results!B32:'[1]combat_sim_results'!B10030=O32), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K33" s="26">
         <v>1</v>
@@ -4808,10 +4815,10 @@
         <v>3</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G34" s="29" t="str">
         <f t="shared" si="2"/>
@@ -4823,9 +4830,9 @@
       <c r="I34" s="26">
         <v>2</v>
       </c>
-      <c r="J34" s="26" t="e">
+      <c r="J34" s="26">
         <f t="array" ref="J34">INDEX([1]combat_sim_results!A33:'[1]combat_sim_results'!E10031, MATCH(1, ([1]combat_sim_results!C33:'[1]combat_sim_results'!C10031=H34)*([1]combat_sim_results!D33:'[1]combat_sim_results'!D10031=I34)*([1]combat_sim_results!A33:'[1]combat_sim_results'!A10031=P33)*([1]combat_sim_results!B33:'[1]combat_sim_results'!B10031=O33), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="K34" s="26">
         <v>3</v>
@@ -4882,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F35" s="26" t="s">
         <v>5</v>
@@ -4893,7 +4900,7 @@
       </c>
       <c r="J35" s="26" t="e">
         <f t="array" ref="J35">INDEX([1]combat_sim_results!A34:'[1]combat_sim_results'!E10032, MATCH(1, ([1]combat_sim_results!C34:'[1]combat_sim_results'!C10032=H35)*([1]combat_sim_results!D34:'[1]combat_sim_results'!D10032=I35)*([1]combat_sim_results!A34:'[1]combat_sim_results'!A10032=P34)*([1]combat_sim_results!B34:'[1]combat_sim_results'!B10032=O34), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K35" s="26">
         <v>1</v>
@@ -4950,14 +4957,14 @@
         <v>2</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="29" t="e">
+      <c r="G36" s="29">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="H36" s="26">
         <v>10</v>
@@ -4965,9 +4972,9 @@
       <c r="I36" s="26">
         <v>3</v>
       </c>
-      <c r="J36" s="26" t="e">
+      <c r="J36" s="26">
         <f t="array" ref="J36">INDEX([1]combat_sim_results!A35:'[1]combat_sim_results'!E10033, MATCH(1, ([1]combat_sim_results!C35:'[1]combat_sim_results'!C10033=H36)*([1]combat_sim_results!D35:'[1]combat_sim_results'!D10033=I36)*([1]combat_sim_results!A35:'[1]combat_sim_results'!A10033=P35)*([1]combat_sim_results!B35:'[1]combat_sim_results'!B10033=O35), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="K36" s="26">
         <v>5</v>
@@ -5016,7 +5023,7 @@
         <v>5.75</v>
       </c>
       <c r="Z36" s="30" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="3:26" x14ac:dyDescent="0.25">
@@ -5027,10 +5034,10 @@
         <v>3</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G37" s="29" t="str">
         <f t="shared" si="2"/>
@@ -5038,7 +5045,7 @@
       </c>
       <c r="J37" s="26" t="e">
         <f t="array" ref="J37">INDEX([1]combat_sim_results!A36:'[1]combat_sim_results'!E10034, MATCH(1, ([1]combat_sim_results!C36:'[1]combat_sim_results'!C10034=H37)*([1]combat_sim_results!D36:'[1]combat_sim_results'!D10034=I37)*([1]combat_sim_results!A36:'[1]combat_sim_results'!A10034=P36)*([1]combat_sim_results!B36:'[1]combat_sim_results'!B10034=O36), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K37" s="26">
         <v>3</v>
@@ -5095,7 +5102,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="26" t="s">
         <v>5</v>
@@ -5106,7 +5113,7 @@
       </c>
       <c r="J38" s="26" t="e">
         <f t="array" ref="J38">INDEX([1]combat_sim_results!A37:'[1]combat_sim_results'!E10035, MATCH(1, ([1]combat_sim_results!C37:'[1]combat_sim_results'!C10035=H38)*([1]combat_sim_results!D37:'[1]combat_sim_results'!D10035=I38)*([1]combat_sim_results!A37:'[1]combat_sim_results'!A10035=P37)*([1]combat_sim_results!B37:'[1]combat_sim_results'!B10035=O37), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K38" s="26">
         <v>5</v>
@@ -5163,10 +5170,10 @@
         <v>2</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G39" s="29" t="str">
         <f t="shared" si="2"/>
@@ -5174,7 +5181,7 @@
       </c>
       <c r="J39" s="26" t="e">
         <f t="array" ref="J39">INDEX([1]combat_sim_results!A38:'[1]combat_sim_results'!E10036, MATCH(1, ([1]combat_sim_results!C38:'[1]combat_sim_results'!C10036=H39)*([1]combat_sim_results!D38:'[1]combat_sim_results'!D10036=I39)*([1]combat_sim_results!A38:'[1]combat_sim_results'!A10036=P38)*([1]combat_sim_results!B38:'[1]combat_sim_results'!B10036=O38), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K39" s="26">
         <v>5</v>
@@ -5231,7 +5238,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40" s="26" t="s">
         <v>5</v>
@@ -5242,7 +5249,7 @@
       </c>
       <c r="J40" s="26" t="e">
         <f t="array" ref="J40">INDEX([1]combat_sim_results!A39:'[1]combat_sim_results'!E10037, MATCH(1, ([1]combat_sim_results!C39:'[1]combat_sim_results'!C10037=H40)*([1]combat_sim_results!D39:'[1]combat_sim_results'!D10037=I40)*([1]combat_sim_results!A39:'[1]combat_sim_results'!A10037=P39)*([1]combat_sim_results!B39:'[1]combat_sim_results'!B10037=O39), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K40" s="26">
         <v>1</v>
@@ -5299,10 +5306,10 @@
         <v>1</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G41" s="29" t="str">
         <f t="shared" si="2"/>
@@ -5310,7 +5317,7 @@
       </c>
       <c r="J41" s="26" t="e">
         <f t="array" ref="J41">INDEX([1]combat_sim_results!A40:'[1]combat_sim_results'!E10038, MATCH(1, ([1]combat_sim_results!C40:'[1]combat_sim_results'!C10038=H41)*([1]combat_sim_results!D40:'[1]combat_sim_results'!D10038=I41)*([1]combat_sim_results!A40:'[1]combat_sim_results'!A10038=P40)*([1]combat_sim_results!B40:'[1]combat_sim_results'!B10038=O40), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K41" s="26">
         <v>1</v>
@@ -5367,14 +5374,14 @@
         <v>2</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F42" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="29" t="e">
+      <c r="G42" s="29">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="H42" s="26">
         <v>8</v>
@@ -5382,9 +5389,9 @@
       <c r="I42" s="26">
         <v>4</v>
       </c>
-      <c r="J42" s="26" t="e">
+      <c r="J42" s="26">
         <f t="array" ref="J42">INDEX([1]combat_sim_results!A41:'[1]combat_sim_results'!E10039, MATCH(1, ([1]combat_sim_results!C41:'[1]combat_sim_results'!C10039=H42)*([1]combat_sim_results!D41:'[1]combat_sim_results'!D10039=I42)*([1]combat_sim_results!A41:'[1]combat_sim_results'!A10039=P41)*([1]combat_sim_results!B41:'[1]combat_sim_results'!B10039=O41), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="K42" s="26">
         <v>6</v>
@@ -5433,7 +5440,7 @@
         <v>4.6666666666666661</v>
       </c>
       <c r="Z42" s="30" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
@@ -5452,7 +5459,7 @@
       </c>
       <c r="J43" s="26" t="e">
         <f t="array" ref="J43">INDEX([1]combat_sim_results!A42:'[1]combat_sim_results'!E10040, MATCH(1, ([1]combat_sim_results!C42:'[1]combat_sim_results'!C10040=H43)*([1]combat_sim_results!D42:'[1]combat_sim_results'!D10040=I43)*([1]combat_sim_results!A42:'[1]combat_sim_results'!A10040=P42)*([1]combat_sim_results!B42:'[1]combat_sim_results'!B10040=O42), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K43" s="26">
         <v>6</v>
@@ -5509,7 +5516,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F44" s="26" t="s">
         <v>5</v>
@@ -5520,7 +5527,7 @@
       </c>
       <c r="J44" s="26" t="e">
         <f t="array" ref="J44">INDEX([1]combat_sim_results!A43:'[1]combat_sim_results'!E10041, MATCH(1, ([1]combat_sim_results!C43:'[1]combat_sim_results'!C10041=H44)*([1]combat_sim_results!D43:'[1]combat_sim_results'!D10041=I44)*([1]combat_sim_results!A43:'[1]combat_sim_results'!A10041=P43)*([1]combat_sim_results!B43:'[1]combat_sim_results'!B10041=O43), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K44" s="26">
         <v>6</v>
@@ -5577,7 +5584,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F45" s="26" t="s">
         <v>5</v>
@@ -5588,7 +5595,7 @@
       </c>
       <c r="J45" s="26" t="e">
         <f t="array" ref="J45">INDEX([1]combat_sim_results!A44:'[1]combat_sim_results'!E10042, MATCH(1, ([1]combat_sim_results!C44:'[1]combat_sim_results'!C10042=H45)*([1]combat_sim_results!D44:'[1]combat_sim_results'!D10042=I45)*([1]combat_sim_results!A44:'[1]combat_sim_results'!A10042=P44)*([1]combat_sim_results!B44:'[1]combat_sim_results'!B10042=O44), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K45" s="26">
         <v>6</v>
@@ -5637,7 +5644,7 @@
         <v>7.666666666666667</v>
       </c>
       <c r="Z45" s="30" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.25">
@@ -5648,7 +5655,7 @@
         <v>3</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" s="26" t="s">
         <v>5</v>
@@ -5659,7 +5666,7 @@
       </c>
       <c r="J46" s="26" t="e">
         <f t="array" ref="J46">INDEX([1]combat_sim_results!A45:'[1]combat_sim_results'!E10043, MATCH(1, ([1]combat_sim_results!C45:'[1]combat_sim_results'!C10043=H46)*([1]combat_sim_results!D45:'[1]combat_sim_results'!D10043=I46)*([1]combat_sim_results!A45:'[1]combat_sim_results'!A10043=P45)*([1]combat_sim_results!B45:'[1]combat_sim_results'!B10043=O45), 0),5)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="K46" s="26">
         <v>6</v>
@@ -5716,14 +5723,14 @@
         <v>1</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F47" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="29" t="e">
+      <c r="G47" s="29">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="H47" s="26">
         <v>11</v>
@@ -5731,9 +5738,9 @@
       <c r="I47" s="26">
         <v>4</v>
       </c>
-      <c r="J47" s="26" t="e">
+      <c r="J47" s="26">
         <f t="array" ref="J47">INDEX([1]combat_sim_results!A46:'[1]combat_sim_results'!E10044, MATCH(1, ([1]combat_sim_results!C46:'[1]combat_sim_results'!C10044=H47)*([1]combat_sim_results!D46:'[1]combat_sim_results'!D10044=I47)*([1]combat_sim_results!A46:'[1]combat_sim_results'!A10044=P46)*([1]combat_sim_results!B46:'[1]combat_sim_results'!B10044=O46), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="K47" s="26">
         <v>7</v>
@@ -5782,7 +5789,7 @@
         <v>8.9166666666666661</v>
       </c>
       <c r="Z47" s="30" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="3:26" x14ac:dyDescent="0.25">
@@ -5793,14 +5800,14 @@
         <v>2</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="29" t="e">
+      <c r="G48" s="29">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="H48" s="26">
         <v>15</v>
@@ -5808,16 +5815,16 @@
       <c r="I48" s="26">
         <v>4</v>
       </c>
-      <c r="J48" s="26" t="e">
+      <c r="J48" s="26">
         <f t="array" ref="J48">INDEX([1]combat_sim_results!A47:'[1]combat_sim_results'!E10045, MATCH(1, ([1]combat_sim_results!C47:'[1]combat_sim_results'!C10045=H48)*([1]combat_sim_results!D47:'[1]combat_sim_results'!D10045=I48)*([1]combat_sim_results!A47:'[1]combat_sim_results'!A10045=P47)*([1]combat_sim_results!B47:'[1]combat_sim_results'!B10045=O47), 0),5)</f>
-        <v>#REF!</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="Y48" s="26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z48" s="30" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="3:25" x14ac:dyDescent="0.25">
@@ -5831,9 +5838,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J49" s="26" t="e">
+      <c r="J49" s="26">
         <f t="array" ref="J49">INDEX([1]combat_sim_results!A48:'[1]combat_sim_results'!E10046, MATCH(1, ([1]combat_sim_results!C48:'[1]combat_sim_results'!C10046=H49)*([1]combat_sim_results!D48:'[1]combat_sim_results'!D10046=I49)*([1]combat_sim_results!A48:'[1]combat_sim_results'!A10046=P48)*([1]combat_sim_results!B48:'[1]combat_sim_results'!B10046=O48), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y49" s="26">
         <f t="shared" si="3"/>
@@ -5851,9 +5858,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J50" s="26" t="e">
+      <c r="J50" s="26">
         <f t="array" ref="J50">INDEX([1]combat_sim_results!A49:'[1]combat_sim_results'!E10047, MATCH(1, ([1]combat_sim_results!C49:'[1]combat_sim_results'!C10047=H50)*([1]combat_sim_results!D49:'[1]combat_sim_results'!D10047=I50)*([1]combat_sim_results!A49:'[1]combat_sim_results'!A10047=P49)*([1]combat_sim_results!B49:'[1]combat_sim_results'!B10047=O49), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y50" s="26">
         <f t="shared" si="3"/>
@@ -5871,9 +5878,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J51" s="26" t="e">
+      <c r="J51" s="26">
         <f t="array" ref="J51">INDEX([1]combat_sim_results!A50:'[1]combat_sim_results'!E10048, MATCH(1, ([1]combat_sim_results!C50:'[1]combat_sim_results'!C10048=H51)*([1]combat_sim_results!D50:'[1]combat_sim_results'!D10048=I51)*([1]combat_sim_results!A50:'[1]combat_sim_results'!A10048=P50)*([1]combat_sim_results!B50:'[1]combat_sim_results'!B10048=O50), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y51" s="26">
         <f t="shared" si="3"/>
@@ -5891,9 +5898,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J52" s="26" t="e">
+      <c r="J52" s="26">
         <f t="array" ref="J52">INDEX([1]combat_sim_results!A51:'[1]combat_sim_results'!E10049, MATCH(1, ([1]combat_sim_results!C51:'[1]combat_sim_results'!C10049=H52)*([1]combat_sim_results!D51:'[1]combat_sim_results'!D10049=I52)*([1]combat_sim_results!A51:'[1]combat_sim_results'!A10049=P51)*([1]combat_sim_results!B51:'[1]combat_sim_results'!B10049=O51), 0),5)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="Y52" s="26">
         <f t="shared" si="3"/>
@@ -5939,7 +5946,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5949,7 +5956,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
balance: oil rag is cheaper, tool effects stack
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -401,10 +401,6 @@
     <t>l</t>
   </si>
   <si>
-    <t>Oil Rag
-for 3 Fabric</t>
-  </si>
-  <si>
     <t>2:2 Metal:Fabric</t>
   </si>
   <si>
@@ -444,6 +440,10 @@
   </si>
   <si>
     <t>+1 ATK for -1 Carry</t>
+  </si>
+  <si>
+    <t>Oil Rag
+for 2 Fabric</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1674,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1815,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K3" s="8">
         <v>2</v>
@@ -1861,7 +1861,7 @@
         <v>41</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K4" s="8">
         <v>3</v>
@@ -1904,7 +1904,7 @@
         <v>65</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>68</v>
@@ -1950,7 +1950,7 @@
         <v>25</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="J6" s="23" t="s">
         <v>84</v>
@@ -2039,13 +2039,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K8" s="8">
         <v>7</v>
@@ -2085,10 +2085,10 @@
         <v>3</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>69</v>
@@ -2183,7 +2183,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K11" s="14">
         <v>2</v>
@@ -2269,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>36</v>
@@ -2361,13 +2361,13 @@
         <v>4</v>
       </c>
       <c r="H15" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>113</v>
-      </c>
       <c r="J15" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K15" s="14">
         <v>6</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Disassemble --> Ditch for The Crusher
I never documented Disassemble, so I'm going to assume I meant Ditch.

Made other adjustments too
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -167,9 +167,6 @@
     <t>+1 ATK for 4 Metal</t>
   </si>
   <si>
-    <t xml:space="preserve">+2 Duct Tape for Disassembling 1 Tool </t>
-  </si>
-  <si>
     <t>Bandages
 for 1 Fabric, 1 Duct Tape</t>
   </si>
@@ -444,6 +441,9 @@
   <si>
     <t>Oil Rag
 for 2 Fabric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+2 Duct Tape for Ditching 1 Tool </t>
   </si>
 </sst>
 </file>
@@ -621,11 +621,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,10 +1713,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -1728,16 +1728,16 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1763,13 +1763,13 @@
         <v>2</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="8">
         <v>1</v>
@@ -1779,7 +1779,7 @@
         <v>1.75</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N2" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K2,K$9:K$15,0))</f>
@@ -1788,7 +1788,7 @@
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -1809,13 +1809,13 @@
         <v>2</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K3" s="8">
         <v>2</v>
@@ -1825,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N3" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K3,K$9:K$15,0))</f>
@@ -1855,13 +1855,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K4" s="8">
         <v>3</v>
@@ -1871,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N4" s="7" t="str">
         <f t="shared" ref="N4:N7" si="1">INDEX(A$9:A$15,MATCH(K4,K$9:K$15,0))</f>
@@ -1901,13 +1901,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" s="8">
         <v>4</v>
@@ -1917,7 +1917,7 @@
         <v>2.25</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N5" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -1950,10 +1950,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="8">
         <v>5</v>
@@ -1963,7 +1963,7 @@
         <v>3.333333333333333</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N6" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1996,10 +1996,10 @@
         <v>35</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K7" s="8">
         <v>6</v>
@@ -2009,7 +2009,7 @@
         <v>2.25</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N7" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -2039,13 +2039,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K8" s="8">
         <v>7</v>
@@ -2055,7 +2055,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N8" s="7" t="str">
         <f>INDEX(A$9:A$15,MATCH(K8,K$9:K$15,0))</f>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="9" spans="1:14" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>12</v>
@@ -2085,13 +2085,13 @@
         <v>3</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" s="14">
         <v>7</v>
@@ -2101,7 +2101,7 @@
         <v>5.416666666666667</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N9" s="13" t="str">
         <f>INDEX(A$2:A$8,MATCH(K9,K$2:K$8,0))</f>
@@ -2134,10 +2134,10 @@
         <v>33</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10" s="14">
         <v>1</v>
@@ -2147,7 +2147,7 @@
         <v>2.5</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N10" s="13" t="str">
         <f t="shared" ref="N10:N15" si="2">INDEX(A$2:A$8,MATCH(K10,K$2:K$8,0))</f>
@@ -2180,10 +2180,10 @@
         <v>39</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="14">
         <v>2</v>
@@ -2193,7 +2193,7 @@
         <v>2.5833333333333335</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N11" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2223,10 +2223,10 @@
         <v>4</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>37</v>
@@ -2239,7 +2239,7 @@
         <v>5.166666666666667</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N12" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="13" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>12</v>
@@ -2269,13 +2269,13 @@
         <v>4</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>36</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K13" s="14">
         <v>3</v>
@@ -2285,7 +2285,7 @@
         <v>4.5</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N13" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2314,14 +2314,14 @@
       <c r="G14" s="14">
         <v>4</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>40</v>
+      <c r="H14" s="32" t="s">
+        <v>125</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K14" s="14">
         <v>5</v>
@@ -2331,7 +2331,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N14" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2360,14 +2360,14 @@
       <c r="G15" s="14">
         <v>4</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="J15" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K15" s="14">
         <v>6</v>
@@ -2377,7 +2377,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N15" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2395,7 +2395,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,7 +2418,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2426,15 +2426,15 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2442,15 +2442,15 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2491,12 +2491,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -2577,7 +2577,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="24">
         <f>B3/SUM($B3:$D3)</f>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="24">
         <f>B4/SUM($B4:$D4)</f>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="24">
         <f>B5/SUM($B5:$D5)</f>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="24">
         <f>4/9</f>
@@ -2691,34 +2691,34 @@
   <sheetData>
     <row r="1" spans="1:26" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>91</v>
-      </c>
       <c r="F1" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G1" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>104</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>105</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>2</v>
@@ -2733,13 +2733,13 @@
         <v>15</v>
       </c>
       <c r="O1" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="27" t="s">
-        <v>95</v>
-      </c>
       <c r="Q1" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R1" s="25" t="s">
         <v>21</v>
@@ -2748,7 +2748,7 @@
         <v>16</v>
       </c>
       <c r="T1" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U1" s="25" t="s">
         <v>20</v>
@@ -2763,10 +2763,10 @@
         <v>27</v>
       </c>
       <c r="Y1" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z1" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
         <v>2.5</v>
       </c>
       <c r="Z2" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="J3" s="26" t="e">
         <f t="array" ref="J3">INDEX([1]combat_sim_results!A2:'[1]combat_sim_results'!E10000, MATCH(1, ([1]combat_sim_results!C2:'[1]combat_sim_results'!C10000=H3)*([1]combat_sim_results!D2:'[1]combat_sim_results'!D10000=I3)*([1]combat_sim_results!A2:'[1]combat_sim_results'!A10000=P2)*([1]combat_sim_results!B2:'[1]combat_sim_results'!B10000=O2), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K3" s="26">
         <v>4</v>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="J4" s="26" t="e">
         <f t="array" ref="J4">INDEX([1]combat_sim_results!A3:'[1]combat_sim_results'!E10001, MATCH(1, ([1]combat_sim_results!C3:'[1]combat_sim_results'!C10001=H4)*([1]combat_sim_results!D3:'[1]combat_sim_results'!D10001=I4)*([1]combat_sim_results!A3:'[1]combat_sim_results'!A10001=P3)*([1]combat_sim_results!B3:'[1]combat_sim_results'!B10001=O3), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K4" s="26">
         <v>1</v>
@@ -2989,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>17</v>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="J5" s="26" t="e">
         <f t="array" ref="J5">INDEX([1]combat_sim_results!A4:'[1]combat_sim_results'!E10002, MATCH(1, ([1]combat_sim_results!C4:'[1]combat_sim_results'!C10002=H5)*([1]combat_sim_results!D4:'[1]combat_sim_results'!D10002=I5)*([1]combat_sim_results!A4:'[1]combat_sim_results'!A10002=P4)*([1]combat_sim_results!B4:'[1]combat_sim_results'!B10002=O4), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K5" s="26">
         <v>1</v>
@@ -3068,9 +3068,9 @@
       <c r="F6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="H6" s="26">
         <v>14</v>
@@ -3078,9 +3078,9 @@
       <c r="I6" s="26">
         <v>2</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="26" t="e">
         <f t="array" ref="J6">INDEX([1]combat_sim_results!A5:'[1]combat_sim_results'!E10003, MATCH(1, ([1]combat_sim_results!C5:'[1]combat_sim_results'!C10003=H6)*([1]combat_sim_results!D5:'[1]combat_sim_results'!D10003=I6)*([1]combat_sim_results!A5:'[1]combat_sim_results'!A10003=P5)*([1]combat_sim_results!B5:'[1]combat_sim_results'!B10003=O5), 0),5)</f>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="K6" s="26">
         <v>6</v>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="J7" s="26" t="e">
         <f t="array" ref="J7">INDEX([1]combat_sim_results!A6:'[1]combat_sim_results'!E10004, MATCH(1, ([1]combat_sim_results!C6:'[1]combat_sim_results'!C10004=H7)*([1]combat_sim_results!D6:'[1]combat_sim_results'!D10004=I7)*([1]combat_sim_results!A6:'[1]combat_sim_results'!A10004=P6)*([1]combat_sim_results!B6:'[1]combat_sim_results'!B10004=O6), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K7" s="26">
         <v>6</v>
@@ -3217,7 +3217,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>17</v>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="J8" s="26" t="e">
         <f t="array" ref="J8">INDEX([1]combat_sim_results!A7:'[1]combat_sim_results'!E10005, MATCH(1, ([1]combat_sim_results!C7:'[1]combat_sim_results'!C10005=H8)*([1]combat_sim_results!D7:'[1]combat_sim_results'!D10005=I8)*([1]combat_sim_results!A7:'[1]combat_sim_results'!A10005=P7)*([1]combat_sim_results!B7:'[1]combat_sim_results'!B10005=O7), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K8" s="26">
         <v>6</v>
@@ -3296,9 +3296,9 @@
       <c r="F9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.88600000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="H9" s="26">
         <v>8</v>
@@ -3306,9 +3306,9 @@
       <c r="I9" s="26">
         <v>4</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="26" t="e">
         <f t="array" ref="J9">INDEX([1]combat_sim_results!A8:'[1]combat_sim_results'!E10006, MATCH(1, ([1]combat_sim_results!C8:'[1]combat_sim_results'!C10006=H9)*([1]combat_sim_results!D8:'[1]combat_sim_results'!D10006=I9)*([1]combat_sim_results!A8:'[1]combat_sim_results'!A10006=P8)*([1]combat_sim_results!B8:'[1]combat_sim_results'!B10006=O8), 0),5)</f>
-        <v>0.88600000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="K9" s="26">
         <v>13</v>
@@ -3371,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>5</v>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="J10" s="26" t="e">
         <f t="array" ref="J10">INDEX([1]combat_sim_results!A9:'[1]combat_sim_results'!E10007, MATCH(1, ([1]combat_sim_results!C9:'[1]combat_sim_results'!C10007=H10)*([1]combat_sim_results!D9:'[1]combat_sim_results'!D10007=I10)*([1]combat_sim_results!A9:'[1]combat_sim_results'!A10007=P9)*([1]combat_sim_results!B9:'[1]combat_sim_results'!B10007=O9), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K10" s="26">
         <v>9</v>
@@ -3445,7 +3445,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="26" t="s">
         <v>5</v>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="J11" s="26" t="e">
         <f t="array" ref="J11">INDEX([1]combat_sim_results!A10:'[1]combat_sim_results'!E10008, MATCH(1, ([1]combat_sim_results!C10:'[1]combat_sim_results'!C10008=H11)*([1]combat_sim_results!D10:'[1]combat_sim_results'!D10008=I11)*([1]combat_sim_results!A10:'[1]combat_sim_results'!A10008=P10)*([1]combat_sim_results!B10:'[1]combat_sim_results'!B10008=O10), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K11" s="26">
         <v>7</v>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="J12" s="26" t="e">
         <f t="array" ref="J12">INDEX([1]combat_sim_results!A11:'[1]combat_sim_results'!E10009, MATCH(1, ([1]combat_sim_results!C11:'[1]combat_sim_results'!C10009=H12)*([1]combat_sim_results!D11:'[1]combat_sim_results'!D10009=I12)*([1]combat_sim_results!A11:'[1]combat_sim_results'!A10009=P11)*([1]combat_sim_results!B11:'[1]combat_sim_results'!B10009=O11), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K12" s="26">
         <v>9</v>
@@ -3593,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>5</v>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="J13" s="26" t="e">
         <f t="array" ref="J13">INDEX([1]combat_sim_results!A12:'[1]combat_sim_results'!E10010, MATCH(1, ([1]combat_sim_results!C12:'[1]combat_sim_results'!C10010=H13)*([1]combat_sim_results!D12:'[1]combat_sim_results'!D10010=I13)*([1]combat_sim_results!A12:'[1]combat_sim_results'!A10010=P12)*([1]combat_sim_results!B12:'[1]combat_sim_results'!B10010=O12), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K13" s="26">
         <v>6</v>
@@ -3667,7 +3667,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="26" t="s">
         <v>5</v>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="J14" s="26" t="e">
         <f t="array" ref="J14">INDEX([1]combat_sim_results!A13:'[1]combat_sim_results'!E10011, MATCH(1, ([1]combat_sim_results!C13:'[1]combat_sim_results'!C10011=H14)*([1]combat_sim_results!D13:'[1]combat_sim_results'!D10011=I14)*([1]combat_sim_results!A13:'[1]combat_sim_results'!A10011=P13)*([1]combat_sim_results!B13:'[1]combat_sim_results'!B10011=O13), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K14" s="26">
         <v>2</v>
@@ -3746,9 +3746,9 @@
       <c r="F15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.98599999999999999</v>
+        <v>#REF!</v>
       </c>
       <c r="H15" s="26">
         <v>12</v>
@@ -3756,9 +3756,9 @@
       <c r="I15" s="26">
         <v>2</v>
       </c>
-      <c r="J15" s="26">
+      <c r="J15" s="26" t="e">
         <f t="array" ref="J15">INDEX([1]combat_sim_results!A14:'[1]combat_sim_results'!E10012, MATCH(1, ([1]combat_sim_results!C14:'[1]combat_sim_results'!C10012=H15)*([1]combat_sim_results!D14:'[1]combat_sim_results'!D10012=I15)*([1]combat_sim_results!A14:'[1]combat_sim_results'!A10012=P14)*([1]combat_sim_results!B14:'[1]combat_sim_results'!B10012=O14), 0),5)</f>
-        <v>0.98599999999999999</v>
+        <v>#REF!</v>
       </c>
       <c r="K15" s="26">
         <v>9</v>
@@ -3832,7 +3832,7 @@
       </c>
       <c r="J16" s="26" t="e">
         <f t="array" ref="J16">INDEX([1]combat_sim_results!A15:'[1]combat_sim_results'!E10013, MATCH(1, ([1]combat_sim_results!C15:'[1]combat_sim_results'!C10013=H16)*([1]combat_sim_results!D15:'[1]combat_sim_results'!D10013=I16)*([1]combat_sim_results!A15:'[1]combat_sim_results'!A10013=P15)*([1]combat_sim_results!B15:'[1]combat_sim_results'!B10013=O15), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K16" s="26">
         <v>9</v>
@@ -3900,9 +3900,9 @@
       <c r="F17" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="29" t="e">
         <f t="shared" si="1"/>
-        <v>0.33400000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="H17" s="26">
         <v>11</v>
@@ -3910,9 +3910,9 @@
       <c r="I17" s="26">
         <v>4</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="26" t="e">
         <f t="array" ref="J17">INDEX([1]combat_sim_results!A16:'[1]combat_sim_results'!E10014, MATCH(1, ([1]combat_sim_results!C16:'[1]combat_sim_results'!C10014=H17)*([1]combat_sim_results!D16:'[1]combat_sim_results'!D10014=I17)*([1]combat_sim_results!A16:'[1]combat_sim_results'!A10014=P16)*([1]combat_sim_results!B16:'[1]combat_sim_results'!B10014=O16), 0),5)</f>
-        <v>0.33400000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="K17" s="26">
         <v>14</v>
@@ -3961,7 +3961,7 @@
         <v>7.5</v>
       </c>
       <c r="Z17" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>5</v>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="J18" s="26" t="e">
         <f t="array" ref="J18">INDEX([1]combat_sim_results!A17:'[1]combat_sim_results'!E10015, MATCH(1, ([1]combat_sim_results!C17:'[1]combat_sim_results'!C10015=H18)*([1]combat_sim_results!D17:'[1]combat_sim_results'!D10015=I18)*([1]combat_sim_results!A17:'[1]combat_sim_results'!A10015=P17)*([1]combat_sim_results!B17:'[1]combat_sim_results'!B10015=O17), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K18" s="26">
         <v>6</v>
@@ -4052,7 +4052,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>5</v>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="J19" s="26" t="e">
         <f t="array" ref="J19">INDEX([1]combat_sim_results!A18:'[1]combat_sim_results'!E10016, MATCH(1, ([1]combat_sim_results!C18:'[1]combat_sim_results'!C10016=H19)*([1]combat_sim_results!D18:'[1]combat_sim_results'!D10016=I19)*([1]combat_sim_results!A18:'[1]combat_sim_results'!A10016=P18)*([1]combat_sim_results!B18:'[1]combat_sim_results'!B10016=O18), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K19" s="26">
         <v>6</v>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="J20" s="26" t="e">
         <f t="array" ref="J20">INDEX([1]combat_sim_results!A19:'[1]combat_sim_results'!E10017, MATCH(1, ([1]combat_sim_results!C19:'[1]combat_sim_results'!C10017=H20)*([1]combat_sim_results!D19:'[1]combat_sim_results'!D10017=I20)*([1]combat_sim_results!A19:'[1]combat_sim_results'!A10017=P19)*([1]combat_sim_results!B19:'[1]combat_sim_results'!B10017=O19), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K20" s="26">
         <v>6</v>
@@ -4200,7 +4200,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>6</v>
@@ -4265,7 +4265,7 @@
         <v>9.25</v>
       </c>
       <c r="Z21" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="J22" s="26" t="e">
         <f t="array" ref="J22">INDEX([1]combat_sim_results!A21:'[1]combat_sim_results'!E10019, MATCH(1, ([1]combat_sim_results!C21:'[1]combat_sim_results'!C10019=H22)*([1]combat_sim_results!D21:'[1]combat_sim_results'!D10019=I22)*([1]combat_sim_results!A21:'[1]combat_sim_results'!A10019=P21)*([1]combat_sim_results!B21:'[1]combat_sim_results'!B10019=O21), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="Y22" s="26">
         <f t="shared" si="0"/>
@@ -4311,9 +4311,9 @@
         <f t="shared" ref="G23:G52" si="2">IF(F23="Battle",J23,"")</f>
         <v/>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="26" t="e">
         <f t="array" ref="J23">INDEX([1]combat_sim_results!A22:'[1]combat_sim_results'!E10020, MATCH(1, ([1]combat_sim_results!C22:'[1]combat_sim_results'!C10020=H23)*([1]combat_sim_results!D22:'[1]combat_sim_results'!D10020=I23)*([1]combat_sim_results!A22:'[1]combat_sim_results'!A10020=P22)*([1]combat_sim_results!B22:'[1]combat_sim_results'!B10020=O22), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y23" s="26">
         <f t="shared" si="0"/>
@@ -4337,9 +4337,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J24" s="26">
+      <c r="J24" s="26" t="e">
         <f t="array" ref="J24">INDEX([1]combat_sim_results!A23:'[1]combat_sim_results'!E10021, MATCH(1, ([1]combat_sim_results!C23:'[1]combat_sim_results'!C10021=H24)*([1]combat_sim_results!D23:'[1]combat_sim_results'!D10021=I24)*([1]combat_sim_results!A23:'[1]combat_sim_results'!A10021=P23)*([1]combat_sim_results!B23:'[1]combat_sim_results'!B10021=O23), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y24" s="26">
         <f t="shared" si="0"/>
@@ -4363,9 +4363,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J25" s="26">
+      <c r="J25" s="26" t="e">
         <f t="array" ref="J25">INDEX([1]combat_sim_results!A24:'[1]combat_sim_results'!E10022, MATCH(1, ([1]combat_sim_results!C24:'[1]combat_sim_results'!C10022=H25)*([1]combat_sim_results!D24:'[1]combat_sim_results'!D10022=I25)*([1]combat_sim_results!A24:'[1]combat_sim_results'!A10022=P24)*([1]combat_sim_results!B24:'[1]combat_sim_results'!B10022=O24), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y25" s="26">
         <f t="shared" si="0"/>
@@ -4389,9 +4389,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J26" s="26">
+      <c r="J26" s="26" t="e">
         <f t="array" ref="J26">INDEX([1]combat_sim_results!A25:'[1]combat_sim_results'!E10023, MATCH(1, ([1]combat_sim_results!C25:'[1]combat_sim_results'!C10023=H26)*([1]combat_sim_results!D25:'[1]combat_sim_results'!D10023=I26)*([1]combat_sim_results!A25:'[1]combat_sim_results'!A10023=P25)*([1]combat_sim_results!B25:'[1]combat_sim_results'!B10023=O25), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y26" s="26">
         <f t="shared" si="0"/>
@@ -4403,9 +4403,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J27" s="26">
+      <c r="J27" s="26" t="e">
         <f t="array" ref="J27">INDEX([1]combat_sim_results!A26:'[1]combat_sim_results'!E10024, MATCH(1, ([1]combat_sim_results!C26:'[1]combat_sim_results'!C10024=H27)*([1]combat_sim_results!D26:'[1]combat_sim_results'!D10024=I27)*([1]combat_sim_results!A26:'[1]combat_sim_results'!A10024=P26)*([1]combat_sim_results!B26:'[1]combat_sim_results'!B10024=O26), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -4413,9 +4413,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="26" t="e">
         <f t="array" ref="J28">INDEX([1]combat_sim_results!A27:'[1]combat_sim_results'!E10025, MATCH(1, ([1]combat_sim_results!C27:'[1]combat_sim_results'!C10025=H28)*([1]combat_sim_results!D27:'[1]combat_sim_results'!D10025=I28)*([1]combat_sim_results!A27:'[1]combat_sim_results'!A10025=P27)*([1]combat_sim_results!B27:'[1]combat_sim_results'!B10025=O27), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="K28" s="26">
         <v>4</v>
@@ -4464,7 +4464,7 @@
         <v>2.5</v>
       </c>
       <c r="Z28" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -4475,7 +4475,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="26" t="s">
         <v>5</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="J29" s="26" t="e">
         <f t="array" ref="J29">INDEX([1]combat_sim_results!A28:'[1]combat_sim_results'!E10026, MATCH(1, ([1]combat_sim_results!C28:'[1]combat_sim_results'!C10026=H29)*([1]combat_sim_results!D28:'[1]combat_sim_results'!D10026=I29)*([1]combat_sim_results!A28:'[1]combat_sim_results'!A10026=P28)*([1]combat_sim_results!B28:'[1]combat_sim_results'!B10026=O28), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K29" s="26">
         <v>0</v>
@@ -4554,7 +4554,7 @@
       </c>
       <c r="J30" s="26" t="e">
         <f t="array" ref="J30">INDEX([1]combat_sim_results!A29:'[1]combat_sim_results'!E10027, MATCH(1, ([1]combat_sim_results!C29:'[1]combat_sim_results'!C10027=H30)*([1]combat_sim_results!D29:'[1]combat_sim_results'!D10027=I30)*([1]combat_sim_results!A29:'[1]combat_sim_results'!A10027=P29)*([1]combat_sim_results!B29:'[1]combat_sim_results'!B10027=O29), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K30" s="26">
         <v>3</v>
@@ -4611,7 +4611,7 @@
         <v>3</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="26" t="s">
         <v>17</v>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="J31" s="26" t="e">
         <f t="array" ref="J31">INDEX([1]combat_sim_results!A30:'[1]combat_sim_results'!E10028, MATCH(1, ([1]combat_sim_results!C30:'[1]combat_sim_results'!C10028=H31)*([1]combat_sim_results!D30:'[1]combat_sim_results'!D10028=I31)*([1]combat_sim_results!A30:'[1]combat_sim_results'!A10028=P30)*([1]combat_sim_results!B30:'[1]combat_sim_results'!B10028=O30), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K31" s="26">
         <v>3</v>
@@ -4679,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>5</v>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="J32" s="26" t="e">
         <f t="array" ref="J32">INDEX([1]combat_sim_results!A31:'[1]combat_sim_results'!E10029, MATCH(1, ([1]combat_sim_results!C31:'[1]combat_sim_results'!C10029=H32)*([1]combat_sim_results!D31:'[1]combat_sim_results'!D10029=I32)*([1]combat_sim_results!A31:'[1]combat_sim_results'!A10029=P31)*([1]combat_sim_results!B31:'[1]combat_sim_results'!B10029=O31), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K32" s="26">
         <v>1</v>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="J33" s="26" t="e">
         <f t="array" ref="J33">INDEX([1]combat_sim_results!A32:'[1]combat_sim_results'!E10030, MATCH(1, ([1]combat_sim_results!C32:'[1]combat_sim_results'!C10030=H33)*([1]combat_sim_results!D32:'[1]combat_sim_results'!D10030=I33)*([1]combat_sim_results!A32:'[1]combat_sim_results'!A10030=P32)*([1]combat_sim_results!B32:'[1]combat_sim_results'!B10030=O32), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K33" s="26">
         <v>1</v>
@@ -4815,7 +4815,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F34" s="26" t="s">
         <v>17</v>
@@ -4830,9 +4830,9 @@
       <c r="I34" s="26">
         <v>2</v>
       </c>
-      <c r="J34" s="26">
+      <c r="J34" s="26" t="e">
         <f t="array" ref="J34">INDEX([1]combat_sim_results!A33:'[1]combat_sim_results'!E10031, MATCH(1, ([1]combat_sim_results!C33:'[1]combat_sim_results'!C10031=H34)*([1]combat_sim_results!D33:'[1]combat_sim_results'!D10031=I34)*([1]combat_sim_results!A33:'[1]combat_sim_results'!A10031=P33)*([1]combat_sim_results!B33:'[1]combat_sim_results'!B10031=O33), 0),5)</f>
-        <v>0.97299999999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="K34" s="26">
         <v>3</v>
@@ -4889,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F35" s="26" t="s">
         <v>5</v>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="J35" s="26" t="e">
         <f t="array" ref="J35">INDEX([1]combat_sim_results!A34:'[1]combat_sim_results'!E10032, MATCH(1, ([1]combat_sim_results!C34:'[1]combat_sim_results'!C10032=H35)*([1]combat_sim_results!D34:'[1]combat_sim_results'!D10032=I35)*([1]combat_sim_results!A34:'[1]combat_sim_results'!A10032=P34)*([1]combat_sim_results!B34:'[1]combat_sim_results'!B10032=O34), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K35" s="26">
         <v>1</v>
@@ -4957,14 +4957,14 @@
         <v>2</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.59099999999999997</v>
+        <v>#REF!</v>
       </c>
       <c r="H36" s="26">
         <v>10</v>
@@ -4972,9 +4972,9 @@
       <c r="I36" s="26">
         <v>3</v>
       </c>
-      <c r="J36" s="26">
+      <c r="J36" s="26" t="e">
         <f t="array" ref="J36">INDEX([1]combat_sim_results!A35:'[1]combat_sim_results'!E10033, MATCH(1, ([1]combat_sim_results!C35:'[1]combat_sim_results'!C10033=H36)*([1]combat_sim_results!D35:'[1]combat_sim_results'!D10033=I36)*([1]combat_sim_results!A35:'[1]combat_sim_results'!A10033=P35)*([1]combat_sim_results!B35:'[1]combat_sim_results'!B10033=O35), 0),5)</f>
-        <v>0.59099999999999997</v>
+        <v>#REF!</v>
       </c>
       <c r="K36" s="26">
         <v>5</v>
@@ -5023,7 +5023,7 @@
         <v>5.75</v>
       </c>
       <c r="Z36" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="3:26" x14ac:dyDescent="0.25">
@@ -5045,7 +5045,7 @@
       </c>
       <c r="J37" s="26" t="e">
         <f t="array" ref="J37">INDEX([1]combat_sim_results!A36:'[1]combat_sim_results'!E10034, MATCH(1, ([1]combat_sim_results!C36:'[1]combat_sim_results'!C10034=H37)*([1]combat_sim_results!D36:'[1]combat_sim_results'!D10034=I37)*([1]combat_sim_results!A36:'[1]combat_sim_results'!A10034=P36)*([1]combat_sim_results!B36:'[1]combat_sim_results'!B10034=O36), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K37" s="26">
         <v>3</v>
@@ -5113,7 +5113,7 @@
       </c>
       <c r="J38" s="26" t="e">
         <f t="array" ref="J38">INDEX([1]combat_sim_results!A37:'[1]combat_sim_results'!E10035, MATCH(1, ([1]combat_sim_results!C37:'[1]combat_sim_results'!C10035=H38)*([1]combat_sim_results!D37:'[1]combat_sim_results'!D10035=I38)*([1]combat_sim_results!A37:'[1]combat_sim_results'!A10035=P37)*([1]combat_sim_results!B37:'[1]combat_sim_results'!B10035=O37), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K38" s="26">
         <v>5</v>
@@ -5170,7 +5170,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F39" s="26" t="s">
         <v>17</v>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="J39" s="26" t="e">
         <f t="array" ref="J39">INDEX([1]combat_sim_results!A38:'[1]combat_sim_results'!E10036, MATCH(1, ([1]combat_sim_results!C38:'[1]combat_sim_results'!C10036=H39)*([1]combat_sim_results!D38:'[1]combat_sim_results'!D10036=I39)*([1]combat_sim_results!A38:'[1]combat_sim_results'!A10036=P38)*([1]combat_sim_results!B38:'[1]combat_sim_results'!B10036=O38), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K39" s="26">
         <v>5</v>
@@ -5249,7 +5249,7 @@
       </c>
       <c r="J40" s="26" t="e">
         <f t="array" ref="J40">INDEX([1]combat_sim_results!A39:'[1]combat_sim_results'!E10037, MATCH(1, ([1]combat_sim_results!C39:'[1]combat_sim_results'!C10037=H40)*([1]combat_sim_results!D39:'[1]combat_sim_results'!D10037=I40)*([1]combat_sim_results!A39:'[1]combat_sim_results'!A10037=P39)*([1]combat_sim_results!B39:'[1]combat_sim_results'!B10037=O39), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K40" s="26">
         <v>1</v>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="J41" s="26" t="e">
         <f t="array" ref="J41">INDEX([1]combat_sim_results!A40:'[1]combat_sim_results'!E10038, MATCH(1, ([1]combat_sim_results!C40:'[1]combat_sim_results'!C10038=H41)*([1]combat_sim_results!D40:'[1]combat_sim_results'!D10038=I41)*([1]combat_sim_results!A40:'[1]combat_sim_results'!A10038=P40)*([1]combat_sim_results!B40:'[1]combat_sim_results'!B10038=O40), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K41" s="26">
         <v>1</v>
@@ -5379,9 +5379,9 @@
       <c r="F42" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.89100000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="H42" s="26">
         <v>8</v>
@@ -5389,9 +5389,9 @@
       <c r="I42" s="26">
         <v>4</v>
       </c>
-      <c r="J42" s="26">
+      <c r="J42" s="26" t="e">
         <f t="array" ref="J42">INDEX([1]combat_sim_results!A41:'[1]combat_sim_results'!E10039, MATCH(1, ([1]combat_sim_results!C41:'[1]combat_sim_results'!C10039=H42)*([1]combat_sim_results!D41:'[1]combat_sim_results'!D10039=I42)*([1]combat_sim_results!A41:'[1]combat_sim_results'!A10039=P41)*([1]combat_sim_results!B41:'[1]combat_sim_results'!B10039=O41), 0),5)</f>
-        <v>0.89100000000000001</v>
+        <v>#REF!</v>
       </c>
       <c r="K42" s="26">
         <v>6</v>
@@ -5440,7 +5440,7 @@
         <v>4.6666666666666661</v>
       </c>
       <c r="Z42" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
@@ -5459,7 +5459,7 @@
       </c>
       <c r="J43" s="26" t="e">
         <f t="array" ref="J43">INDEX([1]combat_sim_results!A42:'[1]combat_sim_results'!E10040, MATCH(1, ([1]combat_sim_results!C42:'[1]combat_sim_results'!C10040=H43)*([1]combat_sim_results!D42:'[1]combat_sim_results'!D10040=I43)*([1]combat_sim_results!A42:'[1]combat_sim_results'!A10040=P42)*([1]combat_sim_results!B42:'[1]combat_sim_results'!B10040=O42), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K43" s="26">
         <v>6</v>
@@ -5516,7 +5516,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F44" s="26" t="s">
         <v>5</v>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="J44" s="26" t="e">
         <f t="array" ref="J44">INDEX([1]combat_sim_results!A43:'[1]combat_sim_results'!E10041, MATCH(1, ([1]combat_sim_results!C43:'[1]combat_sim_results'!C10041=H44)*([1]combat_sim_results!D43:'[1]combat_sim_results'!D10041=I44)*([1]combat_sim_results!A43:'[1]combat_sim_results'!A10041=P43)*([1]combat_sim_results!B43:'[1]combat_sim_results'!B10041=O43), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K44" s="26">
         <v>6</v>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="J45" s="26" t="e">
         <f t="array" ref="J45">INDEX([1]combat_sim_results!A44:'[1]combat_sim_results'!E10042, MATCH(1, ([1]combat_sim_results!C44:'[1]combat_sim_results'!C10042=H45)*([1]combat_sim_results!D44:'[1]combat_sim_results'!D10042=I45)*([1]combat_sim_results!A44:'[1]combat_sim_results'!A10042=P44)*([1]combat_sim_results!B44:'[1]combat_sim_results'!B10042=O44), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K45" s="26">
         <v>6</v>
@@ -5644,7 +5644,7 @@
         <v>7.666666666666667</v>
       </c>
       <c r="Z45" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.25">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="J46" s="26" t="e">
         <f t="array" ref="J46">INDEX([1]combat_sim_results!A45:'[1]combat_sim_results'!E10043, MATCH(1, ([1]combat_sim_results!C45:'[1]combat_sim_results'!C10043=H46)*([1]combat_sim_results!D45:'[1]combat_sim_results'!D10043=I46)*([1]combat_sim_results!A45:'[1]combat_sim_results'!A10043=P45)*([1]combat_sim_results!B45:'[1]combat_sim_results'!B10043=O45), 0),5)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="K46" s="26">
         <v>6</v>
@@ -5728,9 +5728,9 @@
       <c r="F47" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.80300000000000005</v>
+        <v>#REF!</v>
       </c>
       <c r="H47" s="26">
         <v>11</v>
@@ -5738,9 +5738,9 @@
       <c r="I47" s="26">
         <v>4</v>
       </c>
-      <c r="J47" s="26">
+      <c r="J47" s="26" t="e">
         <f t="array" ref="J47">INDEX([1]combat_sim_results!A46:'[1]combat_sim_results'!E10044, MATCH(1, ([1]combat_sim_results!C46:'[1]combat_sim_results'!C10044=H47)*([1]combat_sim_results!D46:'[1]combat_sim_results'!D10044=I47)*([1]combat_sim_results!A46:'[1]combat_sim_results'!A10044=P46)*([1]combat_sim_results!B46:'[1]combat_sim_results'!B10044=O46), 0),5)</f>
-        <v>0.80300000000000005</v>
+        <v>#REF!</v>
       </c>
       <c r="K47" s="26">
         <v>7</v>
@@ -5789,7 +5789,7 @@
         <v>8.9166666666666661</v>
       </c>
       <c r="Z47" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="3:26" x14ac:dyDescent="0.25">
@@ -5805,9 +5805,9 @@
       <c r="F48" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G48" s="29" t="e">
         <f t="shared" si="2"/>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="H48" s="26">
         <v>15</v>
@@ -5815,16 +5815,16 @@
       <c r="I48" s="26">
         <v>4</v>
       </c>
-      <c r="J48" s="26">
+      <c r="J48" s="26" t="e">
         <f t="array" ref="J48">INDEX([1]combat_sim_results!A47:'[1]combat_sim_results'!E10045, MATCH(1, ([1]combat_sim_results!C47:'[1]combat_sim_results'!C10045=H48)*([1]combat_sim_results!D47:'[1]combat_sim_results'!D10045=I48)*([1]combat_sim_results!A47:'[1]combat_sim_results'!A10045=P47)*([1]combat_sim_results!B47:'[1]combat_sim_results'!B10045=O47), 0),5)</f>
-        <v>0.89700000000000002</v>
+        <v>#REF!</v>
       </c>
       <c r="Y48" s="26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z48" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="3:25" x14ac:dyDescent="0.25">
@@ -5838,9 +5838,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J49" s="26">
+      <c r="J49" s="26" t="e">
         <f t="array" ref="J49">INDEX([1]combat_sim_results!A48:'[1]combat_sim_results'!E10046, MATCH(1, ([1]combat_sim_results!C48:'[1]combat_sim_results'!C10046=H49)*([1]combat_sim_results!D48:'[1]combat_sim_results'!D10046=I49)*([1]combat_sim_results!A48:'[1]combat_sim_results'!A10046=P48)*([1]combat_sim_results!B48:'[1]combat_sim_results'!B10046=O48), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y49" s="26">
         <f t="shared" si="3"/>
@@ -5858,9 +5858,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J50" s="26">
+      <c r="J50" s="26" t="e">
         <f t="array" ref="J50">INDEX([1]combat_sim_results!A49:'[1]combat_sim_results'!E10047, MATCH(1, ([1]combat_sim_results!C49:'[1]combat_sim_results'!C10047=H50)*([1]combat_sim_results!D49:'[1]combat_sim_results'!D10047=I50)*([1]combat_sim_results!A49:'[1]combat_sim_results'!A10047=P49)*([1]combat_sim_results!B49:'[1]combat_sim_results'!B10047=O49), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y50" s="26">
         <f t="shared" si="3"/>
@@ -5878,9 +5878,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J51" s="26">
+      <c r="J51" s="26" t="e">
         <f t="array" ref="J51">INDEX([1]combat_sim_results!A50:'[1]combat_sim_results'!E10048, MATCH(1, ([1]combat_sim_results!C50:'[1]combat_sim_results'!C10048=H51)*([1]combat_sim_results!D50:'[1]combat_sim_results'!D10048=I51)*([1]combat_sim_results!A50:'[1]combat_sim_results'!A10048=P50)*([1]combat_sim_results!B50:'[1]combat_sim_results'!B10048=O50), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y51" s="26">
         <f t="shared" si="3"/>
@@ -5898,9 +5898,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J52" s="26">
+      <c r="J52" s="26" t="e">
         <f t="array" ref="J52">INDEX([1]combat_sim_results!A51:'[1]combat_sim_results'!E10049, MATCH(1, ([1]combat_sim_results!C51:'[1]combat_sim_results'!C10049=H52)*([1]combat_sim_results!D51:'[1]combat_sim_results'!D10049=I52)*([1]combat_sim_results!A51:'[1]combat_sim_results'!A10049=P51)*([1]combat_sim_results!B51:'[1]combat_sim_results'!B10049=O51), 0),5)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="Y52" s="26">
         <f t="shared" si="3"/>
@@ -5946,7 +5946,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>